<commit_message>
got rid of the ugly images
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -34,6 +34,9 @@
     <t>imgUrl</t>
   </si>
   <si>
+    <t>imgOK</t>
+  </si>
+  <si>
     <t>"You know how long that takes in Texas at 75 miles an hour? That's a particularly flat highway."</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2013/07/22/Protesters-Split_jpg_312x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>“MARRIAGE = ONE MAN &amp; ONE MAN. Enough of these activist judges. FAVORITE if you agree. I know the silent majority out there is with us!”</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/03/04/Patrick3-web_jpg_312x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>"Apparently I’ve outfoxed the campaign deal, so maybe I need to be a consultant. I’m not going to run all over the state. I work."</t>
   </si>
   <si>
@@ -88,6 +97,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/03/26/JimHogan_jpg_75x75_crop_q100.jpg</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>"Out there on Twitter, in front of the Alamo in your campaign, you know, you’ve been huffing and puffing like the big bad wolf and now you’re dancing around, tiptoeing like Little Red Riding Hood on this issue."</t>
   </si>
   <si>
@@ -106,6 +118,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/04/15/CastroPatrick309_jpg_75x75_crop_q100.jpg</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>"Dewhurst has asked me to cease distribution of this information. He also asked me not to run against him for Lt. Gov. I didn't really give a damn what David wanted then, and I don't give a damn now. The voters of Texas need to know."</t>
   </si>
   <si>
@@ -124,6 +139,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/videos/pattersonspot_png_260x1000_q100.png</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>"Some Democrats have said they wanted me to be the nominee. Well, they’ve got me and I’m coming."</t>
   </si>
   <si>
@@ -142,6 +160,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/05/27/DAN_PATRICK_RUNOFF9501_jpg_800x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>"The uninformed opinions of a Washington, D.C., desk jockey who's never stepped foot in Texas couldn't be less relevant to what's actually happening on the ground."</t>
   </si>
   <si>
@@ -160,6 +181,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/09/19/ttf-davisabbott-3_JPG_312x1000_q100.JPG</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>“We need to look at the states, which are lavatories of innovation and democracy.”</t>
   </si>
   <si>
@@ -178,6 +202,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/09/21/xxTribFest_Perry392_jpg_260x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>"We don't settle political differences with indictments in this country. It is outrageous that some would use partisan political theatrics to rip away at the very fabric of our state's constitution."</t>
   </si>
   <si>
@@ -196,6 +223,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/videos/Perry_in_court_Nov_2014_jpg_260x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>“And all I can do is deal with the issues that are before me. … The job of attorney general is to represent and defend in court the laws of their client, which is the state Legislature, unless and until a court strikes it down.”</t>
   </si>
   <si>
@@ -214,6 +244,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/11/11/UP9A9907_jpg_312x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>"If that dog has to be The Boy in the Plastic Bubble, we're going to take good care of that dog."</t>
   </si>
   <si>
@@ -232,6 +265,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/10/09/ClayJenkinsTribLiveTTCrop_jpg_312x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>"The only way we will have lost tonight is if we stop fighting. I am so proud of all that we have accomplished."</t>
   </si>
   <si>
@@ -250,6 +286,9 @@
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/2014/07/12/TXTDavisCanvas-CCR001_jpg_800x1000_q100.jpg</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>“We were elected to govern. If we blow it by not governing, then shame on us.”</t>
   </si>
   <si>
@@ -266,6 +305,9 @@
   </si>
   <si>
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/MichaelMcCaul_1_jpg_75x75_crop_q100.jpg</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -281,10 +323,10 @@
       <b/>
       <sz val="10.0"/>
     </font>
+    <font/>
     <font>
       <sz val="10.0"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -320,14 +362,17 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="1" borderId="1" applyFont="1" fontId="2" applyNumberFormat="1">
-      <alignment/>
-    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="1" borderId="1" applyFont="1" fontId="3" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+      <alignment/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3"/>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -374,3263 +419,3305 @@
       <c t="s" s="2" r="G1">
         <v>6</v>
       </c>
+      <c t="s" s="3" r="H1">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
-      <c s="3" r="A2">
+      <c s="4" r="A2">
         <v>0.0</v>
       </c>
-      <c t="s" s="4" r="B2">
-        <v>7</v>
-      </c>
-      <c t="s" s="4" r="C2">
+      <c t="s" s="5" r="B2">
         <v>8</v>
       </c>
-      <c t="s" s="4" r="D2">
+      <c t="s" s="5" r="C2">
         <v>9</v>
       </c>
-      <c t="s" s="4" r="E2">
+      <c t="s" s="5" r="D2">
         <v>10</v>
       </c>
-      <c t="s" s="5" r="F2">
+      <c t="s" s="5" r="E2">
         <v>11</v>
       </c>
-      <c t="s" s="5" r="G2">
+      <c t="s" s="6" r="F2">
         <v>12</v>
       </c>
+      <c t="s" s="6" r="G2">
+        <v>13</v>
+      </c>
+      <c t="s" s="3" r="H2">
+        <v>14</v>
+      </c>
     </row>
     <row r="3">
-      <c s="3" r="A3">
+      <c s="4" r="A3">
         <v>1.0</v>
       </c>
-      <c t="s" s="4" r="B3">
-        <v>13</v>
-      </c>
-      <c t="s" s="4" r="C3">
-        <v>14</v>
-      </c>
-      <c t="s" s="4" r="D3">
+      <c t="s" s="5" r="B3">
         <v>15</v>
       </c>
-      <c t="s" s="4" r="E3">
+      <c t="s" s="5" r="C3">
         <v>16</v>
       </c>
-      <c t="s" s="5" r="F3">
+      <c t="s" s="5" r="D3">
         <v>17</v>
       </c>
-      <c t="s" s="4" r="G3">
+      <c t="s" s="5" r="E3">
         <v>18</v>
       </c>
+      <c t="s" s="6" r="F3">
+        <v>19</v>
+      </c>
+      <c t="s" s="5" r="G3">
+        <v>20</v>
+      </c>
+      <c t="s" s="3" r="H3">
+        <v>21</v>
+      </c>
     </row>
     <row r="4">
-      <c s="3" r="A4">
+      <c s="4" r="A4">
         <v>2.0</v>
       </c>
-      <c t="s" s="4" r="B4">
-        <v>19</v>
-      </c>
-      <c t="s" s="4" r="C4">
-        <v>20</v>
-      </c>
-      <c t="s" s="4" r="D4">
-        <v>21</v>
-      </c>
-      <c t="s" s="4" r="E4">
+      <c t="s" s="5" r="B4">
         <v>22</v>
       </c>
-      <c t="s" s="5" r="F4">
+      <c t="s" s="5" r="C4">
         <v>23</v>
       </c>
-      <c t="s" s="5" r="G4">
+      <c t="s" s="5" r="D4">
         <v>24</v>
       </c>
+      <c t="s" s="5" r="E4">
+        <v>25</v>
+      </c>
+      <c t="s" s="6" r="F4">
+        <v>26</v>
+      </c>
+      <c t="s" s="6" r="G4">
+        <v>27</v>
+      </c>
+      <c t="s" s="3" r="H4">
+        <v>28</v>
+      </c>
     </row>
     <row r="5">
-      <c s="3" r="A5">
+      <c s="4" r="A5">
         <v>3.0</v>
       </c>
-      <c t="s" s="4" r="B5">
-        <v>25</v>
-      </c>
-      <c t="s" s="4" r="C5">
-        <v>26</v>
-      </c>
-      <c t="s" s="4" r="D5">
-        <v>27</v>
-      </c>
-      <c t="s" s="4" r="E5">
-        <v>28</v>
-      </c>
-      <c t="s" s="5" r="F5">
+      <c t="s" s="5" r="B5">
         <v>29</v>
       </c>
-      <c t="s" s="5" r="G5">
+      <c t="s" s="5" r="C5">
         <v>30</v>
       </c>
+      <c t="s" s="5" r="D5">
+        <v>31</v>
+      </c>
+      <c t="s" s="5" r="E5">
+        <v>32</v>
+      </c>
+      <c t="s" s="6" r="F5">
+        <v>33</v>
+      </c>
+      <c t="s" s="6" r="G5">
+        <v>34</v>
+      </c>
+      <c t="s" s="3" r="H5">
+        <v>35</v>
+      </c>
     </row>
     <row r="6">
-      <c s="3" r="A6">
+      <c s="4" r="A6">
         <v>4.0</v>
       </c>
-      <c t="s" s="4" r="B6">
-        <v>31</v>
-      </c>
-      <c t="s" s="4" r="C6">
-        <v>32</v>
-      </c>
-      <c t="s" s="4" r="D6">
-        <v>33</v>
-      </c>
-      <c t="s" s="4" r="E6">
-        <v>34</v>
-      </c>
-      <c t="s" s="5" r="F6">
-        <v>35</v>
-      </c>
-      <c t="s" s="5" r="G6">
+      <c t="s" s="5" r="B6">
         <v>36</v>
       </c>
+      <c t="s" s="5" r="C6">
+        <v>37</v>
+      </c>
+      <c t="s" s="5" r="D6">
+        <v>38</v>
+      </c>
+      <c t="s" s="5" r="E6">
+        <v>39</v>
+      </c>
+      <c t="s" s="6" r="F6">
+        <v>40</v>
+      </c>
+      <c t="s" s="6" r="G6">
+        <v>41</v>
+      </c>
+      <c t="s" s="3" r="H6">
+        <v>42</v>
+      </c>
     </row>
     <row r="7">
-      <c s="3" r="A7">
+      <c s="4" r="A7">
         <v>5.0</v>
       </c>
-      <c t="s" s="4" r="B7">
-        <v>37</v>
-      </c>
-      <c t="s" s="4" r="C7">
-        <v>38</v>
-      </c>
-      <c t="s" s="4" r="D7">
-        <v>39</v>
-      </c>
-      <c t="s" s="4" r="E7">
-        <v>40</v>
-      </c>
-      <c t="s" s="5" r="F7">
-        <v>41</v>
-      </c>
-      <c t="s" s="5" r="G7">
-        <v>42</v>
+      <c t="s" s="5" r="B7">
+        <v>43</v>
+      </c>
+      <c t="s" s="5" r="C7">
+        <v>44</v>
+      </c>
+      <c t="s" s="5" r="D7">
+        <v>45</v>
+      </c>
+      <c t="s" s="5" r="E7">
+        <v>46</v>
+      </c>
+      <c t="s" s="6" r="F7">
+        <v>47</v>
+      </c>
+      <c t="s" s="6" r="G7">
+        <v>48</v>
+      </c>
+      <c t="s" s="3" r="H7">
+        <v>49</v>
       </c>
     </row>
     <row r="8">
-      <c s="3" r="A8">
+      <c s="4" r="A8">
         <v>6.0</v>
       </c>
-      <c t="s" s="4" r="B8">
-        <v>43</v>
-      </c>
-      <c t="s" s="4" r="C8">
-        <v>44</v>
-      </c>
-      <c t="s" s="4" r="D8">
-        <v>45</v>
-      </c>
-      <c t="s" s="4" r="E8">
-        <v>46</v>
-      </c>
-      <c t="s" s="5" r="F8">
-        <v>47</v>
-      </c>
-      <c t="s" s="5" r="G8">
-        <v>48</v>
+      <c t="s" s="5" r="B8">
+        <v>50</v>
+      </c>
+      <c t="s" s="5" r="C8">
+        <v>51</v>
+      </c>
+      <c t="s" s="5" r="D8">
+        <v>52</v>
+      </c>
+      <c t="s" s="5" r="E8">
+        <v>53</v>
+      </c>
+      <c t="s" s="6" r="F8">
+        <v>54</v>
+      </c>
+      <c t="s" s="6" r="G8">
+        <v>55</v>
+      </c>
+      <c t="s" s="3" r="H8">
+        <v>56</v>
       </c>
     </row>
     <row r="9">
-      <c s="3" r="A9">
+      <c s="4" r="A9">
         <v>7.0</v>
       </c>
-      <c t="s" s="4" r="B9">
-        <v>49</v>
-      </c>
-      <c t="s" s="4" r="C9">
-        <v>50</v>
-      </c>
-      <c t="s" s="4" r="D9">
-        <v>51</v>
-      </c>
-      <c t="s" s="4" r="E9">
-        <v>52</v>
-      </c>
-      <c t="s" s="5" r="F9">
-        <v>53</v>
-      </c>
-      <c t="s" s="5" r="G9">
-        <v>54</v>
+      <c t="s" s="5" r="B9">
+        <v>57</v>
+      </c>
+      <c t="s" s="5" r="C9">
+        <v>58</v>
+      </c>
+      <c t="s" s="5" r="D9">
+        <v>59</v>
+      </c>
+      <c t="s" s="5" r="E9">
+        <v>60</v>
+      </c>
+      <c t="s" s="6" r="F9">
+        <v>61</v>
+      </c>
+      <c t="s" s="6" r="G9">
+        <v>62</v>
+      </c>
+      <c t="s" s="3" r="H9">
+        <v>63</v>
       </c>
     </row>
     <row r="10">
-      <c s="3" r="A10">
+      <c s="4" r="A10">
         <v>8.0</v>
       </c>
-      <c t="s" s="4" r="B10">
-        <v>55</v>
-      </c>
-      <c t="s" s="4" r="C10">
-        <v>56</v>
-      </c>
-      <c t="s" s="4" r="D10">
-        <v>57</v>
-      </c>
-      <c t="s" s="4" r="E10">
-        <v>58</v>
-      </c>
-      <c t="s" s="5" r="F10">
-        <v>59</v>
-      </c>
-      <c t="s" s="5" r="G10">
-        <v>60</v>
+      <c t="s" s="5" r="B10">
+        <v>64</v>
+      </c>
+      <c t="s" s="5" r="C10">
+        <v>65</v>
+      </c>
+      <c t="s" s="5" r="D10">
+        <v>66</v>
+      </c>
+      <c t="s" s="5" r="E10">
+        <v>67</v>
+      </c>
+      <c t="s" s="6" r="F10">
+        <v>68</v>
+      </c>
+      <c t="s" s="6" r="G10">
+        <v>69</v>
+      </c>
+      <c t="s" s="3" r="H10">
+        <v>70</v>
       </c>
     </row>
     <row r="11">
-      <c s="3" r="A11">
+      <c s="4" r="A11">
         <v>9.0</v>
       </c>
-      <c t="s" s="4" r="B11">
-        <v>61</v>
-      </c>
-      <c t="s" s="4" r="C11">
-        <v>62</v>
-      </c>
-      <c t="s" s="4" r="D11">
-        <v>63</v>
-      </c>
-      <c t="s" s="4" r="E11">
-        <v>64</v>
-      </c>
-      <c t="s" s="5" r="F11">
-        <v>65</v>
-      </c>
-      <c t="s" s="5" r="G11">
-        <v>66</v>
+      <c t="s" s="5" r="B11">
+        <v>71</v>
+      </c>
+      <c t="s" s="5" r="C11">
+        <v>72</v>
+      </c>
+      <c t="s" s="5" r="D11">
+        <v>73</v>
+      </c>
+      <c t="s" s="5" r="E11">
+        <v>74</v>
+      </c>
+      <c t="s" s="6" r="F11">
+        <v>75</v>
+      </c>
+      <c t="s" s="6" r="G11">
+        <v>76</v>
+      </c>
+      <c t="s" s="3" r="H11">
+        <v>77</v>
       </c>
     </row>
     <row r="12">
-      <c s="3" r="A12">
+      <c s="4" r="A12">
         <v>10.0</v>
       </c>
-      <c t="s" s="4" r="B12">
-        <v>67</v>
-      </c>
-      <c t="s" s="4" r="C12">
-        <v>68</v>
-      </c>
-      <c t="s" s="4" r="D12">
-        <v>69</v>
-      </c>
-      <c t="s" s="4" r="E12">
-        <v>70</v>
-      </c>
-      <c t="s" s="5" r="F12">
-        <v>71</v>
-      </c>
-      <c t="s" s="5" r="G12">
-        <v>72</v>
+      <c t="s" s="5" r="B12">
+        <v>78</v>
+      </c>
+      <c t="s" s="5" r="C12">
+        <v>79</v>
+      </c>
+      <c t="s" s="5" r="D12">
+        <v>80</v>
+      </c>
+      <c t="s" s="5" r="E12">
+        <v>81</v>
+      </c>
+      <c t="s" s="6" r="F12">
+        <v>82</v>
+      </c>
+      <c t="s" s="6" r="G12">
+        <v>83</v>
+      </c>
+      <c t="s" s="3" r="H12">
+        <v>84</v>
       </c>
     </row>
     <row r="13">
-      <c s="3" r="A13">
+      <c s="4" r="A13">
         <v>11.0</v>
       </c>
-      <c t="s" s="4" r="B13">
-        <v>73</v>
-      </c>
-      <c t="s" s="4" r="C13">
-        <v>74</v>
-      </c>
-      <c t="s" s="4" r="D13">
-        <v>75</v>
-      </c>
-      <c t="s" s="4" r="E13">
-        <v>76</v>
-      </c>
-      <c t="s" s="5" r="F13">
-        <v>77</v>
-      </c>
-      <c t="s" s="5" r="G13">
-        <v>78</v>
+      <c t="s" s="5" r="B13">
+        <v>85</v>
+      </c>
+      <c t="s" s="5" r="C13">
+        <v>86</v>
+      </c>
+      <c t="s" s="5" r="D13">
+        <v>87</v>
+      </c>
+      <c t="s" s="5" r="E13">
+        <v>88</v>
+      </c>
+      <c t="s" s="6" r="F13">
+        <v>89</v>
+      </c>
+      <c t="s" s="6" r="G13">
+        <v>90</v>
+      </c>
+      <c t="s" s="3" r="H13">
+        <v>91</v>
       </c>
     </row>
     <row r="14">
-      <c s="3" r="A14">
+      <c s="4" r="A14">
         <v>12.0</v>
       </c>
-      <c t="s" s="4" r="B14">
-        <v>79</v>
-      </c>
-      <c t="s" s="4" r="C14">
-        <v>80</v>
-      </c>
-      <c t="s" s="4" r="D14">
-        <v>81</v>
-      </c>
-      <c t="s" s="4" r="E14">
-        <v>82</v>
-      </c>
-      <c t="s" s="5" r="F14">
-        <v>83</v>
-      </c>
-      <c t="s" s="5" r="G14">
-        <v>84</v>
+      <c t="s" s="5" r="B14">
+        <v>92</v>
+      </c>
+      <c t="s" s="5" r="C14">
+        <v>93</v>
+      </c>
+      <c t="s" s="5" r="D14">
+        <v>94</v>
+      </c>
+      <c t="s" s="5" r="E14">
+        <v>95</v>
+      </c>
+      <c t="s" s="6" r="F14">
+        <v>96</v>
+      </c>
+      <c t="s" s="6" r="G14">
+        <v>97</v>
+      </c>
+      <c t="s" s="3" r="H14">
+        <v>98</v>
       </c>
     </row>
     <row r="15">
-      <c s="6" r="A15"/>
+      <c s="7" r="A15"/>
     </row>
     <row r="16">
-      <c s="6" r="A16"/>
+      <c s="7" r="A16"/>
     </row>
     <row r="17">
-      <c s="6" r="A17"/>
+      <c s="7" r="A17"/>
     </row>
     <row r="18">
-      <c s="6" r="A18"/>
+      <c s="7" r="A18"/>
     </row>
     <row r="19">
-      <c s="6" r="A19"/>
+      <c s="7" r="A19"/>
     </row>
     <row r="20">
-      <c s="6" r="A20"/>
+      <c s="7" r="A20"/>
     </row>
     <row r="21">
-      <c s="6" r="A21"/>
+      <c s="7" r="A21"/>
     </row>
     <row r="22">
-      <c s="6" r="A22"/>
+      <c s="7" r="A22"/>
     </row>
     <row r="23">
-      <c s="6" r="A23"/>
+      <c s="7" r="A23"/>
     </row>
     <row r="24">
-      <c s="6" r="A24"/>
+      <c s="7" r="A24"/>
     </row>
     <row r="25">
-      <c s="6" r="A25"/>
+      <c s="7" r="A25"/>
     </row>
     <row r="26">
-      <c s="6" r="A26"/>
+      <c s="7" r="A26"/>
     </row>
     <row r="27">
-      <c s="6" r="A27"/>
+      <c s="7" r="A27"/>
     </row>
     <row r="28">
-      <c s="6" r="A28"/>
+      <c s="7" r="A28"/>
     </row>
     <row r="29">
-      <c s="6" r="A29"/>
+      <c s="7" r="A29"/>
     </row>
     <row r="30">
-      <c s="6" r="A30"/>
+      <c s="7" r="A30"/>
     </row>
     <row r="31">
-      <c s="6" r="A31"/>
+      <c s="7" r="A31"/>
     </row>
     <row r="32">
-      <c s="6" r="A32"/>
+      <c s="7" r="A32"/>
     </row>
     <row r="33">
-      <c s="6" r="A33"/>
+      <c s="7" r="A33"/>
     </row>
     <row r="34">
-      <c s="6" r="A34"/>
+      <c s="7" r="A34"/>
     </row>
     <row r="35">
-      <c s="6" r="A35"/>
+      <c s="7" r="A35"/>
     </row>
     <row r="36">
-      <c s="6" r="A36"/>
+      <c s="7" r="A36"/>
     </row>
     <row r="37">
-      <c s="6" r="A37"/>
+      <c s="7" r="A37"/>
     </row>
     <row r="38">
-      <c s="6" r="A38"/>
+      <c s="7" r="A38"/>
     </row>
     <row r="39">
-      <c s="6" r="A39"/>
+      <c s="7" r="A39"/>
     </row>
     <row r="40">
-      <c s="6" r="A40"/>
+      <c s="7" r="A40"/>
     </row>
     <row r="41">
-      <c s="6" r="A41"/>
+      <c s="7" r="A41"/>
     </row>
     <row r="42">
-      <c s="6" r="A42"/>
+      <c s="7" r="A42"/>
     </row>
     <row r="43">
-      <c s="6" r="A43"/>
+      <c s="7" r="A43"/>
     </row>
     <row r="44">
-      <c s="6" r="A44"/>
+      <c s="7" r="A44"/>
     </row>
     <row r="45">
-      <c s="6" r="A45"/>
+      <c s="7" r="A45"/>
     </row>
     <row r="46">
-      <c s="6" r="A46"/>
+      <c s="7" r="A46"/>
     </row>
     <row r="47">
-      <c s="6" r="A47"/>
+      <c s="7" r="A47"/>
     </row>
     <row r="48">
-      <c s="6" r="A48"/>
+      <c s="7" r="A48"/>
     </row>
     <row r="49">
-      <c s="6" r="A49"/>
+      <c s="7" r="A49"/>
     </row>
     <row r="50">
-      <c s="6" r="A50"/>
+      <c s="7" r="A50"/>
     </row>
     <row r="51">
-      <c s="6" r="A51"/>
+      <c s="7" r="A51"/>
     </row>
     <row r="52">
-      <c s="6" r="A52"/>
+      <c s="7" r="A52"/>
     </row>
     <row r="53">
-      <c s="6" r="A53"/>
+      <c s="7" r="A53"/>
     </row>
     <row r="54">
-      <c s="6" r="A54"/>
+      <c s="7" r="A54"/>
     </row>
     <row r="55">
-      <c s="6" r="A55"/>
+      <c s="7" r="A55"/>
     </row>
     <row r="56">
-      <c s="6" r="A56"/>
+      <c s="7" r="A56"/>
     </row>
     <row r="57">
-      <c s="6" r="A57"/>
+      <c s="7" r="A57"/>
     </row>
     <row r="58">
-      <c s="6" r="A58"/>
+      <c s="7" r="A58"/>
     </row>
     <row r="59">
-      <c s="6" r="A59"/>
+      <c s="7" r="A59"/>
     </row>
     <row r="60">
-      <c s="6" r="A60"/>
+      <c s="7" r="A60"/>
     </row>
     <row r="61">
-      <c s="6" r="A61"/>
+      <c s="7" r="A61"/>
     </row>
     <row r="62">
-      <c s="6" r="A62"/>
+      <c s="7" r="A62"/>
     </row>
     <row r="63">
-      <c s="6" r="A63"/>
+      <c s="7" r="A63"/>
     </row>
     <row r="64">
-      <c s="6" r="A64"/>
+      <c s="7" r="A64"/>
     </row>
     <row r="65">
-      <c s="6" r="A65"/>
+      <c s="7" r="A65"/>
     </row>
     <row r="66">
-      <c s="6" r="A66"/>
+      <c s="7" r="A66"/>
     </row>
     <row r="67">
-      <c s="6" r="A67"/>
+      <c s="7" r="A67"/>
     </row>
     <row r="68">
-      <c s="6" r="A68"/>
+      <c s="7" r="A68"/>
     </row>
     <row r="69">
-      <c s="6" r="A69"/>
+      <c s="7" r="A69"/>
     </row>
     <row r="70">
-      <c s="6" r="A70"/>
+      <c s="7" r="A70"/>
     </row>
     <row r="71">
-      <c s="6" r="A71"/>
+      <c s="7" r="A71"/>
     </row>
     <row r="72">
-      <c s="6" r="A72"/>
+      <c s="7" r="A72"/>
     </row>
     <row r="73">
-      <c s="6" r="A73"/>
+      <c s="7" r="A73"/>
     </row>
     <row r="74">
-      <c s="6" r="A74"/>
+      <c s="7" r="A74"/>
     </row>
     <row r="75">
-      <c s="6" r="A75"/>
+      <c s="7" r="A75"/>
     </row>
     <row r="76">
-      <c s="6" r="A76"/>
+      <c s="7" r="A76"/>
     </row>
     <row r="77">
-      <c s="6" r="A77"/>
+      <c s="7" r="A77"/>
     </row>
     <row r="78">
-      <c s="6" r="A78"/>
+      <c s="7" r="A78"/>
     </row>
     <row r="79">
-      <c s="6" r="A79"/>
+      <c s="7" r="A79"/>
     </row>
     <row r="80">
-      <c s="6" r="A80"/>
+      <c s="7" r="A80"/>
     </row>
     <row r="81">
-      <c s="6" r="A81"/>
+      <c s="7" r="A81"/>
     </row>
     <row r="82">
-      <c s="6" r="A82"/>
+      <c s="7" r="A82"/>
     </row>
     <row r="83">
-      <c s="6" r="A83"/>
+      <c s="7" r="A83"/>
     </row>
     <row r="84">
-      <c s="6" r="A84"/>
+      <c s="7" r="A84"/>
     </row>
     <row r="85">
-      <c s="6" r="A85"/>
+      <c s="7" r="A85"/>
     </row>
     <row r="86">
-      <c s="6" r="A86"/>
+      <c s="7" r="A86"/>
     </row>
     <row r="87">
-      <c s="6" r="A87"/>
+      <c s="7" r="A87"/>
     </row>
     <row r="88">
-      <c s="6" r="A88"/>
+      <c s="7" r="A88"/>
     </row>
     <row r="89">
-      <c s="6" r="A89"/>
+      <c s="7" r="A89"/>
     </row>
     <row r="90">
-      <c s="6" r="A90"/>
+      <c s="7" r="A90"/>
     </row>
     <row r="91">
-      <c s="6" r="A91"/>
+      <c s="7" r="A91"/>
     </row>
     <row r="92">
-      <c s="6" r="A92"/>
+      <c s="7" r="A92"/>
     </row>
     <row r="93">
-      <c s="6" r="A93"/>
+      <c s="7" r="A93"/>
     </row>
     <row r="94">
-      <c s="6" r="A94"/>
+      <c s="7" r="A94"/>
     </row>
     <row r="95">
-      <c s="6" r="A95"/>
+      <c s="7" r="A95"/>
     </row>
     <row r="96">
-      <c s="6" r="A96"/>
+      <c s="7" r="A96"/>
     </row>
     <row r="97">
-      <c s="6" r="A97"/>
+      <c s="7" r="A97"/>
     </row>
     <row r="98">
-      <c s="6" r="A98"/>
+      <c s="7" r="A98"/>
     </row>
     <row r="99">
-      <c s="6" r="A99"/>
+      <c s="7" r="A99"/>
     </row>
     <row r="100">
-      <c s="6" r="A100"/>
+      <c s="7" r="A100"/>
     </row>
     <row r="101">
-      <c s="6" r="A101"/>
+      <c s="7" r="A101"/>
     </row>
     <row r="102">
-      <c s="6" r="A102"/>
+      <c s="7" r="A102"/>
     </row>
     <row r="103">
-      <c s="6" r="A103"/>
+      <c s="7" r="A103"/>
     </row>
     <row r="104">
-      <c s="6" r="A104"/>
+      <c s="7" r="A104"/>
     </row>
     <row r="105">
-      <c s="6" r="A105"/>
+      <c s="7" r="A105"/>
     </row>
     <row r="106">
-      <c s="6" r="A106"/>
+      <c s="7" r="A106"/>
     </row>
     <row r="107">
-      <c s="6" r="A107"/>
+      <c s="7" r="A107"/>
     </row>
     <row r="108">
-      <c s="6" r="A108"/>
+      <c s="7" r="A108"/>
     </row>
     <row r="109">
-      <c s="6" r="A109"/>
+      <c s="7" r="A109"/>
     </row>
     <row r="110">
-      <c s="6" r="A110"/>
+      <c s="7" r="A110"/>
     </row>
     <row r="111">
-      <c s="6" r="A111"/>
+      <c s="7" r="A111"/>
     </row>
     <row r="112">
-      <c s="6" r="A112"/>
+      <c s="7" r="A112"/>
     </row>
     <row r="113">
-      <c s="6" r="A113"/>
+      <c s="7" r="A113"/>
     </row>
     <row r="114">
-      <c s="6" r="A114"/>
+      <c s="7" r="A114"/>
     </row>
     <row r="115">
-      <c s="6" r="A115"/>
+      <c s="7" r="A115"/>
     </row>
     <row r="116">
-      <c s="6" r="A116"/>
+      <c s="7" r="A116"/>
     </row>
     <row r="117">
-      <c s="6" r="A117"/>
+      <c s="7" r="A117"/>
     </row>
     <row r="118">
-      <c s="6" r="A118"/>
+      <c s="7" r="A118"/>
     </row>
     <row r="119">
-      <c s="6" r="A119"/>
+      <c s="7" r="A119"/>
     </row>
     <row r="120">
-      <c s="6" r="A120"/>
+      <c s="7" r="A120"/>
     </row>
     <row r="121">
-      <c s="6" r="A121"/>
+      <c s="7" r="A121"/>
     </row>
     <row r="122">
-      <c s="6" r="A122"/>
+      <c s="7" r="A122"/>
     </row>
     <row r="123">
-      <c s="6" r="A123"/>
+      <c s="7" r="A123"/>
     </row>
     <row r="124">
-      <c s="6" r="A124"/>
+      <c s="7" r="A124"/>
     </row>
     <row r="125">
-      <c s="6" r="A125"/>
+      <c s="7" r="A125"/>
     </row>
     <row r="126">
-      <c s="6" r="A126"/>
+      <c s="7" r="A126"/>
     </row>
     <row r="127">
-      <c s="6" r="A127"/>
+      <c s="7" r="A127"/>
     </row>
     <row r="128">
-      <c s="6" r="A128"/>
+      <c s="7" r="A128"/>
     </row>
     <row r="129">
-      <c s="6" r="A129"/>
+      <c s="7" r="A129"/>
     </row>
     <row r="130">
-      <c s="6" r="A130"/>
+      <c s="7" r="A130"/>
     </row>
     <row r="131">
-      <c s="6" r="A131"/>
+      <c s="7" r="A131"/>
     </row>
     <row r="132">
-      <c s="6" r="A132"/>
+      <c s="7" r="A132"/>
     </row>
     <row r="133">
-      <c s="6" r="A133"/>
+      <c s="7" r="A133"/>
     </row>
     <row r="134">
-      <c s="6" r="A134"/>
+      <c s="7" r="A134"/>
     </row>
     <row r="135">
-      <c s="6" r="A135"/>
+      <c s="7" r="A135"/>
     </row>
     <row r="136">
-      <c s="6" r="A136"/>
+      <c s="7" r="A136"/>
     </row>
     <row r="137">
-      <c s="6" r="A137"/>
+      <c s="7" r="A137"/>
     </row>
     <row r="138">
-      <c s="6" r="A138"/>
+      <c s="7" r="A138"/>
     </row>
     <row r="139">
-      <c s="6" r="A139"/>
+      <c s="7" r="A139"/>
     </row>
     <row r="140">
-      <c s="6" r="A140"/>
+      <c s="7" r="A140"/>
     </row>
     <row r="141">
-      <c s="6" r="A141"/>
+      <c s="7" r="A141"/>
     </row>
     <row r="142">
-      <c s="6" r="A142"/>
+      <c s="7" r="A142"/>
     </row>
     <row r="143">
-      <c s="6" r="A143"/>
+      <c s="7" r="A143"/>
     </row>
     <row r="144">
-      <c s="6" r="A144"/>
+      <c s="7" r="A144"/>
     </row>
     <row r="145">
-      <c s="6" r="A145"/>
+      <c s="7" r="A145"/>
     </row>
     <row r="146">
-      <c s="6" r="A146"/>
+      <c s="7" r="A146"/>
     </row>
     <row r="147">
-      <c s="6" r="A147"/>
+      <c s="7" r="A147"/>
     </row>
     <row r="148">
-      <c s="6" r="A148"/>
+      <c s="7" r="A148"/>
     </row>
     <row r="149">
-      <c s="6" r="A149"/>
+      <c s="7" r="A149"/>
     </row>
     <row r="150">
-      <c s="6" r="A150"/>
+      <c s="7" r="A150"/>
     </row>
     <row r="151">
-      <c s="6" r="A151"/>
+      <c s="7" r="A151"/>
     </row>
     <row r="152">
-      <c s="6" r="A152"/>
+      <c s="7" r="A152"/>
     </row>
     <row r="153">
-      <c s="6" r="A153"/>
+      <c s="7" r="A153"/>
     </row>
     <row r="154">
-      <c s="6" r="A154"/>
+      <c s="7" r="A154"/>
     </row>
     <row r="155">
-      <c s="6" r="A155"/>
+      <c s="7" r="A155"/>
     </row>
     <row r="156">
-      <c s="6" r="A156"/>
+      <c s="7" r="A156"/>
     </row>
     <row r="157">
-      <c s="6" r="A157"/>
+      <c s="7" r="A157"/>
     </row>
     <row r="158">
-      <c s="6" r="A158"/>
+      <c s="7" r="A158"/>
     </row>
     <row r="159">
-      <c s="6" r="A159"/>
+      <c s="7" r="A159"/>
     </row>
     <row r="160">
-      <c s="6" r="A160"/>
+      <c s="7" r="A160"/>
     </row>
     <row r="161">
-      <c s="6" r="A161"/>
+      <c s="7" r="A161"/>
     </row>
     <row r="162">
-      <c s="6" r="A162"/>
+      <c s="7" r="A162"/>
     </row>
     <row r="163">
-      <c s="6" r="A163"/>
+      <c s="7" r="A163"/>
     </row>
     <row r="164">
-      <c s="6" r="A164"/>
+      <c s="7" r="A164"/>
     </row>
     <row r="165">
-      <c s="6" r="A165"/>
+      <c s="7" r="A165"/>
     </row>
     <row r="166">
-      <c s="6" r="A166"/>
+      <c s="7" r="A166"/>
     </row>
     <row r="167">
-      <c s="6" r="A167"/>
+      <c s="7" r="A167"/>
     </row>
     <row r="168">
-      <c s="6" r="A168"/>
+      <c s="7" r="A168"/>
     </row>
     <row r="169">
-      <c s="6" r="A169"/>
+      <c s="7" r="A169"/>
     </row>
     <row r="170">
-      <c s="6" r="A170"/>
+      <c s="7" r="A170"/>
     </row>
     <row r="171">
-      <c s="6" r="A171"/>
+      <c s="7" r="A171"/>
     </row>
     <row r="172">
-      <c s="6" r="A172"/>
+      <c s="7" r="A172"/>
     </row>
     <row r="173">
-      <c s="6" r="A173"/>
+      <c s="7" r="A173"/>
     </row>
     <row r="174">
-      <c s="6" r="A174"/>
+      <c s="7" r="A174"/>
     </row>
     <row r="175">
-      <c s="6" r="A175"/>
+      <c s="7" r="A175"/>
     </row>
     <row r="176">
-      <c s="6" r="A176"/>
+      <c s="7" r="A176"/>
     </row>
     <row r="177">
-      <c s="6" r="A177"/>
+      <c s="7" r="A177"/>
     </row>
     <row r="178">
-      <c s="6" r="A178"/>
+      <c s="7" r="A178"/>
     </row>
     <row r="179">
-      <c s="6" r="A179"/>
+      <c s="7" r="A179"/>
     </row>
     <row r="180">
-      <c s="6" r="A180"/>
+      <c s="7" r="A180"/>
     </row>
     <row r="181">
-      <c s="6" r="A181"/>
+      <c s="7" r="A181"/>
     </row>
     <row r="182">
-      <c s="6" r="A182"/>
+      <c s="7" r="A182"/>
     </row>
     <row r="183">
-      <c s="6" r="A183"/>
+      <c s="7" r="A183"/>
     </row>
     <row r="184">
-      <c s="6" r="A184"/>
+      <c s="7" r="A184"/>
     </row>
     <row r="185">
-      <c s="6" r="A185"/>
+      <c s="7" r="A185"/>
     </row>
     <row r="186">
-      <c s="6" r="A186"/>
+      <c s="7" r="A186"/>
     </row>
     <row r="187">
-      <c s="6" r="A187"/>
+      <c s="7" r="A187"/>
     </row>
     <row r="188">
-      <c s="6" r="A188"/>
+      <c s="7" r="A188"/>
     </row>
     <row r="189">
-      <c s="6" r="A189"/>
+      <c s="7" r="A189"/>
     </row>
     <row r="190">
-      <c s="6" r="A190"/>
+      <c s="7" r="A190"/>
     </row>
     <row r="191">
-      <c s="6" r="A191"/>
+      <c s="7" r="A191"/>
     </row>
     <row r="192">
-      <c s="6" r="A192"/>
+      <c s="7" r="A192"/>
     </row>
     <row r="193">
-      <c s="6" r="A193"/>
+      <c s="7" r="A193"/>
     </row>
     <row r="194">
-      <c s="6" r="A194"/>
+      <c s="7" r="A194"/>
     </row>
     <row r="195">
-      <c s="6" r="A195"/>
+      <c s="7" r="A195"/>
     </row>
     <row r="196">
-      <c s="6" r="A196"/>
+      <c s="7" r="A196"/>
     </row>
     <row r="197">
-      <c s="6" r="A197"/>
+      <c s="7" r="A197"/>
     </row>
     <row r="198">
-      <c s="6" r="A198"/>
+      <c s="7" r="A198"/>
     </row>
     <row r="199">
-      <c s="6" r="A199"/>
+      <c s="7" r="A199"/>
     </row>
     <row r="200">
-      <c s="6" r="A200"/>
+      <c s="7" r="A200"/>
     </row>
     <row r="201">
-      <c s="6" r="A201"/>
+      <c s="7" r="A201"/>
     </row>
     <row r="202">
-      <c s="6" r="A202"/>
+      <c s="7" r="A202"/>
     </row>
     <row r="203">
-      <c s="6" r="A203"/>
+      <c s="7" r="A203"/>
     </row>
     <row r="204">
-      <c s="6" r="A204"/>
+      <c s="7" r="A204"/>
     </row>
     <row r="205">
-      <c s="6" r="A205"/>
+      <c s="7" r="A205"/>
     </row>
     <row r="206">
-      <c s="6" r="A206"/>
+      <c s="7" r="A206"/>
     </row>
     <row r="207">
-      <c s="6" r="A207"/>
+      <c s="7" r="A207"/>
     </row>
     <row r="208">
-      <c s="6" r="A208"/>
+      <c s="7" r="A208"/>
     </row>
     <row r="209">
-      <c s="6" r="A209"/>
+      <c s="7" r="A209"/>
     </row>
     <row r="210">
-      <c s="6" r="A210"/>
+      <c s="7" r="A210"/>
     </row>
     <row r="211">
-      <c s="6" r="A211"/>
+      <c s="7" r="A211"/>
     </row>
     <row r="212">
-      <c s="6" r="A212"/>
+      <c s="7" r="A212"/>
     </row>
     <row r="213">
-      <c s="6" r="A213"/>
+      <c s="7" r="A213"/>
     </row>
     <row r="214">
-      <c s="6" r="A214"/>
+      <c s="7" r="A214"/>
     </row>
     <row r="215">
-      <c s="6" r="A215"/>
+      <c s="7" r="A215"/>
     </row>
     <row r="216">
-      <c s="6" r="A216"/>
+      <c s="7" r="A216"/>
     </row>
     <row r="217">
-      <c s="6" r="A217"/>
+      <c s="7" r="A217"/>
     </row>
     <row r="218">
-      <c s="6" r="A218"/>
+      <c s="7" r="A218"/>
     </row>
     <row r="219">
-      <c s="6" r="A219"/>
+      <c s="7" r="A219"/>
     </row>
     <row r="220">
-      <c s="6" r="A220"/>
+      <c s="7" r="A220"/>
     </row>
     <row r="221">
-      <c s="6" r="A221"/>
+      <c s="7" r="A221"/>
     </row>
     <row r="222">
-      <c s="6" r="A222"/>
+      <c s="7" r="A222"/>
     </row>
     <row r="223">
-      <c s="6" r="A223"/>
+      <c s="7" r="A223"/>
     </row>
     <row r="224">
-      <c s="6" r="A224"/>
+      <c s="7" r="A224"/>
     </row>
     <row r="225">
-      <c s="6" r="A225"/>
+      <c s="7" r="A225"/>
     </row>
     <row r="226">
-      <c s="6" r="A226"/>
+      <c s="7" r="A226"/>
     </row>
     <row r="227">
-      <c s="6" r="A227"/>
+      <c s="7" r="A227"/>
     </row>
     <row r="228">
-      <c s="6" r="A228"/>
+      <c s="7" r="A228"/>
     </row>
     <row r="229">
-      <c s="6" r="A229"/>
+      <c s="7" r="A229"/>
     </row>
     <row r="230">
-      <c s="6" r="A230"/>
+      <c s="7" r="A230"/>
     </row>
     <row r="231">
-      <c s="6" r="A231"/>
+      <c s="7" r="A231"/>
     </row>
     <row r="232">
-      <c s="6" r="A232"/>
+      <c s="7" r="A232"/>
     </row>
     <row r="233">
-      <c s="6" r="A233"/>
+      <c s="7" r="A233"/>
     </row>
     <row r="234">
-      <c s="6" r="A234"/>
+      <c s="7" r="A234"/>
     </row>
     <row r="235">
-      <c s="6" r="A235"/>
+      <c s="7" r="A235"/>
     </row>
     <row r="236">
-      <c s="6" r="A236"/>
+      <c s="7" r="A236"/>
     </row>
     <row r="237">
-      <c s="6" r="A237"/>
+      <c s="7" r="A237"/>
     </row>
     <row r="238">
-      <c s="6" r="A238"/>
+      <c s="7" r="A238"/>
     </row>
     <row r="239">
-      <c s="6" r="A239"/>
+      <c s="7" r="A239"/>
     </row>
     <row r="240">
-      <c s="6" r="A240"/>
+      <c s="7" r="A240"/>
     </row>
     <row r="241">
-      <c s="6" r="A241"/>
+      <c s="7" r="A241"/>
     </row>
     <row r="242">
-      <c s="6" r="A242"/>
+      <c s="7" r="A242"/>
     </row>
     <row r="243">
-      <c s="6" r="A243"/>
+      <c s="7" r="A243"/>
     </row>
     <row r="244">
-      <c s="6" r="A244"/>
+      <c s="7" r="A244"/>
     </row>
     <row r="245">
-      <c s="6" r="A245"/>
+      <c s="7" r="A245"/>
     </row>
     <row r="246">
-      <c s="6" r="A246"/>
+      <c s="7" r="A246"/>
     </row>
     <row r="247">
-      <c s="6" r="A247"/>
+      <c s="7" r="A247"/>
     </row>
     <row r="248">
-      <c s="6" r="A248"/>
+      <c s="7" r="A248"/>
     </row>
     <row r="249">
-      <c s="6" r="A249"/>
+      <c s="7" r="A249"/>
     </row>
     <row r="250">
-      <c s="6" r="A250"/>
+      <c s="7" r="A250"/>
     </row>
     <row r="251">
-      <c s="6" r="A251"/>
+      <c s="7" r="A251"/>
     </row>
     <row r="252">
-      <c s="6" r="A252"/>
+      <c s="7" r="A252"/>
     </row>
     <row r="253">
-      <c s="6" r="A253"/>
+      <c s="7" r="A253"/>
     </row>
     <row r="254">
-      <c s="6" r="A254"/>
+      <c s="7" r="A254"/>
     </row>
     <row r="255">
-      <c s="6" r="A255"/>
+      <c s="7" r="A255"/>
     </row>
     <row r="256">
-      <c s="6" r="A256"/>
+      <c s="7" r="A256"/>
     </row>
     <row r="257">
-      <c s="6" r="A257"/>
+      <c s="7" r="A257"/>
     </row>
     <row r="258">
-      <c s="6" r="A258"/>
+      <c s="7" r="A258"/>
     </row>
     <row r="259">
-      <c s="6" r="A259"/>
+      <c s="7" r="A259"/>
     </row>
     <row r="260">
-      <c s="6" r="A260"/>
+      <c s="7" r="A260"/>
     </row>
     <row r="261">
-      <c s="6" r="A261"/>
+      <c s="7" r="A261"/>
     </row>
     <row r="262">
-      <c s="6" r="A262"/>
+      <c s="7" r="A262"/>
     </row>
     <row r="263">
-      <c s="6" r="A263"/>
+      <c s="7" r="A263"/>
     </row>
     <row r="264">
-      <c s="6" r="A264"/>
+      <c s="7" r="A264"/>
     </row>
     <row r="265">
-      <c s="6" r="A265"/>
+      <c s="7" r="A265"/>
     </row>
     <row r="266">
-      <c s="6" r="A266"/>
+      <c s="7" r="A266"/>
     </row>
     <row r="267">
-      <c s="6" r="A267"/>
+      <c s="7" r="A267"/>
     </row>
     <row r="268">
-      <c s="6" r="A268"/>
+      <c s="7" r="A268"/>
     </row>
     <row r="269">
-      <c s="6" r="A269"/>
+      <c s="7" r="A269"/>
     </row>
     <row r="270">
-      <c s="6" r="A270"/>
+      <c s="7" r="A270"/>
     </row>
     <row r="271">
-      <c s="6" r="A271"/>
+      <c s="7" r="A271"/>
     </row>
     <row r="272">
-      <c s="6" r="A272"/>
+      <c s="7" r="A272"/>
     </row>
     <row r="273">
-      <c s="6" r="A273"/>
+      <c s="7" r="A273"/>
     </row>
     <row r="274">
-      <c s="6" r="A274"/>
+      <c s="7" r="A274"/>
     </row>
     <row r="275">
-      <c s="6" r="A275"/>
+      <c s="7" r="A275"/>
     </row>
     <row r="276">
-      <c s="6" r="A276"/>
+      <c s="7" r="A276"/>
     </row>
     <row r="277">
-      <c s="6" r="A277"/>
+      <c s="7" r="A277"/>
     </row>
     <row r="278">
-      <c s="6" r="A278"/>
+      <c s="7" r="A278"/>
     </row>
     <row r="279">
-      <c s="6" r="A279"/>
+      <c s="7" r="A279"/>
     </row>
     <row r="280">
-      <c s="6" r="A280"/>
+      <c s="7" r="A280"/>
     </row>
     <row r="281">
-      <c s="6" r="A281"/>
+      <c s="7" r="A281"/>
     </row>
     <row r="282">
-      <c s="6" r="A282"/>
+      <c s="7" r="A282"/>
     </row>
     <row r="283">
-      <c s="6" r="A283"/>
+      <c s="7" r="A283"/>
     </row>
     <row r="284">
-      <c s="6" r="A284"/>
+      <c s="7" r="A284"/>
     </row>
     <row r="285">
-      <c s="6" r="A285"/>
+      <c s="7" r="A285"/>
     </row>
     <row r="286">
-      <c s="6" r="A286"/>
+      <c s="7" r="A286"/>
     </row>
     <row r="287">
-      <c s="6" r="A287"/>
+      <c s="7" r="A287"/>
     </row>
     <row r="288">
-      <c s="6" r="A288"/>
+      <c s="7" r="A288"/>
     </row>
     <row r="289">
-      <c s="6" r="A289"/>
+      <c s="7" r="A289"/>
     </row>
     <row r="290">
-      <c s="6" r="A290"/>
+      <c s="7" r="A290"/>
     </row>
     <row r="291">
-      <c s="6" r="A291"/>
+      <c s="7" r="A291"/>
     </row>
     <row r="292">
-      <c s="6" r="A292"/>
+      <c s="7" r="A292"/>
     </row>
     <row r="293">
-      <c s="6" r="A293"/>
+      <c s="7" r="A293"/>
     </row>
     <row r="294">
-      <c s="6" r="A294"/>
+      <c s="7" r="A294"/>
     </row>
     <row r="295">
-      <c s="6" r="A295"/>
+      <c s="7" r="A295"/>
     </row>
     <row r="296">
-      <c s="6" r="A296"/>
+      <c s="7" r="A296"/>
     </row>
     <row r="297">
-      <c s="6" r="A297"/>
+      <c s="7" r="A297"/>
     </row>
     <row r="298">
-      <c s="6" r="A298"/>
+      <c s="7" r="A298"/>
     </row>
     <row r="299">
-      <c s="6" r="A299"/>
+      <c s="7" r="A299"/>
     </row>
     <row r="300">
-      <c s="6" r="A300"/>
+      <c s="7" r="A300"/>
     </row>
     <row r="301">
-      <c s="6" r="A301"/>
+      <c s="7" r="A301"/>
     </row>
     <row r="302">
-      <c s="6" r="A302"/>
+      <c s="7" r="A302"/>
     </row>
     <row r="303">
-      <c s="6" r="A303"/>
+      <c s="7" r="A303"/>
     </row>
     <row r="304">
-      <c s="6" r="A304"/>
+      <c s="7" r="A304"/>
     </row>
     <row r="305">
-      <c s="6" r="A305"/>
+      <c s="7" r="A305"/>
     </row>
     <row r="306">
-      <c s="6" r="A306"/>
+      <c s="7" r="A306"/>
     </row>
     <row r="307">
-      <c s="6" r="A307"/>
+      <c s="7" r="A307"/>
     </row>
     <row r="308">
-      <c s="6" r="A308"/>
+      <c s="7" r="A308"/>
     </row>
     <row r="309">
-      <c s="6" r="A309"/>
+      <c s="7" r="A309"/>
     </row>
     <row r="310">
-      <c s="6" r="A310"/>
+      <c s="7" r="A310"/>
     </row>
     <row r="311">
-      <c s="6" r="A311"/>
+      <c s="7" r="A311"/>
     </row>
     <row r="312">
-      <c s="6" r="A312"/>
+      <c s="7" r="A312"/>
     </row>
     <row r="313">
-      <c s="6" r="A313"/>
+      <c s="7" r="A313"/>
     </row>
     <row r="314">
-      <c s="6" r="A314"/>
+      <c s="7" r="A314"/>
     </row>
     <row r="315">
-      <c s="6" r="A315"/>
+      <c s="7" r="A315"/>
     </row>
     <row r="316">
-      <c s="6" r="A316"/>
+      <c s="7" r="A316"/>
     </row>
     <row r="317">
-      <c s="6" r="A317"/>
+      <c s="7" r="A317"/>
     </row>
     <row r="318">
-      <c s="6" r="A318"/>
+      <c s="7" r="A318"/>
     </row>
     <row r="319">
-      <c s="6" r="A319"/>
+      <c s="7" r="A319"/>
     </row>
     <row r="320">
-      <c s="6" r="A320"/>
+      <c s="7" r="A320"/>
     </row>
     <row r="321">
-      <c s="6" r="A321"/>
+      <c s="7" r="A321"/>
     </row>
     <row r="322">
-      <c s="6" r="A322"/>
+      <c s="7" r="A322"/>
     </row>
     <row r="323">
-      <c s="6" r="A323"/>
+      <c s="7" r="A323"/>
     </row>
     <row r="324">
-      <c s="6" r="A324"/>
+      <c s="7" r="A324"/>
     </row>
     <row r="325">
-      <c s="6" r="A325"/>
+      <c s="7" r="A325"/>
     </row>
     <row r="326">
-      <c s="6" r="A326"/>
+      <c s="7" r="A326"/>
     </row>
     <row r="327">
-      <c s="6" r="A327"/>
+      <c s="7" r="A327"/>
     </row>
     <row r="328">
-      <c s="6" r="A328"/>
+      <c s="7" r="A328"/>
     </row>
     <row r="329">
-      <c s="6" r="A329"/>
+      <c s="7" r="A329"/>
     </row>
     <row r="330">
-      <c s="6" r="A330"/>
+      <c s="7" r="A330"/>
     </row>
     <row r="331">
-      <c s="6" r="A331"/>
+      <c s="7" r="A331"/>
     </row>
     <row r="332">
-      <c s="6" r="A332"/>
+      <c s="7" r="A332"/>
     </row>
     <row r="333">
-      <c s="6" r="A333"/>
+      <c s="7" r="A333"/>
     </row>
     <row r="334">
-      <c s="6" r="A334"/>
+      <c s="7" r="A334"/>
     </row>
     <row r="335">
-      <c s="6" r="A335"/>
+      <c s="7" r="A335"/>
     </row>
     <row r="336">
-      <c s="6" r="A336"/>
+      <c s="7" r="A336"/>
     </row>
     <row r="337">
-      <c s="6" r="A337"/>
+      <c s="7" r="A337"/>
     </row>
     <row r="338">
-      <c s="6" r="A338"/>
+      <c s="7" r="A338"/>
     </row>
     <row r="339">
-      <c s="6" r="A339"/>
+      <c s="7" r="A339"/>
     </row>
     <row r="340">
-      <c s="6" r="A340"/>
+      <c s="7" r="A340"/>
     </row>
     <row r="341">
-      <c s="6" r="A341"/>
+      <c s="7" r="A341"/>
     </row>
     <row r="342">
-      <c s="6" r="A342"/>
+      <c s="7" r="A342"/>
     </row>
     <row r="343">
-      <c s="6" r="A343"/>
+      <c s="7" r="A343"/>
     </row>
     <row r="344">
-      <c s="6" r="A344"/>
+      <c s="7" r="A344"/>
     </row>
     <row r="345">
-      <c s="6" r="A345"/>
+      <c s="7" r="A345"/>
     </row>
     <row r="346">
-      <c s="6" r="A346"/>
+      <c s="7" r="A346"/>
     </row>
     <row r="347">
-      <c s="6" r="A347"/>
+      <c s="7" r="A347"/>
     </row>
     <row r="348">
-      <c s="6" r="A348"/>
+      <c s="7" r="A348"/>
     </row>
     <row r="349">
-      <c s="6" r="A349"/>
+      <c s="7" r="A349"/>
     </row>
     <row r="350">
-      <c s="6" r="A350"/>
+      <c s="7" r="A350"/>
     </row>
     <row r="351">
-      <c s="6" r="A351"/>
+      <c s="7" r="A351"/>
     </row>
     <row r="352">
-      <c s="6" r="A352"/>
+      <c s="7" r="A352"/>
     </row>
     <row r="353">
-      <c s="6" r="A353"/>
+      <c s="7" r="A353"/>
     </row>
     <row r="354">
-      <c s="6" r="A354"/>
+      <c s="7" r="A354"/>
     </row>
     <row r="355">
-      <c s="6" r="A355"/>
+      <c s="7" r="A355"/>
     </row>
     <row r="356">
-      <c s="6" r="A356"/>
+      <c s="7" r="A356"/>
     </row>
     <row r="357">
-      <c s="6" r="A357"/>
+      <c s="7" r="A357"/>
     </row>
     <row r="358">
-      <c s="6" r="A358"/>
+      <c s="7" r="A358"/>
     </row>
     <row r="359">
-      <c s="6" r="A359"/>
+      <c s="7" r="A359"/>
     </row>
     <row r="360">
-      <c s="6" r="A360"/>
+      <c s="7" r="A360"/>
     </row>
     <row r="361">
-      <c s="6" r="A361"/>
+      <c s="7" r="A361"/>
     </row>
     <row r="362">
-      <c s="6" r="A362"/>
+      <c s="7" r="A362"/>
     </row>
     <row r="363">
-      <c s="6" r="A363"/>
+      <c s="7" r="A363"/>
     </row>
     <row r="364">
-      <c s="6" r="A364"/>
+      <c s="7" r="A364"/>
     </row>
     <row r="365">
-      <c s="6" r="A365"/>
+      <c s="7" r="A365"/>
     </row>
     <row r="366">
-      <c s="6" r="A366"/>
+      <c s="7" r="A366"/>
     </row>
     <row r="367">
-      <c s="6" r="A367"/>
+      <c s="7" r="A367"/>
     </row>
     <row r="368">
-      <c s="6" r="A368"/>
+      <c s="7" r="A368"/>
     </row>
     <row r="369">
-      <c s="6" r="A369"/>
+      <c s="7" r="A369"/>
     </row>
     <row r="370">
-      <c s="6" r="A370"/>
+      <c s="7" r="A370"/>
     </row>
     <row r="371">
-      <c s="6" r="A371"/>
+      <c s="7" r="A371"/>
     </row>
     <row r="372">
-      <c s="6" r="A372"/>
+      <c s="7" r="A372"/>
     </row>
     <row r="373">
-      <c s="6" r="A373"/>
+      <c s="7" r="A373"/>
     </row>
     <row r="374">
-      <c s="6" r="A374"/>
+      <c s="7" r="A374"/>
     </row>
     <row r="375">
-      <c s="6" r="A375"/>
+      <c s="7" r="A375"/>
     </row>
     <row r="376">
-      <c s="6" r="A376"/>
+      <c s="7" r="A376"/>
     </row>
     <row r="377">
-      <c s="6" r="A377"/>
+      <c s="7" r="A377"/>
     </row>
     <row r="378">
-      <c s="6" r="A378"/>
+      <c s="7" r="A378"/>
     </row>
     <row r="379">
-      <c s="6" r="A379"/>
+      <c s="7" r="A379"/>
     </row>
     <row r="380">
-      <c s="6" r="A380"/>
+      <c s="7" r="A380"/>
     </row>
     <row r="381">
-      <c s="6" r="A381"/>
+      <c s="7" r="A381"/>
     </row>
     <row r="382">
-      <c s="6" r="A382"/>
+      <c s="7" r="A382"/>
     </row>
     <row r="383">
-      <c s="6" r="A383"/>
+      <c s="7" r="A383"/>
     </row>
     <row r="384">
-      <c s="6" r="A384"/>
+      <c s="7" r="A384"/>
     </row>
     <row r="385">
-      <c s="6" r="A385"/>
+      <c s="7" r="A385"/>
     </row>
     <row r="386">
-      <c s="6" r="A386"/>
+      <c s="7" r="A386"/>
     </row>
     <row r="387">
-      <c s="6" r="A387"/>
+      <c s="7" r="A387"/>
     </row>
     <row r="388">
-      <c s="6" r="A388"/>
+      <c s="7" r="A388"/>
     </row>
     <row r="389">
-      <c s="6" r="A389"/>
+      <c s="7" r="A389"/>
     </row>
     <row r="390">
-      <c s="6" r="A390"/>
+      <c s="7" r="A390"/>
     </row>
     <row r="391">
-      <c s="6" r="A391"/>
+      <c s="7" r="A391"/>
     </row>
     <row r="392">
-      <c s="6" r="A392"/>
+      <c s="7" r="A392"/>
     </row>
     <row r="393">
-      <c s="6" r="A393"/>
+      <c s="7" r="A393"/>
     </row>
     <row r="394">
-      <c s="6" r="A394"/>
+      <c s="7" r="A394"/>
     </row>
     <row r="395">
-      <c s="6" r="A395"/>
+      <c s="7" r="A395"/>
     </row>
     <row r="396">
-      <c s="6" r="A396"/>
+      <c s="7" r="A396"/>
     </row>
     <row r="397">
-      <c s="6" r="A397"/>
+      <c s="7" r="A397"/>
     </row>
     <row r="398">
-      <c s="6" r="A398"/>
+      <c s="7" r="A398"/>
     </row>
     <row r="399">
-      <c s="6" r="A399"/>
+      <c s="7" r="A399"/>
     </row>
     <row r="400">
-      <c s="6" r="A400"/>
+      <c s="7" r="A400"/>
     </row>
     <row r="401">
-      <c s="6" r="A401"/>
+      <c s="7" r="A401"/>
     </row>
     <row r="402">
-      <c s="6" r="A402"/>
+      <c s="7" r="A402"/>
     </row>
     <row r="403">
-      <c s="6" r="A403"/>
+      <c s="7" r="A403"/>
     </row>
     <row r="404">
-      <c s="6" r="A404"/>
+      <c s="7" r="A404"/>
     </row>
     <row r="405">
-      <c s="6" r="A405"/>
+      <c s="7" r="A405"/>
     </row>
     <row r="406">
-      <c s="6" r="A406"/>
+      <c s="7" r="A406"/>
     </row>
     <row r="407">
-      <c s="6" r="A407"/>
+      <c s="7" r="A407"/>
     </row>
     <row r="408">
-      <c s="6" r="A408"/>
+      <c s="7" r="A408"/>
     </row>
     <row r="409">
-      <c s="6" r="A409"/>
+      <c s="7" r="A409"/>
     </row>
     <row r="410">
-      <c s="6" r="A410"/>
+      <c s="7" r="A410"/>
     </row>
     <row r="411">
-      <c s="6" r="A411"/>
+      <c s="7" r="A411"/>
     </row>
     <row r="412">
-      <c s="6" r="A412"/>
+      <c s="7" r="A412"/>
     </row>
     <row r="413">
-      <c s="6" r="A413"/>
+      <c s="7" r="A413"/>
     </row>
     <row r="414">
-      <c s="6" r="A414"/>
+      <c s="7" r="A414"/>
     </row>
     <row r="415">
-      <c s="6" r="A415"/>
+      <c s="7" r="A415"/>
     </row>
     <row r="416">
-      <c s="6" r="A416"/>
+      <c s="7" r="A416"/>
     </row>
     <row r="417">
-      <c s="6" r="A417"/>
+      <c s="7" r="A417"/>
     </row>
     <row r="418">
-      <c s="6" r="A418"/>
+      <c s="7" r="A418"/>
     </row>
     <row r="419">
-      <c s="6" r="A419"/>
+      <c s="7" r="A419"/>
     </row>
     <row r="420">
-      <c s="6" r="A420"/>
+      <c s="7" r="A420"/>
     </row>
     <row r="421">
-      <c s="6" r="A421"/>
+      <c s="7" r="A421"/>
     </row>
     <row r="422">
-      <c s="6" r="A422"/>
+      <c s="7" r="A422"/>
     </row>
     <row r="423">
-      <c s="6" r="A423"/>
+      <c s="7" r="A423"/>
     </row>
     <row r="424">
-      <c s="6" r="A424"/>
+      <c s="7" r="A424"/>
     </row>
     <row r="425">
-      <c s="6" r="A425"/>
+      <c s="7" r="A425"/>
     </row>
     <row r="426">
-      <c s="6" r="A426"/>
+      <c s="7" r="A426"/>
     </row>
     <row r="427">
-      <c s="6" r="A427"/>
+      <c s="7" r="A427"/>
     </row>
     <row r="428">
-      <c s="6" r="A428"/>
+      <c s="7" r="A428"/>
     </row>
     <row r="429">
-      <c s="6" r="A429"/>
+      <c s="7" r="A429"/>
     </row>
     <row r="430">
-      <c s="6" r="A430"/>
+      <c s="7" r="A430"/>
     </row>
     <row r="431">
-      <c s="6" r="A431"/>
+      <c s="7" r="A431"/>
     </row>
     <row r="432">
-      <c s="6" r="A432"/>
+      <c s="7" r="A432"/>
     </row>
     <row r="433">
-      <c s="6" r="A433"/>
+      <c s="7" r="A433"/>
     </row>
     <row r="434">
-      <c s="6" r="A434"/>
+      <c s="7" r="A434"/>
     </row>
     <row r="435">
-      <c s="6" r="A435"/>
+      <c s="7" r="A435"/>
     </row>
     <row r="436">
-      <c s="6" r="A436"/>
+      <c s="7" r="A436"/>
     </row>
     <row r="437">
-      <c s="6" r="A437"/>
+      <c s="7" r="A437"/>
     </row>
     <row r="438">
-      <c s="6" r="A438"/>
+      <c s="7" r="A438"/>
     </row>
     <row r="439">
-      <c s="6" r="A439"/>
+      <c s="7" r="A439"/>
     </row>
     <row r="440">
-      <c s="6" r="A440"/>
+      <c s="7" r="A440"/>
     </row>
     <row r="441">
-      <c s="6" r="A441"/>
+      <c s="7" r="A441"/>
     </row>
     <row r="442">
-      <c s="6" r="A442"/>
+      <c s="7" r="A442"/>
     </row>
     <row r="443">
-      <c s="6" r="A443"/>
+      <c s="7" r="A443"/>
     </row>
     <row r="444">
-      <c s="6" r="A444"/>
+      <c s="7" r="A444"/>
     </row>
     <row r="445">
-      <c s="6" r="A445"/>
+      <c s="7" r="A445"/>
     </row>
     <row r="446">
-      <c s="6" r="A446"/>
+      <c s="7" r="A446"/>
     </row>
     <row r="447">
-      <c s="6" r="A447"/>
+      <c s="7" r="A447"/>
     </row>
     <row r="448">
-      <c s="6" r="A448"/>
+      <c s="7" r="A448"/>
     </row>
     <row r="449">
-      <c s="6" r="A449"/>
+      <c s="7" r="A449"/>
     </row>
     <row r="450">
-      <c s="6" r="A450"/>
+      <c s="7" r="A450"/>
     </row>
     <row r="451">
-      <c s="6" r="A451"/>
+      <c s="7" r="A451"/>
     </row>
     <row r="452">
-      <c s="6" r="A452"/>
+      <c s="7" r="A452"/>
     </row>
     <row r="453">
-      <c s="6" r="A453"/>
+      <c s="7" r="A453"/>
     </row>
     <row r="454">
-      <c s="6" r="A454"/>
+      <c s="7" r="A454"/>
     </row>
     <row r="455">
-      <c s="6" r="A455"/>
+      <c s="7" r="A455"/>
     </row>
     <row r="456">
-      <c s="6" r="A456"/>
+      <c s="7" r="A456"/>
     </row>
     <row r="457">
-      <c s="6" r="A457"/>
+      <c s="7" r="A457"/>
     </row>
     <row r="458">
-      <c s="6" r="A458"/>
+      <c s="7" r="A458"/>
     </row>
     <row r="459">
-      <c s="6" r="A459"/>
+      <c s="7" r="A459"/>
     </row>
     <row r="460">
-      <c s="6" r="A460"/>
+      <c s="7" r="A460"/>
     </row>
     <row r="461">
-      <c s="6" r="A461"/>
+      <c s="7" r="A461"/>
     </row>
     <row r="462">
-      <c s="6" r="A462"/>
+      <c s="7" r="A462"/>
     </row>
     <row r="463">
-      <c s="6" r="A463"/>
+      <c s="7" r="A463"/>
     </row>
     <row r="464">
-      <c s="6" r="A464"/>
+      <c s="7" r="A464"/>
     </row>
     <row r="465">
-      <c s="6" r="A465"/>
+      <c s="7" r="A465"/>
     </row>
     <row r="466">
-      <c s="6" r="A466"/>
+      <c s="7" r="A466"/>
     </row>
     <row r="467">
-      <c s="6" r="A467"/>
+      <c s="7" r="A467"/>
     </row>
     <row r="468">
-      <c s="6" r="A468"/>
+      <c s="7" r="A468"/>
     </row>
     <row r="469">
-      <c s="6" r="A469"/>
+      <c s="7" r="A469"/>
     </row>
     <row r="470">
-      <c s="6" r="A470"/>
+      <c s="7" r="A470"/>
     </row>
     <row r="471">
-      <c s="6" r="A471"/>
+      <c s="7" r="A471"/>
     </row>
     <row r="472">
-      <c s="6" r="A472"/>
+      <c s="7" r="A472"/>
     </row>
     <row r="473">
-      <c s="6" r="A473"/>
+      <c s="7" r="A473"/>
     </row>
     <row r="474">
-      <c s="6" r="A474"/>
+      <c s="7" r="A474"/>
     </row>
     <row r="475">
-      <c s="6" r="A475"/>
+      <c s="7" r="A475"/>
     </row>
     <row r="476">
-      <c s="6" r="A476"/>
+      <c s="7" r="A476"/>
     </row>
     <row r="477">
-      <c s="6" r="A477"/>
+      <c s="7" r="A477"/>
     </row>
     <row r="478">
-      <c s="6" r="A478"/>
+      <c s="7" r="A478"/>
     </row>
     <row r="479">
-      <c s="6" r="A479"/>
+      <c s="7" r="A479"/>
     </row>
     <row r="480">
-      <c s="6" r="A480"/>
+      <c s="7" r="A480"/>
     </row>
     <row r="481">
-      <c s="6" r="A481"/>
+      <c s="7" r="A481"/>
     </row>
     <row r="482">
-      <c s="6" r="A482"/>
+      <c s="7" r="A482"/>
     </row>
     <row r="483">
-      <c s="6" r="A483"/>
+      <c s="7" r="A483"/>
     </row>
     <row r="484">
-      <c s="6" r="A484"/>
+      <c s="7" r="A484"/>
     </row>
     <row r="485">
-      <c s="6" r="A485"/>
+      <c s="7" r="A485"/>
     </row>
     <row r="486">
-      <c s="6" r="A486"/>
+      <c s="7" r="A486"/>
     </row>
     <row r="487">
-      <c s="6" r="A487"/>
+      <c s="7" r="A487"/>
     </row>
     <row r="488">
-      <c s="6" r="A488"/>
+      <c s="7" r="A488"/>
     </row>
     <row r="489">
-      <c s="6" r="A489"/>
+      <c s="7" r="A489"/>
     </row>
     <row r="490">
-      <c s="6" r="A490"/>
+      <c s="7" r="A490"/>
     </row>
     <row r="491">
-      <c s="6" r="A491"/>
+      <c s="7" r="A491"/>
     </row>
     <row r="492">
-      <c s="6" r="A492"/>
+      <c s="7" r="A492"/>
     </row>
     <row r="493">
-      <c s="6" r="A493"/>
+      <c s="7" r="A493"/>
     </row>
     <row r="494">
-      <c s="6" r="A494"/>
+      <c s="7" r="A494"/>
     </row>
     <row r="495">
-      <c s="6" r="A495"/>
+      <c s="7" r="A495"/>
     </row>
     <row r="496">
-      <c s="6" r="A496"/>
+      <c s="7" r="A496"/>
     </row>
     <row r="497">
-      <c s="6" r="A497"/>
+      <c s="7" r="A497"/>
     </row>
     <row r="498">
-      <c s="6" r="A498"/>
+      <c s="7" r="A498"/>
     </row>
     <row r="499">
-      <c s="6" r="A499"/>
+      <c s="7" r="A499"/>
     </row>
     <row r="500">
-      <c s="6" r="A500"/>
+      <c s="7" r="A500"/>
     </row>
     <row r="501">
-      <c s="6" r="A501"/>
+      <c s="7" r="A501"/>
     </row>
     <row r="502">
-      <c s="6" r="A502"/>
+      <c s="7" r="A502"/>
     </row>
     <row r="503">
-      <c s="6" r="A503"/>
+      <c s="7" r="A503"/>
     </row>
     <row r="504">
-      <c s="6" r="A504"/>
+      <c s="7" r="A504"/>
     </row>
     <row r="505">
-      <c s="6" r="A505"/>
+      <c s="7" r="A505"/>
     </row>
     <row r="506">
-      <c s="6" r="A506"/>
+      <c s="7" r="A506"/>
     </row>
     <row r="507">
-      <c s="6" r="A507"/>
+      <c s="7" r="A507"/>
     </row>
     <row r="508">
-      <c s="6" r="A508"/>
+      <c s="7" r="A508"/>
     </row>
     <row r="509">
-      <c s="6" r="A509"/>
+      <c s="7" r="A509"/>
     </row>
     <row r="510">
-      <c s="6" r="A510"/>
+      <c s="7" r="A510"/>
     </row>
     <row r="511">
-      <c s="6" r="A511"/>
+      <c s="7" r="A511"/>
     </row>
     <row r="512">
-      <c s="6" r="A512"/>
+      <c s="7" r="A512"/>
     </row>
     <row r="513">
-      <c s="6" r="A513"/>
+      <c s="7" r="A513"/>
     </row>
     <row r="514">
-      <c s="6" r="A514"/>
+      <c s="7" r="A514"/>
     </row>
     <row r="515">
-      <c s="6" r="A515"/>
+      <c s="7" r="A515"/>
     </row>
     <row r="516">
-      <c s="6" r="A516"/>
+      <c s="7" r="A516"/>
     </row>
     <row r="517">
-      <c s="6" r="A517"/>
+      <c s="7" r="A517"/>
     </row>
     <row r="518">
-      <c s="6" r="A518"/>
+      <c s="7" r="A518"/>
     </row>
     <row r="519">
-      <c s="6" r="A519"/>
+      <c s="7" r="A519"/>
     </row>
     <row r="520">
-      <c s="6" r="A520"/>
+      <c s="7" r="A520"/>
     </row>
     <row r="521">
-      <c s="6" r="A521"/>
+      <c s="7" r="A521"/>
     </row>
     <row r="522">
-      <c s="6" r="A522"/>
+      <c s="7" r="A522"/>
     </row>
     <row r="523">
-      <c s="6" r="A523"/>
+      <c s="7" r="A523"/>
     </row>
     <row r="524">
-      <c s="6" r="A524"/>
+      <c s="7" r="A524"/>
     </row>
     <row r="525">
-      <c s="6" r="A525"/>
+      <c s="7" r="A525"/>
     </row>
     <row r="526">
-      <c s="6" r="A526"/>
+      <c s="7" r="A526"/>
     </row>
     <row r="527">
-      <c s="6" r="A527"/>
+      <c s="7" r="A527"/>
     </row>
     <row r="528">
-      <c s="6" r="A528"/>
+      <c s="7" r="A528"/>
     </row>
     <row r="529">
-      <c s="6" r="A529"/>
+      <c s="7" r="A529"/>
     </row>
     <row r="530">
-      <c s="6" r="A530"/>
+      <c s="7" r="A530"/>
     </row>
     <row r="531">
-      <c s="6" r="A531"/>
+      <c s="7" r="A531"/>
     </row>
     <row r="532">
-      <c s="6" r="A532"/>
+      <c s="7" r="A532"/>
     </row>
     <row r="533">
-      <c s="6" r="A533"/>
+      <c s="7" r="A533"/>
     </row>
     <row r="534">
-      <c s="6" r="A534"/>
+      <c s="7" r="A534"/>
     </row>
     <row r="535">
-      <c s="6" r="A535"/>
+      <c s="7" r="A535"/>
     </row>
     <row r="536">
-      <c s="6" r="A536"/>
+      <c s="7" r="A536"/>
     </row>
     <row r="537">
-      <c s="6" r="A537"/>
+      <c s="7" r="A537"/>
     </row>
     <row r="538">
-      <c s="6" r="A538"/>
+      <c s="7" r="A538"/>
     </row>
     <row r="539">
-      <c s="6" r="A539"/>
+      <c s="7" r="A539"/>
     </row>
     <row r="540">
-      <c s="6" r="A540"/>
+      <c s="7" r="A540"/>
     </row>
     <row r="541">
-      <c s="6" r="A541"/>
+      <c s="7" r="A541"/>
     </row>
     <row r="542">
-      <c s="6" r="A542"/>
+      <c s="7" r="A542"/>
     </row>
     <row r="543">
-      <c s="6" r="A543"/>
+      <c s="7" r="A543"/>
     </row>
     <row r="544">
-      <c s="6" r="A544"/>
+      <c s="7" r="A544"/>
     </row>
     <row r="545">
-      <c s="6" r="A545"/>
+      <c s="7" r="A545"/>
     </row>
     <row r="546">
-      <c s="6" r="A546"/>
+      <c s="7" r="A546"/>
     </row>
     <row r="547">
-      <c s="6" r="A547"/>
+      <c s="7" r="A547"/>
     </row>
     <row r="548">
-      <c s="6" r="A548"/>
+      <c s="7" r="A548"/>
     </row>
     <row r="549">
-      <c s="6" r="A549"/>
+      <c s="7" r="A549"/>
     </row>
     <row r="550">
-      <c s="6" r="A550"/>
+      <c s="7" r="A550"/>
     </row>
     <row r="551">
-      <c s="6" r="A551"/>
+      <c s="7" r="A551"/>
     </row>
     <row r="552">
-      <c s="6" r="A552"/>
+      <c s="7" r="A552"/>
     </row>
     <row r="553">
-      <c s="6" r="A553"/>
+      <c s="7" r="A553"/>
     </row>
     <row r="554">
-      <c s="6" r="A554"/>
+      <c s="7" r="A554"/>
     </row>
     <row r="555">
-      <c s="6" r="A555"/>
+      <c s="7" r="A555"/>
     </row>
     <row r="556">
-      <c s="6" r="A556"/>
+      <c s="7" r="A556"/>
     </row>
     <row r="557">
-      <c s="6" r="A557"/>
+      <c s="7" r="A557"/>
     </row>
     <row r="558">
-      <c s="6" r="A558"/>
+      <c s="7" r="A558"/>
     </row>
     <row r="559">
-      <c s="6" r="A559"/>
+      <c s="7" r="A559"/>
     </row>
     <row r="560">
-      <c s="6" r="A560"/>
+      <c s="7" r="A560"/>
     </row>
     <row r="561">
-      <c s="6" r="A561"/>
+      <c s="7" r="A561"/>
     </row>
     <row r="562">
-      <c s="6" r="A562"/>
+      <c s="7" r="A562"/>
     </row>
     <row r="563">
-      <c s="6" r="A563"/>
+      <c s="7" r="A563"/>
     </row>
     <row r="564">
-      <c s="6" r="A564"/>
+      <c s="7" r="A564"/>
     </row>
     <row r="565">
-      <c s="6" r="A565"/>
+      <c s="7" r="A565"/>
     </row>
     <row r="566">
-      <c s="6" r="A566"/>
+      <c s="7" r="A566"/>
     </row>
     <row r="567">
-      <c s="6" r="A567"/>
+      <c s="7" r="A567"/>
     </row>
     <row r="568">
-      <c s="6" r="A568"/>
+      <c s="7" r="A568"/>
     </row>
     <row r="569">
-      <c s="6" r="A569"/>
+      <c s="7" r="A569"/>
     </row>
     <row r="570">
-      <c s="6" r="A570"/>
+      <c s="7" r="A570"/>
     </row>
     <row r="571">
-      <c s="6" r="A571"/>
+      <c s="7" r="A571"/>
     </row>
     <row r="572">
-      <c s="6" r="A572"/>
+      <c s="7" r="A572"/>
     </row>
     <row r="573">
-      <c s="6" r="A573"/>
+      <c s="7" r="A573"/>
     </row>
     <row r="574">
-      <c s="6" r="A574"/>
+      <c s="7" r="A574"/>
     </row>
     <row r="575">
-      <c s="6" r="A575"/>
+      <c s="7" r="A575"/>
     </row>
     <row r="576">
-      <c s="6" r="A576"/>
+      <c s="7" r="A576"/>
     </row>
     <row r="577">
-      <c s="6" r="A577"/>
+      <c s="7" r="A577"/>
     </row>
     <row r="578">
-      <c s="6" r="A578"/>
+      <c s="7" r="A578"/>
     </row>
     <row r="579">
-      <c s="6" r="A579"/>
+      <c s="7" r="A579"/>
     </row>
     <row r="580">
-      <c s="6" r="A580"/>
+      <c s="7" r="A580"/>
     </row>
     <row r="581">
-      <c s="6" r="A581"/>
+      <c s="7" r="A581"/>
     </row>
     <row r="582">
-      <c s="6" r="A582"/>
+      <c s="7" r="A582"/>
     </row>
     <row r="583">
-      <c s="6" r="A583"/>
+      <c s="7" r="A583"/>
     </row>
     <row r="584">
-      <c s="6" r="A584"/>
+      <c s="7" r="A584"/>
     </row>
     <row r="585">
-      <c s="6" r="A585"/>
+      <c s="7" r="A585"/>
     </row>
     <row r="586">
-      <c s="6" r="A586"/>
+      <c s="7" r="A586"/>
     </row>
     <row r="587">
-      <c s="6" r="A587"/>
+      <c s="7" r="A587"/>
     </row>
     <row r="588">
-      <c s="6" r="A588"/>
+      <c s="7" r="A588"/>
     </row>
     <row r="589">
-      <c s="6" r="A589"/>
+      <c s="7" r="A589"/>
     </row>
     <row r="590">
-      <c s="6" r="A590"/>
+      <c s="7" r="A590"/>
     </row>
     <row r="591">
-      <c s="6" r="A591"/>
+      <c s="7" r="A591"/>
     </row>
     <row r="592">
-      <c s="6" r="A592"/>
+      <c s="7" r="A592"/>
     </row>
     <row r="593">
-      <c s="6" r="A593"/>
+      <c s="7" r="A593"/>
     </row>
     <row r="594">
-      <c s="6" r="A594"/>
+      <c s="7" r="A594"/>
     </row>
     <row r="595">
-      <c s="6" r="A595"/>
+      <c s="7" r="A595"/>
     </row>
     <row r="596">
-      <c s="6" r="A596"/>
+      <c s="7" r="A596"/>
     </row>
     <row r="597">
-      <c s="6" r="A597"/>
+      <c s="7" r="A597"/>
     </row>
     <row r="598">
-      <c s="6" r="A598"/>
+      <c s="7" r="A598"/>
     </row>
     <row r="599">
-      <c s="6" r="A599"/>
+      <c s="7" r="A599"/>
     </row>
     <row r="600">
-      <c s="6" r="A600"/>
+      <c s="7" r="A600"/>
     </row>
     <row r="601">
-      <c s="6" r="A601"/>
+      <c s="7" r="A601"/>
     </row>
     <row r="602">
-      <c s="6" r="A602"/>
+      <c s="7" r="A602"/>
     </row>
     <row r="603">
-      <c s="6" r="A603"/>
+      <c s="7" r="A603"/>
     </row>
     <row r="604">
-      <c s="6" r="A604"/>
+      <c s="7" r="A604"/>
     </row>
     <row r="605">
-      <c s="6" r="A605"/>
+      <c s="7" r="A605"/>
     </row>
     <row r="606">
-      <c s="6" r="A606"/>
+      <c s="7" r="A606"/>
     </row>
     <row r="607">
-      <c s="6" r="A607"/>
+      <c s="7" r="A607"/>
     </row>
     <row r="608">
-      <c s="6" r="A608"/>
+      <c s="7" r="A608"/>
     </row>
     <row r="609">
-      <c s="6" r="A609"/>
+      <c s="7" r="A609"/>
     </row>
     <row r="610">
-      <c s="6" r="A610"/>
+      <c s="7" r="A610"/>
     </row>
     <row r="611">
-      <c s="6" r="A611"/>
+      <c s="7" r="A611"/>
     </row>
     <row r="612">
-      <c s="6" r="A612"/>
+      <c s="7" r="A612"/>
     </row>
     <row r="613">
-      <c s="6" r="A613"/>
+      <c s="7" r="A613"/>
     </row>
     <row r="614">
-      <c s="6" r="A614"/>
+      <c s="7" r="A614"/>
     </row>
     <row r="615">
-      <c s="6" r="A615"/>
+      <c s="7" r="A615"/>
     </row>
     <row r="616">
-      <c s="6" r="A616"/>
+      <c s="7" r="A616"/>
     </row>
     <row r="617">
-      <c s="6" r="A617"/>
+      <c s="7" r="A617"/>
     </row>
     <row r="618">
-      <c s="6" r="A618"/>
+      <c s="7" r="A618"/>
     </row>
     <row r="619">
-      <c s="6" r="A619"/>
+      <c s="7" r="A619"/>
     </row>
     <row r="620">
-      <c s="6" r="A620"/>
+      <c s="7" r="A620"/>
     </row>
     <row r="621">
-      <c s="6" r="A621"/>
+      <c s="7" r="A621"/>
     </row>
     <row r="622">
-      <c s="6" r="A622"/>
+      <c s="7" r="A622"/>
     </row>
     <row r="623">
-      <c s="6" r="A623"/>
+      <c s="7" r="A623"/>
     </row>
     <row r="624">
-      <c s="6" r="A624"/>
+      <c s="7" r="A624"/>
     </row>
     <row r="625">
-      <c s="6" r="A625"/>
+      <c s="7" r="A625"/>
     </row>
     <row r="626">
-      <c s="6" r="A626"/>
+      <c s="7" r="A626"/>
     </row>
     <row r="627">
-      <c s="6" r="A627"/>
+      <c s="7" r="A627"/>
     </row>
     <row r="628">
-      <c s="6" r="A628"/>
+      <c s="7" r="A628"/>
     </row>
     <row r="629">
-      <c s="6" r="A629"/>
+      <c s="7" r="A629"/>
     </row>
     <row r="630">
-      <c s="6" r="A630"/>
+      <c s="7" r="A630"/>
     </row>
     <row r="631">
-      <c s="6" r="A631"/>
+      <c s="7" r="A631"/>
     </row>
     <row r="632">
-      <c s="6" r="A632"/>
+      <c s="7" r="A632"/>
     </row>
     <row r="633">
-      <c s="6" r="A633"/>
+      <c s="7" r="A633"/>
     </row>
     <row r="634">
-      <c s="6" r="A634"/>
+      <c s="7" r="A634"/>
     </row>
     <row r="635">
-      <c s="6" r="A635"/>
+      <c s="7" r="A635"/>
     </row>
     <row r="636">
-      <c s="6" r="A636"/>
+      <c s="7" r="A636"/>
     </row>
     <row r="637">
-      <c s="6" r="A637"/>
+      <c s="7" r="A637"/>
     </row>
     <row r="638">
-      <c s="6" r="A638"/>
+      <c s="7" r="A638"/>
     </row>
     <row r="639">
-      <c s="6" r="A639"/>
+      <c s="7" r="A639"/>
     </row>
     <row r="640">
-      <c s="6" r="A640"/>
+      <c s="7" r="A640"/>
     </row>
     <row r="641">
-      <c s="6" r="A641"/>
+      <c s="7" r="A641"/>
     </row>
     <row r="642">
-      <c s="6" r="A642"/>
+      <c s="7" r="A642"/>
     </row>
     <row r="643">
-      <c s="6" r="A643"/>
+      <c s="7" r="A643"/>
     </row>
     <row r="644">
-      <c s="6" r="A644"/>
+      <c s="7" r="A644"/>
     </row>
     <row r="645">
-      <c s="6" r="A645"/>
+      <c s="7" r="A645"/>
     </row>
     <row r="646">
-      <c s="6" r="A646"/>
+      <c s="7" r="A646"/>
     </row>
     <row r="647">
-      <c s="6" r="A647"/>
+      <c s="7" r="A647"/>
     </row>
     <row r="648">
-      <c s="6" r="A648"/>
+      <c s="7" r="A648"/>
     </row>
     <row r="649">
-      <c s="6" r="A649"/>
+      <c s="7" r="A649"/>
     </row>
     <row r="650">
-      <c s="6" r="A650"/>
+      <c s="7" r="A650"/>
     </row>
     <row r="651">
-      <c s="6" r="A651"/>
+      <c s="7" r="A651"/>
     </row>
     <row r="652">
-      <c s="6" r="A652"/>
+      <c s="7" r="A652"/>
     </row>
     <row r="653">
-      <c s="6" r="A653"/>
+      <c s="7" r="A653"/>
     </row>
     <row r="654">
-      <c s="6" r="A654"/>
+      <c s="7" r="A654"/>
     </row>
     <row r="655">
-      <c s="6" r="A655"/>
+      <c s="7" r="A655"/>
     </row>
     <row r="656">
-      <c s="6" r="A656"/>
+      <c s="7" r="A656"/>
     </row>
     <row r="657">
-      <c s="6" r="A657"/>
+      <c s="7" r="A657"/>
     </row>
     <row r="658">
-      <c s="6" r="A658"/>
+      <c s="7" r="A658"/>
     </row>
     <row r="659">
-      <c s="6" r="A659"/>
+      <c s="7" r="A659"/>
     </row>
     <row r="660">
-      <c s="6" r="A660"/>
+      <c s="7" r="A660"/>
     </row>
     <row r="661">
-      <c s="6" r="A661"/>
+      <c s="7" r="A661"/>
     </row>
     <row r="662">
-      <c s="6" r="A662"/>
+      <c s="7" r="A662"/>
     </row>
     <row r="663">
-      <c s="6" r="A663"/>
+      <c s="7" r="A663"/>
     </row>
     <row r="664">
-      <c s="6" r="A664"/>
+      <c s="7" r="A664"/>
     </row>
     <row r="665">
-      <c s="6" r="A665"/>
+      <c s="7" r="A665"/>
     </row>
     <row r="666">
-      <c s="6" r="A666"/>
+      <c s="7" r="A666"/>
     </row>
     <row r="667">
-      <c s="6" r="A667"/>
+      <c s="7" r="A667"/>
     </row>
     <row r="668">
-      <c s="6" r="A668"/>
+      <c s="7" r="A668"/>
     </row>
     <row r="669">
-      <c s="6" r="A669"/>
+      <c s="7" r="A669"/>
     </row>
     <row r="670">
-      <c s="6" r="A670"/>
+      <c s="7" r="A670"/>
     </row>
     <row r="671">
-      <c s="6" r="A671"/>
+      <c s="7" r="A671"/>
     </row>
     <row r="672">
-      <c s="6" r="A672"/>
+      <c s="7" r="A672"/>
     </row>
     <row r="673">
-      <c s="6" r="A673"/>
+      <c s="7" r="A673"/>
     </row>
     <row r="674">
-      <c s="6" r="A674"/>
+      <c s="7" r="A674"/>
     </row>
     <row r="675">
-      <c s="6" r="A675"/>
+      <c s="7" r="A675"/>
     </row>
     <row r="676">
-      <c s="6" r="A676"/>
+      <c s="7" r="A676"/>
     </row>
     <row r="677">
-      <c s="6" r="A677"/>
+      <c s="7" r="A677"/>
     </row>
     <row r="678">
-      <c s="6" r="A678"/>
+      <c s="7" r="A678"/>
     </row>
     <row r="679">
-      <c s="6" r="A679"/>
+      <c s="7" r="A679"/>
     </row>
     <row r="680">
-      <c s="6" r="A680"/>
+      <c s="7" r="A680"/>
     </row>
     <row r="681">
-      <c s="6" r="A681"/>
+      <c s="7" r="A681"/>
     </row>
     <row r="682">
-      <c s="6" r="A682"/>
+      <c s="7" r="A682"/>
     </row>
     <row r="683">
-      <c s="6" r="A683"/>
+      <c s="7" r="A683"/>
     </row>
     <row r="684">
-      <c s="6" r="A684"/>
+      <c s="7" r="A684"/>
     </row>
     <row r="685">
-      <c s="6" r="A685"/>
+      <c s="7" r="A685"/>
     </row>
     <row r="686">
-      <c s="6" r="A686"/>
+      <c s="7" r="A686"/>
     </row>
     <row r="687">
-      <c s="6" r="A687"/>
+      <c s="7" r="A687"/>
     </row>
     <row r="688">
-      <c s="6" r="A688"/>
+      <c s="7" r="A688"/>
     </row>
     <row r="689">
-      <c s="6" r="A689"/>
+      <c s="7" r="A689"/>
     </row>
     <row r="690">
-      <c s="6" r="A690"/>
+      <c s="7" r="A690"/>
     </row>
     <row r="691">
-      <c s="6" r="A691"/>
+      <c s="7" r="A691"/>
     </row>
     <row r="692">
-      <c s="6" r="A692"/>
+      <c s="7" r="A692"/>
     </row>
     <row r="693">
-      <c s="6" r="A693"/>
+      <c s="7" r="A693"/>
     </row>
     <row r="694">
-      <c s="6" r="A694"/>
+      <c s="7" r="A694"/>
     </row>
     <row r="695">
-      <c s="6" r="A695"/>
+      <c s="7" r="A695"/>
     </row>
     <row r="696">
-      <c s="6" r="A696"/>
+      <c s="7" r="A696"/>
     </row>
     <row r="697">
-      <c s="6" r="A697"/>
+      <c s="7" r="A697"/>
     </row>
     <row r="698">
-      <c s="6" r="A698"/>
+      <c s="7" r="A698"/>
     </row>
     <row r="699">
-      <c s="6" r="A699"/>
+      <c s="7" r="A699"/>
     </row>
     <row r="700">
-      <c s="6" r="A700"/>
+      <c s="7" r="A700"/>
     </row>
     <row r="701">
-      <c s="6" r="A701"/>
+      <c s="7" r="A701"/>
     </row>
     <row r="702">
-      <c s="6" r="A702"/>
+      <c s="7" r="A702"/>
     </row>
     <row r="703">
-      <c s="6" r="A703"/>
+      <c s="7" r="A703"/>
     </row>
     <row r="704">
-      <c s="6" r="A704"/>
+      <c s="7" r="A704"/>
     </row>
     <row r="705">
-      <c s="6" r="A705"/>
+      <c s="7" r="A705"/>
     </row>
     <row r="706">
-      <c s="6" r="A706"/>
+      <c s="7" r="A706"/>
     </row>
     <row r="707">
-      <c s="6" r="A707"/>
+      <c s="7" r="A707"/>
     </row>
     <row r="708">
-      <c s="6" r="A708"/>
+      <c s="7" r="A708"/>
     </row>
     <row r="709">
-      <c s="6" r="A709"/>
+      <c s="7" r="A709"/>
     </row>
     <row r="710">
-      <c s="6" r="A710"/>
+      <c s="7" r="A710"/>
     </row>
     <row r="711">
-      <c s="6" r="A711"/>
+      <c s="7" r="A711"/>
     </row>
     <row r="712">
-      <c s="6" r="A712"/>
+      <c s="7" r="A712"/>
     </row>
     <row r="713">
-      <c s="6" r="A713"/>
+      <c s="7" r="A713"/>
     </row>
     <row r="714">
-      <c s="6" r="A714"/>
+      <c s="7" r="A714"/>
     </row>
     <row r="715">
-      <c s="6" r="A715"/>
+      <c s="7" r="A715"/>
     </row>
     <row r="716">
-      <c s="6" r="A716"/>
+      <c s="7" r="A716"/>
     </row>
     <row r="717">
-      <c s="6" r="A717"/>
+      <c s="7" r="A717"/>
     </row>
     <row r="718">
-      <c s="6" r="A718"/>
+      <c s="7" r="A718"/>
     </row>
     <row r="719">
-      <c s="6" r="A719"/>
+      <c s="7" r="A719"/>
     </row>
     <row r="720">
-      <c s="6" r="A720"/>
+      <c s="7" r="A720"/>
     </row>
     <row r="721">
-      <c s="6" r="A721"/>
+      <c s="7" r="A721"/>
     </row>
     <row r="722">
-      <c s="6" r="A722"/>
+      <c s="7" r="A722"/>
     </row>
     <row r="723">
-      <c s="6" r="A723"/>
+      <c s="7" r="A723"/>
     </row>
     <row r="724">
-      <c s="6" r="A724"/>
+      <c s="7" r="A724"/>
     </row>
     <row r="725">
-      <c s="6" r="A725"/>
+      <c s="7" r="A725"/>
     </row>
     <row r="726">
-      <c s="6" r="A726"/>
+      <c s="7" r="A726"/>
     </row>
     <row r="727">
-      <c s="6" r="A727"/>
+      <c s="7" r="A727"/>
     </row>
     <row r="728">
-      <c s="6" r="A728"/>
+      <c s="7" r="A728"/>
     </row>
     <row r="729">
-      <c s="6" r="A729"/>
+      <c s="7" r="A729"/>
     </row>
     <row r="730">
-      <c s="6" r="A730"/>
+      <c s="7" r="A730"/>
     </row>
     <row r="731">
-      <c s="6" r="A731"/>
+      <c s="7" r="A731"/>
     </row>
     <row r="732">
-      <c s="6" r="A732"/>
+      <c s="7" r="A732"/>
     </row>
     <row r="733">
-      <c s="6" r="A733"/>
+      <c s="7" r="A733"/>
     </row>
     <row r="734">
-      <c s="6" r="A734"/>
+      <c s="7" r="A734"/>
     </row>
     <row r="735">
-      <c s="6" r="A735"/>
+      <c s="7" r="A735"/>
     </row>
     <row r="736">
-      <c s="6" r="A736"/>
+      <c s="7" r="A736"/>
     </row>
     <row r="737">
-      <c s="6" r="A737"/>
+      <c s="7" r="A737"/>
     </row>
     <row r="738">
-      <c s="6" r="A738"/>
+      <c s="7" r="A738"/>
     </row>
     <row r="739">
-      <c s="6" r="A739"/>
+      <c s="7" r="A739"/>
     </row>
     <row r="740">
-      <c s="6" r="A740"/>
+      <c s="7" r="A740"/>
     </row>
     <row r="741">
-      <c s="6" r="A741"/>
+      <c s="7" r="A741"/>
     </row>
     <row r="742">
-      <c s="6" r="A742"/>
+      <c s="7" r="A742"/>
     </row>
     <row r="743">
-      <c s="6" r="A743"/>
+      <c s="7" r="A743"/>
     </row>
     <row r="744">
-      <c s="6" r="A744"/>
+      <c s="7" r="A744"/>
     </row>
     <row r="745">
-      <c s="6" r="A745"/>
+      <c s="7" r="A745"/>
     </row>
     <row r="746">
-      <c s="6" r="A746"/>
+      <c s="7" r="A746"/>
     </row>
     <row r="747">
-      <c s="6" r="A747"/>
+      <c s="7" r="A747"/>
     </row>
     <row r="748">
-      <c s="6" r="A748"/>
+      <c s="7" r="A748"/>
     </row>
     <row r="749">
-      <c s="6" r="A749"/>
+      <c s="7" r="A749"/>
     </row>
     <row r="750">
-      <c s="6" r="A750"/>
+      <c s="7" r="A750"/>
     </row>
     <row r="751">
-      <c s="6" r="A751"/>
+      <c s="7" r="A751"/>
     </row>
     <row r="752">
-      <c s="6" r="A752"/>
+      <c s="7" r="A752"/>
     </row>
     <row r="753">
-      <c s="6" r="A753"/>
+      <c s="7" r="A753"/>
     </row>
     <row r="754">
-      <c s="6" r="A754"/>
+      <c s="7" r="A754"/>
     </row>
     <row r="755">
-      <c s="6" r="A755"/>
+      <c s="7" r="A755"/>
     </row>
     <row r="756">
-      <c s="6" r="A756"/>
+      <c s="7" r="A756"/>
     </row>
     <row r="757">
-      <c s="6" r="A757"/>
+      <c s="7" r="A757"/>
     </row>
     <row r="758">
-      <c s="6" r="A758"/>
+      <c s="7" r="A758"/>
     </row>
     <row r="759">
-      <c s="6" r="A759"/>
+      <c s="7" r="A759"/>
     </row>
     <row r="760">
-      <c s="6" r="A760"/>
+      <c s="7" r="A760"/>
     </row>
     <row r="761">
-      <c s="6" r="A761"/>
+      <c s="7" r="A761"/>
     </row>
     <row r="762">
-      <c s="6" r="A762"/>
+      <c s="7" r="A762"/>
     </row>
     <row r="763">
-      <c s="6" r="A763"/>
+      <c s="7" r="A763"/>
     </row>
     <row r="764">
-      <c s="6" r="A764"/>
+      <c s="7" r="A764"/>
     </row>
     <row r="765">
-      <c s="6" r="A765"/>
+      <c s="7" r="A765"/>
     </row>
     <row r="766">
-      <c s="6" r="A766"/>
+      <c s="7" r="A766"/>
     </row>
     <row r="767">
-      <c s="6" r="A767"/>
+      <c s="7" r="A767"/>
     </row>
     <row r="768">
-      <c s="6" r="A768"/>
+      <c s="7" r="A768"/>
     </row>
     <row r="769">
-      <c s="6" r="A769"/>
+      <c s="7" r="A769"/>
     </row>
     <row r="770">
-      <c s="6" r="A770"/>
+      <c s="7" r="A770"/>
     </row>
     <row r="771">
-      <c s="6" r="A771"/>
+      <c s="7" r="A771"/>
     </row>
     <row r="772">
-      <c s="6" r="A772"/>
+      <c s="7" r="A772"/>
     </row>
     <row r="773">
-      <c s="6" r="A773"/>
+      <c s="7" r="A773"/>
     </row>
     <row r="774">
-      <c s="6" r="A774"/>
+      <c s="7" r="A774"/>
     </row>
     <row r="775">
-      <c s="6" r="A775"/>
+      <c s="7" r="A775"/>
     </row>
     <row r="776">
-      <c s="6" r="A776"/>
+      <c s="7" r="A776"/>
     </row>
     <row r="777">
-      <c s="6" r="A777"/>
+      <c s="7" r="A777"/>
     </row>
     <row r="778">
-      <c s="6" r="A778"/>
+      <c s="7" r="A778"/>
     </row>
     <row r="779">
-      <c s="6" r="A779"/>
+      <c s="7" r="A779"/>
     </row>
     <row r="780">
-      <c s="6" r="A780"/>
+      <c s="7" r="A780"/>
     </row>
     <row r="781">
-      <c s="6" r="A781"/>
+      <c s="7" r="A781"/>
     </row>
     <row r="782">
-      <c s="6" r="A782"/>
+      <c s="7" r="A782"/>
     </row>
     <row r="783">
-      <c s="6" r="A783"/>
+      <c s="7" r="A783"/>
     </row>
     <row r="784">
-      <c s="6" r="A784"/>
+      <c s="7" r="A784"/>
     </row>
     <row r="785">
-      <c s="6" r="A785"/>
+      <c s="7" r="A785"/>
     </row>
     <row r="786">
-      <c s="6" r="A786"/>
+      <c s="7" r="A786"/>
     </row>
     <row r="787">
-      <c s="6" r="A787"/>
+      <c s="7" r="A787"/>
     </row>
     <row r="788">
-      <c s="6" r="A788"/>
+      <c s="7" r="A788"/>
     </row>
     <row r="789">
-      <c s="6" r="A789"/>
+      <c s="7" r="A789"/>
     </row>
     <row r="790">
-      <c s="6" r="A790"/>
+      <c s="7" r="A790"/>
     </row>
     <row r="791">
-      <c s="6" r="A791"/>
+      <c s="7" r="A791"/>
     </row>
     <row r="792">
-      <c s="6" r="A792"/>
+      <c s="7" r="A792"/>
     </row>
     <row r="793">
-      <c s="6" r="A793"/>
+      <c s="7" r="A793"/>
     </row>
     <row r="794">
-      <c s="6" r="A794"/>
+      <c s="7" r="A794"/>
     </row>
     <row r="795">
-      <c s="6" r="A795"/>
+      <c s="7" r="A795"/>
     </row>
     <row r="796">
-      <c s="6" r="A796"/>
+      <c s="7" r="A796"/>
     </row>
     <row r="797">
-      <c s="6" r="A797"/>
+      <c s="7" r="A797"/>
     </row>
     <row r="798">
-      <c s="6" r="A798"/>
+      <c s="7" r="A798"/>
     </row>
     <row r="799">
-      <c s="6" r="A799"/>
+      <c s="7" r="A799"/>
     </row>
     <row r="800">
-      <c s="6" r="A800"/>
+      <c s="7" r="A800"/>
     </row>
     <row r="801">
-      <c s="6" r="A801"/>
+      <c s="7" r="A801"/>
     </row>
     <row r="802">
-      <c s="6" r="A802"/>
+      <c s="7" r="A802"/>
     </row>
     <row r="803">
-      <c s="6" r="A803"/>
+      <c s="7" r="A803"/>
     </row>
     <row r="804">
-      <c s="6" r="A804"/>
+      <c s="7" r="A804"/>
     </row>
     <row r="805">
-      <c s="6" r="A805"/>
+      <c s="7" r="A805"/>
     </row>
     <row r="806">
-      <c s="6" r="A806"/>
+      <c s="7" r="A806"/>
     </row>
     <row r="807">
-      <c s="6" r="A807"/>
+      <c s="7" r="A807"/>
     </row>
     <row r="808">
-      <c s="6" r="A808"/>
+      <c s="7" r="A808"/>
     </row>
     <row r="809">
-      <c s="6" r="A809"/>
+      <c s="7" r="A809"/>
     </row>
     <row r="810">
-      <c s="6" r="A810"/>
+      <c s="7" r="A810"/>
     </row>
     <row r="811">
-      <c s="6" r="A811"/>
+      <c s="7" r="A811"/>
     </row>
     <row r="812">
-      <c s="6" r="A812"/>
+      <c s="7" r="A812"/>
     </row>
     <row r="813">
-      <c s="6" r="A813"/>
+      <c s="7" r="A813"/>
     </row>
     <row r="814">
-      <c s="6" r="A814"/>
+      <c s="7" r="A814"/>
     </row>
     <row r="815">
-      <c s="6" r="A815"/>
+      <c s="7" r="A815"/>
     </row>
     <row r="816">
-      <c s="6" r="A816"/>
+      <c s="7" r="A816"/>
     </row>
     <row r="817">
-      <c s="6" r="A817"/>
+      <c s="7" r="A817"/>
     </row>
     <row r="818">
-      <c s="6" r="A818"/>
+      <c s="7" r="A818"/>
     </row>
     <row r="819">
-      <c s="6" r="A819"/>
+      <c s="7" r="A819"/>
     </row>
     <row r="820">
-      <c s="6" r="A820"/>
+      <c s="7" r="A820"/>
     </row>
     <row r="821">
-      <c s="6" r="A821"/>
+      <c s="7" r="A821"/>
     </row>
     <row r="822">
-      <c s="6" r="A822"/>
+      <c s="7" r="A822"/>
     </row>
     <row r="823">
-      <c s="6" r="A823"/>
+      <c s="7" r="A823"/>
     </row>
     <row r="824">
-      <c s="6" r="A824"/>
+      <c s="7" r="A824"/>
     </row>
     <row r="825">
-      <c s="6" r="A825"/>
+      <c s="7" r="A825"/>
     </row>
     <row r="826">
-      <c s="6" r="A826"/>
+      <c s="7" r="A826"/>
     </row>
     <row r="827">
-      <c s="6" r="A827"/>
+      <c s="7" r="A827"/>
     </row>
     <row r="828">
-      <c s="6" r="A828"/>
+      <c s="7" r="A828"/>
     </row>
     <row r="829">
-      <c s="6" r="A829"/>
+      <c s="7" r="A829"/>
     </row>
     <row r="830">
-      <c s="6" r="A830"/>
+      <c s="7" r="A830"/>
     </row>
     <row r="831">
-      <c s="6" r="A831"/>
+      <c s="7" r="A831"/>
     </row>
     <row r="832">
-      <c s="6" r="A832"/>
+      <c s="7" r="A832"/>
     </row>
     <row r="833">
-      <c s="6" r="A833"/>
+      <c s="7" r="A833"/>
     </row>
     <row r="834">
-      <c s="6" r="A834"/>
+      <c s="7" r="A834"/>
     </row>
     <row r="835">
-      <c s="6" r="A835"/>
+      <c s="7" r="A835"/>
     </row>
     <row r="836">
-      <c s="6" r="A836"/>
+      <c s="7" r="A836"/>
     </row>
     <row r="837">
-      <c s="6" r="A837"/>
+      <c s="7" r="A837"/>
     </row>
     <row r="838">
-      <c s="6" r="A838"/>
+      <c s="7" r="A838"/>
     </row>
     <row r="839">
-      <c s="6" r="A839"/>
+      <c s="7" r="A839"/>
     </row>
     <row r="840">
-      <c s="6" r="A840"/>
+      <c s="7" r="A840"/>
     </row>
     <row r="841">
-      <c s="6" r="A841"/>
+      <c s="7" r="A841"/>
     </row>
     <row r="842">
-      <c s="6" r="A842"/>
+      <c s="7" r="A842"/>
     </row>
     <row r="843">
-      <c s="6" r="A843"/>
+      <c s="7" r="A843"/>
     </row>
     <row r="844">
-      <c s="6" r="A844"/>
+      <c s="7" r="A844"/>
     </row>
     <row r="845">
-      <c s="6" r="A845"/>
+      <c s="7" r="A845"/>
     </row>
     <row r="846">
-      <c s="6" r="A846"/>
+      <c s="7" r="A846"/>
     </row>
     <row r="847">
-      <c s="6" r="A847"/>
+      <c s="7" r="A847"/>
     </row>
     <row r="848">
-      <c s="6" r="A848"/>
+      <c s="7" r="A848"/>
     </row>
     <row r="849">
-      <c s="6" r="A849"/>
+      <c s="7" r="A849"/>
     </row>
     <row r="850">
-      <c s="6" r="A850"/>
+      <c s="7" r="A850"/>
     </row>
     <row r="851">
-      <c s="6" r="A851"/>
+      <c s="7" r="A851"/>
     </row>
     <row r="852">
-      <c s="6" r="A852"/>
+      <c s="7" r="A852"/>
     </row>
     <row r="853">
-      <c s="6" r="A853"/>
+      <c s="7" r="A853"/>
     </row>
     <row r="854">
-      <c s="6" r="A854"/>
+      <c s="7" r="A854"/>
     </row>
     <row r="855">
-      <c s="6" r="A855"/>
+      <c s="7" r="A855"/>
     </row>
     <row r="856">
-      <c s="6" r="A856"/>
+      <c s="7" r="A856"/>
     </row>
     <row r="857">
-      <c s="6" r="A857"/>
+      <c s="7" r="A857"/>
     </row>
     <row r="858">
-      <c s="6" r="A858"/>
+      <c s="7" r="A858"/>
     </row>
     <row r="859">
-      <c s="6" r="A859"/>
+      <c s="7" r="A859"/>
     </row>
     <row r="860">
-      <c s="6" r="A860"/>
+      <c s="7" r="A860"/>
     </row>
     <row r="861">
-      <c s="6" r="A861"/>
+      <c s="7" r="A861"/>
     </row>
     <row r="862">
-      <c s="6" r="A862"/>
+      <c s="7" r="A862"/>
     </row>
     <row r="863">
-      <c s="6" r="A863"/>
+      <c s="7" r="A863"/>
     </row>
     <row r="864">
-      <c s="6" r="A864"/>
+      <c s="7" r="A864"/>
     </row>
     <row r="865">
-      <c s="6" r="A865"/>
+      <c s="7" r="A865"/>
     </row>
     <row r="866">
-      <c s="6" r="A866"/>
+      <c s="7" r="A866"/>
     </row>
     <row r="867">
-      <c s="6" r="A867"/>
+      <c s="7" r="A867"/>
     </row>
     <row r="868">
-      <c s="6" r="A868"/>
+      <c s="7" r="A868"/>
     </row>
     <row r="869">
-      <c s="6" r="A869"/>
+      <c s="7" r="A869"/>
     </row>
     <row r="870">
-      <c s="6" r="A870"/>
+      <c s="7" r="A870"/>
     </row>
     <row r="871">
-      <c s="6" r="A871"/>
+      <c s="7" r="A871"/>
     </row>
     <row r="872">
-      <c s="6" r="A872"/>
+      <c s="7" r="A872"/>
     </row>
     <row r="873">
-      <c s="6" r="A873"/>
+      <c s="7" r="A873"/>
     </row>
     <row r="874">
-      <c s="6" r="A874"/>
+      <c s="7" r="A874"/>
     </row>
     <row r="875">
-      <c s="6" r="A875"/>
+      <c s="7" r="A875"/>
     </row>
     <row r="876">
-      <c s="6" r="A876"/>
+      <c s="7" r="A876"/>
     </row>
     <row r="877">
-      <c s="6" r="A877"/>
+      <c s="7" r="A877"/>
     </row>
     <row r="878">
-      <c s="6" r="A878"/>
+      <c s="7" r="A878"/>
     </row>
     <row r="879">
-      <c s="6" r="A879"/>
+      <c s="7" r="A879"/>
     </row>
     <row r="880">
-      <c s="6" r="A880"/>
+      <c s="7" r="A880"/>
     </row>
     <row r="881">
-      <c s="6" r="A881"/>
+      <c s="7" r="A881"/>
     </row>
     <row r="882">
-      <c s="6" r="A882"/>
+      <c s="7" r="A882"/>
     </row>
     <row r="883">
-      <c s="6" r="A883"/>
+      <c s="7" r="A883"/>
     </row>
     <row r="884">
-      <c s="6" r="A884"/>
+      <c s="7" r="A884"/>
     </row>
     <row r="885">
-      <c s="6" r="A885"/>
+      <c s="7" r="A885"/>
     </row>
     <row r="886">
-      <c s="6" r="A886"/>
+      <c s="7" r="A886"/>
     </row>
     <row r="887">
-      <c s="6" r="A887"/>
+      <c s="7" r="A887"/>
     </row>
     <row r="888">
-      <c s="6" r="A888"/>
+      <c s="7" r="A888"/>
     </row>
     <row r="889">
-      <c s="6" r="A889"/>
+      <c s="7" r="A889"/>
     </row>
     <row r="890">
-      <c s="6" r="A890"/>
+      <c s="7" r="A890"/>
     </row>
     <row r="891">
-      <c s="6" r="A891"/>
+      <c s="7" r="A891"/>
     </row>
     <row r="892">
-      <c s="6" r="A892"/>
+      <c s="7" r="A892"/>
     </row>
     <row r="893">
-      <c s="6" r="A893"/>
+      <c s="7" r="A893"/>
     </row>
     <row r="894">
-      <c s="6" r="A894"/>
+      <c s="7" r="A894"/>
     </row>
     <row r="895">
-      <c s="6" r="A895"/>
+      <c s="7" r="A895"/>
     </row>
     <row r="896">
-      <c s="6" r="A896"/>
+      <c s="7" r="A896"/>
     </row>
     <row r="897">
-      <c s="6" r="A897"/>
+      <c s="7" r="A897"/>
     </row>
     <row r="898">
-      <c s="6" r="A898"/>
+      <c s="7" r="A898"/>
     </row>
     <row r="899">
-      <c s="6" r="A899"/>
+      <c s="7" r="A899"/>
     </row>
     <row r="900">
-      <c s="6" r="A900"/>
+      <c s="7" r="A900"/>
     </row>
     <row r="901">
-      <c s="6" r="A901"/>
+      <c s="7" r="A901"/>
     </row>
     <row r="902">
-      <c s="6" r="A902"/>
+      <c s="7" r="A902"/>
     </row>
     <row r="903">
-      <c s="6" r="A903"/>
+      <c s="7" r="A903"/>
     </row>
     <row r="904">
-      <c s="6" r="A904"/>
+      <c s="7" r="A904"/>
     </row>
     <row r="905">
-      <c s="6" r="A905"/>
+      <c s="7" r="A905"/>
     </row>
     <row r="906">
-      <c s="6" r="A906"/>
+      <c s="7" r="A906"/>
     </row>
     <row r="907">
-      <c s="6" r="A907"/>
+      <c s="7" r="A907"/>
     </row>
     <row r="908">
-      <c s="6" r="A908"/>
+      <c s="7" r="A908"/>
     </row>
     <row r="909">
-      <c s="6" r="A909"/>
+      <c s="7" r="A909"/>
     </row>
     <row r="910">
-      <c s="6" r="A910"/>
+      <c s="7" r="A910"/>
     </row>
     <row r="911">
-      <c s="6" r="A911"/>
+      <c s="7" r="A911"/>
     </row>
     <row r="912">
-      <c s="6" r="A912"/>
+      <c s="7" r="A912"/>
     </row>
     <row r="913">
-      <c s="6" r="A913"/>
+      <c s="7" r="A913"/>
     </row>
     <row r="914">
-      <c s="6" r="A914"/>
+      <c s="7" r="A914"/>
     </row>
     <row r="915">
-      <c s="6" r="A915"/>
+      <c s="7" r="A915"/>
     </row>
     <row r="916">
-      <c s="6" r="A916"/>
+      <c s="7" r="A916"/>
     </row>
     <row r="917">
-      <c s="6" r="A917"/>
+      <c s="7" r="A917"/>
     </row>
     <row r="918">
-      <c s="6" r="A918"/>
+      <c s="7" r="A918"/>
     </row>
     <row r="919">
-      <c s="6" r="A919"/>
+      <c s="7" r="A919"/>
     </row>
     <row r="920">
-      <c s="6" r="A920"/>
+      <c s="7" r="A920"/>
     </row>
     <row r="921">
-      <c s="6" r="A921"/>
+      <c s="7" r="A921"/>
     </row>
     <row r="922">
-      <c s="6" r="A922"/>
+      <c s="7" r="A922"/>
     </row>
     <row r="923">
-      <c s="6" r="A923"/>
+      <c s="7" r="A923"/>
     </row>
     <row r="924">
-      <c s="6" r="A924"/>
+      <c s="7" r="A924"/>
     </row>
     <row r="925">
-      <c s="6" r="A925"/>
+      <c s="7" r="A925"/>
     </row>
     <row r="926">
-      <c s="6" r="A926"/>
+      <c s="7" r="A926"/>
     </row>
     <row r="927">
-      <c s="6" r="A927"/>
+      <c s="7" r="A927"/>
     </row>
     <row r="928">
-      <c s="6" r="A928"/>
+      <c s="7" r="A928"/>
     </row>
     <row r="929">
-      <c s="6" r="A929"/>
+      <c s="7" r="A929"/>
     </row>
     <row r="930">
-      <c s="6" r="A930"/>
+      <c s="7" r="A930"/>
     </row>
     <row r="931">
-      <c s="6" r="A931"/>
+      <c s="7" r="A931"/>
     </row>
     <row r="932">
-      <c s="6" r="A932"/>
+      <c s="7" r="A932"/>
     </row>
     <row r="933">
-      <c s="6" r="A933"/>
+      <c s="7" r="A933"/>
     </row>
     <row r="934">
-      <c s="6" r="A934"/>
+      <c s="7" r="A934"/>
     </row>
     <row r="935">
-      <c s="6" r="A935"/>
+      <c s="7" r="A935"/>
     </row>
     <row r="936">
-      <c s="6" r="A936"/>
+      <c s="7" r="A936"/>
     </row>
     <row r="937">
-      <c s="6" r="A937"/>
+      <c s="7" r="A937"/>
     </row>
     <row r="938">
-      <c s="6" r="A938"/>
+      <c s="7" r="A938"/>
     </row>
     <row r="939">
-      <c s="6" r="A939"/>
+      <c s="7" r="A939"/>
     </row>
     <row r="940">
-      <c s="6" r="A940"/>
+      <c s="7" r="A940"/>
     </row>
     <row r="941">
-      <c s="6" r="A941"/>
+      <c s="7" r="A941"/>
     </row>
     <row r="942">
-      <c s="6" r="A942"/>
+      <c s="7" r="A942"/>
     </row>
     <row r="943">
-      <c s="6" r="A943"/>
+      <c s="7" r="A943"/>
     </row>
     <row r="944">
-      <c s="6" r="A944"/>
+      <c s="7" r="A944"/>
     </row>
     <row r="945">
-      <c s="6" r="A945"/>
+      <c s="7" r="A945"/>
     </row>
     <row r="946">
-      <c s="6" r="A946"/>
+      <c s="7" r="A946"/>
     </row>
     <row r="947">
-      <c s="6" r="A947"/>
+      <c s="7" r="A947"/>
     </row>
     <row r="948">
-      <c s="6" r="A948"/>
+      <c s="7" r="A948"/>
     </row>
     <row r="949">
-      <c s="6" r="A949"/>
+      <c s="7" r="A949"/>
     </row>
     <row r="950">
-      <c s="6" r="A950"/>
+      <c s="7" r="A950"/>
     </row>
     <row r="951">
-      <c s="6" r="A951"/>
+      <c s="7" r="A951"/>
     </row>
     <row r="952">
-      <c s="6" r="A952"/>
+      <c s="7" r="A952"/>
     </row>
     <row r="953">
-      <c s="6" r="A953"/>
+      <c s="7" r="A953"/>
     </row>
     <row r="954">
-      <c s="6" r="A954"/>
+      <c s="7" r="A954"/>
     </row>
     <row r="955">
-      <c s="6" r="A955"/>
+      <c s="7" r="A955"/>
     </row>
     <row r="956">
-      <c s="6" r="A956"/>
+      <c s="7" r="A956"/>
     </row>
     <row r="957">
-      <c s="6" r="A957"/>
+      <c s="7" r="A957"/>
     </row>
     <row r="958">
-      <c s="6" r="A958"/>
+      <c s="7" r="A958"/>
     </row>
     <row r="959">
-      <c s="6" r="A959"/>
+      <c s="7" r="A959"/>
     </row>
     <row r="960">
-      <c s="6" r="A960"/>
+      <c s="7" r="A960"/>
     </row>
     <row r="961">
-      <c s="6" r="A961"/>
+      <c s="7" r="A961"/>
     </row>
     <row r="962">
-      <c s="6" r="A962"/>
+      <c s="7" r="A962"/>
     </row>
     <row r="963">
-      <c s="6" r="A963"/>
+      <c s="7" r="A963"/>
     </row>
     <row r="964">
-      <c s="6" r="A964"/>
+      <c s="7" r="A964"/>
     </row>
     <row r="965">
-      <c s="6" r="A965"/>
+      <c s="7" r="A965"/>
     </row>
     <row r="966">
-      <c s="6" r="A966"/>
+      <c s="7" r="A966"/>
     </row>
     <row r="967">
-      <c s="6" r="A967"/>
+      <c s="7" r="A967"/>
     </row>
     <row r="968">
-      <c s="6" r="A968"/>
+      <c s="7" r="A968"/>
     </row>
     <row r="969">
-      <c s="6" r="A969"/>
+      <c s="7" r="A969"/>
     </row>
     <row r="970">
-      <c s="6" r="A970"/>
+      <c s="7" r="A970"/>
     </row>
     <row r="971">
-      <c s="6" r="A971"/>
+      <c s="7" r="A971"/>
     </row>
     <row r="972">
-      <c s="6" r="A972"/>
+      <c s="7" r="A972"/>
     </row>
     <row r="973">
-      <c s="6" r="A973"/>
+      <c s="7" r="A973"/>
     </row>
     <row r="974">
-      <c s="6" r="A974"/>
+      <c s="7" r="A974"/>
     </row>
     <row r="975">
-      <c s="6" r="A975"/>
+      <c s="7" r="A975"/>
     </row>
     <row r="976">
-      <c s="6" r="A976"/>
+      <c s="7" r="A976"/>
     </row>
     <row r="977">
-      <c s="6" r="A977"/>
+      <c s="7" r="A977"/>
     </row>
     <row r="978">
-      <c s="6" r="A978"/>
+      <c s="7" r="A978"/>
     </row>
     <row r="979">
-      <c s="6" r="A979"/>
+      <c s="7" r="A979"/>
     </row>
     <row r="980">
-      <c s="6" r="A980"/>
+      <c s="7" r="A980"/>
     </row>
     <row r="981">
-      <c s="6" r="A981"/>
+      <c s="7" r="A981"/>
     </row>
     <row r="982">
-      <c s="6" r="A982"/>
+      <c s="7" r="A982"/>
     </row>
     <row r="983">
-      <c s="6" r="A983"/>
+      <c s="7" r="A983"/>
     </row>
     <row r="984">
-      <c s="6" r="A984"/>
+      <c s="7" r="A984"/>
     </row>
     <row r="985">
-      <c s="6" r="A985"/>
+      <c s="7" r="A985"/>
     </row>
     <row r="986">
-      <c s="6" r="A986"/>
+      <c s="7" r="A986"/>
     </row>
     <row r="987">
-      <c s="6" r="A987"/>
+      <c s="7" r="A987"/>
     </row>
     <row r="988">
-      <c s="6" r="A988"/>
+      <c s="7" r="A988"/>
     </row>
     <row r="989">
-      <c s="6" r="A989"/>
+      <c s="7" r="A989"/>
     </row>
     <row r="990">
-      <c s="6" r="A990"/>
+      <c s="7" r="A990"/>
     </row>
     <row r="991">
-      <c s="6" r="A991"/>
+      <c s="7" r="A991"/>
     </row>
     <row r="992">
-      <c s="6" r="A992"/>
+      <c s="7" r="A992"/>
     </row>
     <row r="993">
-      <c s="6" r="A993"/>
+      <c s="7" r="A993"/>
     </row>
     <row r="994">
-      <c s="6" r="A994"/>
+      <c s="7" r="A994"/>
     </row>
     <row r="995">
-      <c s="6" r="A995"/>
+      <c s="7" r="A995"/>
     </row>
     <row r="996">
-      <c s="6" r="A996"/>
+      <c s="7" r="A996"/>
     </row>
     <row r="997">
-      <c s="6" r="A997"/>
+      <c s="7" r="A997"/>
     </row>
     <row r="998">
-      <c s="6" r="A998"/>
+      <c s="7" r="A998"/>
     </row>
     <row r="999">
-      <c s="6" r="A999"/>
+      <c s="7" r="A999"/>
     </row>
     <row r="1000">
-      <c s="6" r="A1000"/>
+      <c s="7" r="A1000"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
rearranged slider to put img next to blurb, added attribution
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -19,6 +19,9 @@
     <t>quote</t>
   </si>
   <si>
+    <t>speaker</t>
+  </si>
+  <si>
     <t>month</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t>"You know how long that takes in Texas at 75 miles an hour? That's a particularly flat highway."</t>
   </si>
   <si>
+    <t>Judge Edith Jones</t>
+  </si>
+  <si>
     <t>January</t>
   </si>
   <si>
@@ -61,6 +67,9 @@
     <t>“MARRIAGE = ONE MAN &amp; ONE MAN. Enough of these activist judges. FAVORITE if you agree. I know the silent majority out there is with us!”</t>
   </si>
   <si>
+    <t>State Sen. Dan Patrick</t>
+  </si>
+  <si>
     <t>February</t>
   </si>
   <si>
@@ -82,6 +91,9 @@
     <t>"Apparently I’ve outfoxed the campaign deal, so maybe I need to be a consultant. I’m not going to run all over the state. I work."</t>
   </si>
   <si>
+    <t>Jim Hogan</t>
+  </si>
+  <si>
     <t>March</t>
   </si>
   <si>
@@ -103,6 +115,9 @@
     <t>"Out there on Twitter, in front of the Alamo in your campaign, you know, you’ve been huffing and puffing like the big bad wolf and now you’re dancing around, tiptoeing like Little Red Riding Hood on this issue."</t>
   </si>
   <si>
+    <t>San Antonio Mayor Julián Castro</t>
+  </si>
+  <si>
     <t>April</t>
   </si>
   <si>
@@ -124,6 +139,9 @@
     <t>"Dewhurst has asked me to cease distribution of this information. He also asked me not to run against him for Lt. Gov. I didn't really give a damn what David wanted then, and I don't give a damn now. The voters of Texas need to know."</t>
   </si>
   <si>
+    <t>Jerry Patterson</t>
+  </si>
+  <si>
     <t>May</t>
   </si>
   <si>
@@ -145,6 +163,9 @@
     <t>"Some Democrats have said they wanted me to be the nominee. Well, they’ve got me and I’m coming."</t>
   </si>
   <si>
+    <t>State Sen. Dan Patrick</t>
+  </si>
+  <si>
     <t>May</t>
   </si>
   <si>
@@ -166,6 +187,9 @@
     <t>"The uninformed opinions of a Washington, D.C., desk jockey who's never stepped foot in Texas couldn't be less relevant to what's actually happening on the ground."</t>
   </si>
   <si>
+    <t>Karin Johanson</t>
+  </si>
+  <si>
     <t>June</t>
   </si>
   <si>
@@ -187,6 +211,9 @@
     <t>“We need to look at the states, which are lavatories of innovation and democracy.”</t>
   </si>
   <si>
+    <t>Gov. Rick Perry</t>
+  </si>
+  <si>
     <t>August</t>
   </si>
   <si>
@@ -208,6 +235,9 @@
     <t>"We don't settle political differences with indictments in this country. It is outrageous that some would use partisan political theatrics to rip away at the very fabric of our state's constitution."</t>
   </si>
   <si>
+    <t>Gov. Rick Perry</t>
+  </si>
+  <si>
     <t>August</t>
   </si>
   <si>
@@ -229,6 +259,9 @@
     <t>“And all I can do is deal with the issues that are before me. … The job of attorney general is to represent and defend in court the laws of their client, which is the state Legislature, unless and until a court strikes it down.”</t>
   </si>
   <si>
+    <t>Attorney General Greg Abbott</t>
+  </si>
+  <si>
     <t>October</t>
   </si>
   <si>
@@ -250,6 +283,9 @@
     <t>"If that dog has to be The Boy in the Plastic Bubble, we're going to take good care of that dog."</t>
   </si>
   <si>
+    <t>Judge Clay Jenkins</t>
+  </si>
+  <si>
     <t>October</t>
   </si>
   <si>
@@ -271,6 +307,9 @@
     <t>"The only way we will have lost tonight is if we stop fighting. I am so proud of all that we have accomplished."</t>
   </si>
   <si>
+    <t>Wendy Davis</t>
+  </si>
+  <si>
     <t>November</t>
   </si>
   <si>
@@ -290,6 +329,9 @@
   </si>
   <si>
     <t>“We were elected to govern. If we blow it by not governing, then shame on us.”</t>
+  </si>
+  <si>
+    <t>U.S. Rep. Michael McCaul</t>
   </si>
   <si>
     <t>December</t>
@@ -328,12 +370,18 @@
       <sz val="10.0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -354,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -369,6 +417,9 @@
       <alignment/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
       <alignment/>
     </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3"/>
@@ -393,8 +444,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="5" customWidth="1" max="5" width="26.14"/>
-    <col min="6" customWidth="1" max="6" width="25.29"/>
+    <col min="5" customWidth="1" max="5" width="36.43"/>
+    <col min="6" customWidth="1" max="6" width="26.14"/>
+    <col min="7" customWidth="1" max="7" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -419,8 +471,11 @@
       <c t="s" s="2" r="G1">
         <v>6</v>
       </c>
-      <c t="s" s="3" r="H1">
+      <c t="s" s="2" r="H1">
         <v>7</v>
+      </c>
+      <c t="s" s="3" r="I1">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -428,25 +483,28 @@
         <v>0.0</v>
       </c>
       <c t="s" s="5" r="B2">
-        <v>8</v>
-      </c>
-      <c t="s" s="5" r="C2">
         <v>9</v>
       </c>
+      <c t="s" s="6" r="C2">
+        <v>10</v>
+      </c>
       <c t="s" s="5" r="D2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c t="s" s="5" r="E2">
-        <v>11</v>
-      </c>
-      <c t="s" s="6" r="F2">
         <v>12</v>
       </c>
-      <c t="s" s="6" r="G2">
+      <c t="s" s="5" r="F2">
         <v>13</v>
       </c>
-      <c t="s" s="3" r="H2">
+      <c t="s" s="7" r="G2">
         <v>14</v>
+      </c>
+      <c t="s" s="7" r="H2">
+        <v>15</v>
+      </c>
+      <c t="s" s="3" r="I2">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -454,25 +512,28 @@
         <v>1.0</v>
       </c>
       <c t="s" s="5" r="B3">
-        <v>15</v>
-      </c>
-      <c t="s" s="5" r="C3">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c t="s" s="6" r="C3">
+        <v>18</v>
       </c>
       <c t="s" s="5" r="D3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c t="s" s="5" r="E3">
-        <v>18</v>
-      </c>
-      <c t="s" s="6" r="F3">
-        <v>19</v>
-      </c>
-      <c t="s" s="5" r="G3">
         <v>20</v>
       </c>
-      <c t="s" s="3" r="H3">
+      <c t="s" s="5" r="F3">
         <v>21</v>
+      </c>
+      <c t="s" s="7" r="G3">
+        <v>22</v>
+      </c>
+      <c t="s" s="5" r="H3">
+        <v>23</v>
+      </c>
+      <c t="s" s="3" r="I3">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -480,25 +541,28 @@
         <v>2.0</v>
       </c>
       <c t="s" s="5" r="B4">
-        <v>22</v>
-      </c>
-      <c t="s" s="5" r="C4">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c t="s" s="6" r="C4">
+        <v>26</v>
       </c>
       <c t="s" s="5" r="D4">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c t="s" s="5" r="E4">
-        <v>25</v>
-      </c>
-      <c t="s" s="6" r="F4">
-        <v>26</v>
-      </c>
-      <c t="s" s="6" r="G4">
-        <v>27</v>
-      </c>
-      <c t="s" s="3" r="H4">
         <v>28</v>
+      </c>
+      <c t="s" s="5" r="F4">
+        <v>29</v>
+      </c>
+      <c t="s" s="7" r="G4">
+        <v>30</v>
+      </c>
+      <c t="s" s="7" r="H4">
+        <v>31</v>
+      </c>
+      <c t="s" s="3" r="I4">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -506,25 +570,28 @@
         <v>3.0</v>
       </c>
       <c t="s" s="5" r="B5">
-        <v>29</v>
-      </c>
-      <c t="s" s="5" r="C5">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c t="s" s="6" r="C5">
+        <v>34</v>
       </c>
       <c t="s" s="5" r="D5">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c t="s" s="5" r="E5">
-        <v>32</v>
-      </c>
-      <c t="s" s="6" r="F5">
-        <v>33</v>
-      </c>
-      <c t="s" s="6" r="G5">
-        <v>34</v>
-      </c>
-      <c t="s" s="3" r="H5">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c t="s" s="5" r="F5">
+        <v>37</v>
+      </c>
+      <c t="s" s="7" r="G5">
+        <v>38</v>
+      </c>
+      <c t="s" s="7" r="H5">
+        <v>39</v>
+      </c>
+      <c t="s" s="3" r="I5">
+        <v>40</v>
       </c>
     </row>
     <row r="6">
@@ -532,25 +599,28 @@
         <v>4.0</v>
       </c>
       <c t="s" s="5" r="B6">
-        <v>36</v>
-      </c>
-      <c t="s" s="5" r="C6">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c t="s" s="6" r="C6">
+        <v>42</v>
       </c>
       <c t="s" s="5" r="D6">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c t="s" s="5" r="E6">
-        <v>39</v>
-      </c>
-      <c t="s" s="6" r="F6">
-        <v>40</v>
-      </c>
-      <c t="s" s="6" r="G6">
-        <v>41</v>
-      </c>
-      <c t="s" s="3" r="H6">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c t="s" s="5" r="F6">
+        <v>45</v>
+      </c>
+      <c t="s" s="7" r="G6">
+        <v>46</v>
+      </c>
+      <c t="s" s="7" r="H6">
+        <v>47</v>
+      </c>
+      <c t="s" s="3" r="I6">
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -558,25 +628,28 @@
         <v>5.0</v>
       </c>
       <c t="s" s="5" r="B7">
-        <v>43</v>
-      </c>
-      <c t="s" s="5" r="C7">
-        <v>44</v>
+        <v>49</v>
+      </c>
+      <c t="s" s="6" r="C7">
+        <v>50</v>
       </c>
       <c t="s" s="5" r="D7">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c t="s" s="5" r="E7">
-        <v>46</v>
-      </c>
-      <c t="s" s="6" r="F7">
-        <v>47</v>
-      </c>
-      <c t="s" s="6" r="G7">
-        <v>48</v>
-      </c>
-      <c t="s" s="3" r="H7">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c t="s" s="5" r="F7">
+        <v>53</v>
+      </c>
+      <c t="s" s="7" r="G7">
+        <v>54</v>
+      </c>
+      <c t="s" s="7" r="H7">
+        <v>55</v>
+      </c>
+      <c t="s" s="3" r="I7">
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -584,25 +657,28 @@
         <v>6.0</v>
       </c>
       <c t="s" s="5" r="B8">
-        <v>50</v>
-      </c>
-      <c t="s" s="5" r="C8">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c t="s" s="6" r="C8">
+        <v>58</v>
       </c>
       <c t="s" s="5" r="D8">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c t="s" s="5" r="E8">
-        <v>53</v>
-      </c>
-      <c t="s" s="6" r="F8">
-        <v>54</v>
-      </c>
-      <c t="s" s="6" r="G8">
-        <v>55</v>
-      </c>
-      <c t="s" s="3" r="H8">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c t="s" s="5" r="F8">
+        <v>61</v>
+      </c>
+      <c t="s" s="7" r="G8">
+        <v>62</v>
+      </c>
+      <c t="s" s="7" r="H8">
+        <v>63</v>
+      </c>
+      <c t="s" s="3" r="I8">
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -610,25 +686,28 @@
         <v>7.0</v>
       </c>
       <c t="s" s="5" r="B9">
-        <v>57</v>
-      </c>
-      <c t="s" s="5" r="C9">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c t="s" s="6" r="C9">
+        <v>66</v>
       </c>
       <c t="s" s="5" r="D9">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c t="s" s="5" r="E9">
-        <v>60</v>
-      </c>
-      <c t="s" s="6" r="F9">
-        <v>61</v>
-      </c>
-      <c t="s" s="6" r="G9">
-        <v>62</v>
-      </c>
-      <c t="s" s="3" r="H9">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c t="s" s="5" r="F9">
+        <v>69</v>
+      </c>
+      <c t="s" s="7" r="G9">
+        <v>70</v>
+      </c>
+      <c t="s" s="7" r="H9">
+        <v>71</v>
+      </c>
+      <c t="s" s="3" r="I9">
+        <v>72</v>
       </c>
     </row>
     <row r="10">
@@ -636,25 +715,28 @@
         <v>8.0</v>
       </c>
       <c t="s" s="5" r="B10">
-        <v>64</v>
-      </c>
-      <c t="s" s="5" r="C10">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c t="s" s="6" r="C10">
+        <v>74</v>
       </c>
       <c t="s" s="5" r="D10">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c t="s" s="5" r="E10">
-        <v>67</v>
-      </c>
-      <c t="s" s="6" r="F10">
-        <v>68</v>
-      </c>
-      <c t="s" s="6" r="G10">
-        <v>69</v>
-      </c>
-      <c t="s" s="3" r="H10">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c t="s" s="5" r="F10">
+        <v>77</v>
+      </c>
+      <c t="s" s="7" r="G10">
+        <v>78</v>
+      </c>
+      <c t="s" s="7" r="H10">
+        <v>79</v>
+      </c>
+      <c t="s" s="3" r="I10">
+        <v>80</v>
       </c>
     </row>
     <row r="11">
@@ -662,25 +744,28 @@
         <v>9.0</v>
       </c>
       <c t="s" s="5" r="B11">
-        <v>71</v>
-      </c>
-      <c t="s" s="5" r="C11">
-        <v>72</v>
+        <v>81</v>
+      </c>
+      <c t="s" s="6" r="C11">
+        <v>82</v>
       </c>
       <c t="s" s="5" r="D11">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c t="s" s="5" r="E11">
-        <v>74</v>
-      </c>
-      <c t="s" s="6" r="F11">
-        <v>75</v>
-      </c>
-      <c t="s" s="6" r="G11">
-        <v>76</v>
-      </c>
-      <c t="s" s="3" r="H11">
-        <v>77</v>
+        <v>84</v>
+      </c>
+      <c t="s" s="5" r="F11">
+        <v>85</v>
+      </c>
+      <c t="s" s="7" r="G11">
+        <v>86</v>
+      </c>
+      <c t="s" s="7" r="H11">
+        <v>87</v>
+      </c>
+      <c t="s" s="3" r="I11">
+        <v>88</v>
       </c>
     </row>
     <row r="12">
@@ -688,25 +773,28 @@
         <v>10.0</v>
       </c>
       <c t="s" s="5" r="B12">
-        <v>78</v>
-      </c>
-      <c t="s" s="5" r="C12">
-        <v>79</v>
+        <v>89</v>
+      </c>
+      <c t="s" s="6" r="C12">
+        <v>90</v>
       </c>
       <c t="s" s="5" r="D12">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c t="s" s="5" r="E12">
-        <v>81</v>
-      </c>
-      <c t="s" s="6" r="F12">
-        <v>82</v>
-      </c>
-      <c t="s" s="6" r="G12">
-        <v>83</v>
-      </c>
-      <c t="s" s="3" r="H12">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c t="s" s="5" r="F12">
+        <v>93</v>
+      </c>
+      <c t="s" s="7" r="G12">
+        <v>94</v>
+      </c>
+      <c t="s" s="7" r="H12">
+        <v>95</v>
+      </c>
+      <c t="s" s="3" r="I12">
+        <v>96</v>
       </c>
     </row>
     <row r="13">
@@ -714,25 +802,28 @@
         <v>11.0</v>
       </c>
       <c t="s" s="5" r="B13">
-        <v>85</v>
-      </c>
-      <c t="s" s="5" r="C13">
-        <v>86</v>
+        <v>97</v>
+      </c>
+      <c t="s" s="6" r="C13">
+        <v>98</v>
       </c>
       <c t="s" s="5" r="D13">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c t="s" s="5" r="E13">
-        <v>88</v>
-      </c>
-      <c t="s" s="6" r="F13">
-        <v>89</v>
-      </c>
-      <c t="s" s="6" r="G13">
-        <v>90</v>
-      </c>
-      <c t="s" s="3" r="H13">
-        <v>91</v>
+        <v>100</v>
+      </c>
+      <c t="s" s="5" r="F13">
+        <v>101</v>
+      </c>
+      <c t="s" s="7" r="G13">
+        <v>102</v>
+      </c>
+      <c t="s" s="7" r="H13">
+        <v>103</v>
+      </c>
+      <c t="s" s="3" r="I13">
+        <v>104</v>
       </c>
     </row>
     <row r="14">
@@ -740,2984 +831,2987 @@
         <v>12.0</v>
       </c>
       <c t="s" s="5" r="B14">
-        <v>92</v>
-      </c>
-      <c t="s" s="5" r="C14">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c t="s" s="6" r="C14">
+        <v>106</v>
       </c>
       <c t="s" s="5" r="D14">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c t="s" s="5" r="E14">
-        <v>95</v>
-      </c>
-      <c t="s" s="6" r="F14">
-        <v>96</v>
-      </c>
-      <c t="s" s="6" r="G14">
-        <v>97</v>
-      </c>
-      <c t="s" s="3" r="H14">
-        <v>98</v>
+        <v>108</v>
+      </c>
+      <c t="s" s="5" r="F14">
+        <v>109</v>
+      </c>
+      <c t="s" s="7" r="G14">
+        <v>110</v>
+      </c>
+      <c t="s" s="7" r="H14">
+        <v>111</v>
+      </c>
+      <c t="s" s="3" r="I14">
+        <v>112</v>
       </c>
     </row>
     <row r="15">
-      <c s="7" r="A15"/>
+      <c s="8" r="A15"/>
     </row>
     <row r="16">
-      <c s="7" r="A16"/>
+      <c s="8" r="A16"/>
     </row>
     <row r="17">
-      <c s="7" r="A17"/>
+      <c s="8" r="A17"/>
     </row>
     <row r="18">
-      <c s="7" r="A18"/>
+      <c s="8" r="A18"/>
     </row>
     <row r="19">
-      <c s="7" r="A19"/>
+      <c s="8" r="A19"/>
     </row>
     <row r="20">
-      <c s="7" r="A20"/>
+      <c s="8" r="A20"/>
     </row>
     <row r="21">
-      <c s="7" r="A21"/>
+      <c s="8" r="A21"/>
     </row>
     <row r="22">
-      <c s="7" r="A22"/>
+      <c s="8" r="A22"/>
     </row>
     <row r="23">
-      <c s="7" r="A23"/>
+      <c s="8" r="A23"/>
     </row>
     <row r="24">
-      <c s="7" r="A24"/>
+      <c s="8" r="A24"/>
     </row>
     <row r="25">
-      <c s="7" r="A25"/>
+      <c s="8" r="A25"/>
     </row>
     <row r="26">
-      <c s="7" r="A26"/>
+      <c s="8" r="A26"/>
     </row>
     <row r="27">
-      <c s="7" r="A27"/>
+      <c s="8" r="A27"/>
     </row>
     <row r="28">
-      <c s="7" r="A28"/>
+      <c s="8" r="A28"/>
     </row>
     <row r="29">
-      <c s="7" r="A29"/>
+      <c s="8" r="A29"/>
     </row>
     <row r="30">
-      <c s="7" r="A30"/>
+      <c s="8" r="A30"/>
     </row>
     <row r="31">
-      <c s="7" r="A31"/>
+      <c s="8" r="A31"/>
     </row>
     <row r="32">
-      <c s="7" r="A32"/>
+      <c s="8" r="A32"/>
     </row>
     <row r="33">
-      <c s="7" r="A33"/>
+      <c s="8" r="A33"/>
     </row>
     <row r="34">
-      <c s="7" r="A34"/>
+      <c s="8" r="A34"/>
     </row>
     <row r="35">
-      <c s="7" r="A35"/>
+      <c s="8" r="A35"/>
     </row>
     <row r="36">
-      <c s="7" r="A36"/>
+      <c s="8" r="A36"/>
     </row>
     <row r="37">
-      <c s="7" r="A37"/>
+      <c s="8" r="A37"/>
     </row>
     <row r="38">
-      <c s="7" r="A38"/>
+      <c s="8" r="A38"/>
     </row>
     <row r="39">
-      <c s="7" r="A39"/>
+      <c s="8" r="A39"/>
     </row>
     <row r="40">
-      <c s="7" r="A40"/>
+      <c s="8" r="A40"/>
     </row>
     <row r="41">
-      <c s="7" r="A41"/>
+      <c s="8" r="A41"/>
     </row>
     <row r="42">
-      <c s="7" r="A42"/>
+      <c s="8" r="A42"/>
     </row>
     <row r="43">
-      <c s="7" r="A43"/>
+      <c s="8" r="A43"/>
     </row>
     <row r="44">
-      <c s="7" r="A44"/>
+      <c s="8" r="A44"/>
     </row>
     <row r="45">
-      <c s="7" r="A45"/>
+      <c s="8" r="A45"/>
     </row>
     <row r="46">
-      <c s="7" r="A46"/>
+      <c s="8" r="A46"/>
     </row>
     <row r="47">
-      <c s="7" r="A47"/>
+      <c s="8" r="A47"/>
     </row>
     <row r="48">
-      <c s="7" r="A48"/>
+      <c s="8" r="A48"/>
     </row>
     <row r="49">
-      <c s="7" r="A49"/>
+      <c s="8" r="A49"/>
     </row>
     <row r="50">
-      <c s="7" r="A50"/>
+      <c s="8" r="A50"/>
     </row>
     <row r="51">
-      <c s="7" r="A51"/>
+      <c s="8" r="A51"/>
     </row>
     <row r="52">
-      <c s="7" r="A52"/>
+      <c s="8" r="A52"/>
     </row>
     <row r="53">
-      <c s="7" r="A53"/>
+      <c s="8" r="A53"/>
     </row>
     <row r="54">
-      <c s="7" r="A54"/>
+      <c s="8" r="A54"/>
     </row>
     <row r="55">
-      <c s="7" r="A55"/>
+      <c s="8" r="A55"/>
     </row>
     <row r="56">
-      <c s="7" r="A56"/>
+      <c s="8" r="A56"/>
     </row>
     <row r="57">
-      <c s="7" r="A57"/>
+      <c s="8" r="A57"/>
     </row>
     <row r="58">
-      <c s="7" r="A58"/>
+      <c s="8" r="A58"/>
     </row>
     <row r="59">
-      <c s="7" r="A59"/>
+      <c s="8" r="A59"/>
     </row>
     <row r="60">
-      <c s="7" r="A60"/>
+      <c s="8" r="A60"/>
     </row>
     <row r="61">
-      <c s="7" r="A61"/>
+      <c s="8" r="A61"/>
     </row>
     <row r="62">
-      <c s="7" r="A62"/>
+      <c s="8" r="A62"/>
     </row>
     <row r="63">
-      <c s="7" r="A63"/>
+      <c s="8" r="A63"/>
     </row>
     <row r="64">
-      <c s="7" r="A64"/>
+      <c s="8" r="A64"/>
     </row>
     <row r="65">
-      <c s="7" r="A65"/>
+      <c s="8" r="A65"/>
     </row>
     <row r="66">
-      <c s="7" r="A66"/>
+      <c s="8" r="A66"/>
     </row>
     <row r="67">
-      <c s="7" r="A67"/>
+      <c s="8" r="A67"/>
     </row>
     <row r="68">
-      <c s="7" r="A68"/>
+      <c s="8" r="A68"/>
     </row>
     <row r="69">
-      <c s="7" r="A69"/>
+      <c s="8" r="A69"/>
     </row>
     <row r="70">
-      <c s="7" r="A70"/>
+      <c s="8" r="A70"/>
     </row>
     <row r="71">
-      <c s="7" r="A71"/>
+      <c s="8" r="A71"/>
     </row>
     <row r="72">
-      <c s="7" r="A72"/>
+      <c s="8" r="A72"/>
     </row>
     <row r="73">
-      <c s="7" r="A73"/>
+      <c s="8" r="A73"/>
     </row>
     <row r="74">
-      <c s="7" r="A74"/>
+      <c s="8" r="A74"/>
     </row>
     <row r="75">
-      <c s="7" r="A75"/>
+      <c s="8" r="A75"/>
     </row>
     <row r="76">
-      <c s="7" r="A76"/>
+      <c s="8" r="A76"/>
     </row>
     <row r="77">
-      <c s="7" r="A77"/>
+      <c s="8" r="A77"/>
     </row>
     <row r="78">
-      <c s="7" r="A78"/>
+      <c s="8" r="A78"/>
     </row>
     <row r="79">
-      <c s="7" r="A79"/>
+      <c s="8" r="A79"/>
     </row>
     <row r="80">
-      <c s="7" r="A80"/>
+      <c s="8" r="A80"/>
     </row>
     <row r="81">
-      <c s="7" r="A81"/>
+      <c s="8" r="A81"/>
     </row>
     <row r="82">
-      <c s="7" r="A82"/>
+      <c s="8" r="A82"/>
     </row>
     <row r="83">
-      <c s="7" r="A83"/>
+      <c s="8" r="A83"/>
     </row>
     <row r="84">
-      <c s="7" r="A84"/>
+      <c s="8" r="A84"/>
     </row>
     <row r="85">
-      <c s="7" r="A85"/>
+      <c s="8" r="A85"/>
     </row>
     <row r="86">
-      <c s="7" r="A86"/>
+      <c s="8" r="A86"/>
     </row>
     <row r="87">
-      <c s="7" r="A87"/>
+      <c s="8" r="A87"/>
     </row>
     <row r="88">
-      <c s="7" r="A88"/>
+      <c s="8" r="A88"/>
     </row>
     <row r="89">
-      <c s="7" r="A89"/>
+      <c s="8" r="A89"/>
     </row>
     <row r="90">
-      <c s="7" r="A90"/>
+      <c s="8" r="A90"/>
     </row>
     <row r="91">
-      <c s="7" r="A91"/>
+      <c s="8" r="A91"/>
     </row>
     <row r="92">
-      <c s="7" r="A92"/>
+      <c s="8" r="A92"/>
     </row>
     <row r="93">
-      <c s="7" r="A93"/>
+      <c s="8" r="A93"/>
     </row>
     <row r="94">
-      <c s="7" r="A94"/>
+      <c s="8" r="A94"/>
     </row>
     <row r="95">
-      <c s="7" r="A95"/>
+      <c s="8" r="A95"/>
     </row>
     <row r="96">
-      <c s="7" r="A96"/>
+      <c s="8" r="A96"/>
     </row>
     <row r="97">
-      <c s="7" r="A97"/>
+      <c s="8" r="A97"/>
     </row>
     <row r="98">
-      <c s="7" r="A98"/>
+      <c s="8" r="A98"/>
     </row>
     <row r="99">
-      <c s="7" r="A99"/>
+      <c s="8" r="A99"/>
     </row>
     <row r="100">
-      <c s="7" r="A100"/>
+      <c s="8" r="A100"/>
     </row>
     <row r="101">
-      <c s="7" r="A101"/>
+      <c s="8" r="A101"/>
     </row>
     <row r="102">
-      <c s="7" r="A102"/>
+      <c s="8" r="A102"/>
     </row>
     <row r="103">
-      <c s="7" r="A103"/>
+      <c s="8" r="A103"/>
     </row>
     <row r="104">
-      <c s="7" r="A104"/>
+      <c s="8" r="A104"/>
     </row>
     <row r="105">
-      <c s="7" r="A105"/>
+      <c s="8" r="A105"/>
     </row>
     <row r="106">
-      <c s="7" r="A106"/>
+      <c s="8" r="A106"/>
     </row>
     <row r="107">
-      <c s="7" r="A107"/>
+      <c s="8" r="A107"/>
     </row>
     <row r="108">
-      <c s="7" r="A108"/>
+      <c s="8" r="A108"/>
     </row>
     <row r="109">
-      <c s="7" r="A109"/>
+      <c s="8" r="A109"/>
     </row>
     <row r="110">
-      <c s="7" r="A110"/>
+      <c s="8" r="A110"/>
     </row>
     <row r="111">
-      <c s="7" r="A111"/>
+      <c s="8" r="A111"/>
     </row>
     <row r="112">
-      <c s="7" r="A112"/>
+      <c s="8" r="A112"/>
     </row>
     <row r="113">
-      <c s="7" r="A113"/>
+      <c s="8" r="A113"/>
     </row>
     <row r="114">
-      <c s="7" r="A114"/>
+      <c s="8" r="A114"/>
     </row>
     <row r="115">
-      <c s="7" r="A115"/>
+      <c s="8" r="A115"/>
     </row>
     <row r="116">
-      <c s="7" r="A116"/>
+      <c s="8" r="A116"/>
     </row>
     <row r="117">
-      <c s="7" r="A117"/>
+      <c s="8" r="A117"/>
     </row>
     <row r="118">
-      <c s="7" r="A118"/>
+      <c s="8" r="A118"/>
     </row>
     <row r="119">
-      <c s="7" r="A119"/>
+      <c s="8" r="A119"/>
     </row>
     <row r="120">
-      <c s="7" r="A120"/>
+      <c s="8" r="A120"/>
     </row>
     <row r="121">
-      <c s="7" r="A121"/>
+      <c s="8" r="A121"/>
     </row>
     <row r="122">
-      <c s="7" r="A122"/>
+      <c s="8" r="A122"/>
     </row>
     <row r="123">
-      <c s="7" r="A123"/>
+      <c s="8" r="A123"/>
     </row>
     <row r="124">
-      <c s="7" r="A124"/>
+      <c s="8" r="A124"/>
     </row>
     <row r="125">
-      <c s="7" r="A125"/>
+      <c s="8" r="A125"/>
     </row>
     <row r="126">
-      <c s="7" r="A126"/>
+      <c s="8" r="A126"/>
     </row>
     <row r="127">
-      <c s="7" r="A127"/>
+      <c s="8" r="A127"/>
     </row>
     <row r="128">
-      <c s="7" r="A128"/>
+      <c s="8" r="A128"/>
     </row>
     <row r="129">
-      <c s="7" r="A129"/>
+      <c s="8" r="A129"/>
     </row>
     <row r="130">
-      <c s="7" r="A130"/>
+      <c s="8" r="A130"/>
     </row>
     <row r="131">
-      <c s="7" r="A131"/>
+      <c s="8" r="A131"/>
     </row>
     <row r="132">
-      <c s="7" r="A132"/>
+      <c s="8" r="A132"/>
     </row>
     <row r="133">
-      <c s="7" r="A133"/>
+      <c s="8" r="A133"/>
     </row>
     <row r="134">
-      <c s="7" r="A134"/>
+      <c s="8" r="A134"/>
     </row>
     <row r="135">
-      <c s="7" r="A135"/>
+      <c s="8" r="A135"/>
     </row>
     <row r="136">
-      <c s="7" r="A136"/>
+      <c s="8" r="A136"/>
     </row>
     <row r="137">
-      <c s="7" r="A137"/>
+      <c s="8" r="A137"/>
     </row>
     <row r="138">
-      <c s="7" r="A138"/>
+      <c s="8" r="A138"/>
     </row>
     <row r="139">
-      <c s="7" r="A139"/>
+      <c s="8" r="A139"/>
     </row>
     <row r="140">
-      <c s="7" r="A140"/>
+      <c s="8" r="A140"/>
     </row>
     <row r="141">
-      <c s="7" r="A141"/>
+      <c s="8" r="A141"/>
     </row>
     <row r="142">
-      <c s="7" r="A142"/>
+      <c s="8" r="A142"/>
     </row>
     <row r="143">
-      <c s="7" r="A143"/>
+      <c s="8" r="A143"/>
     </row>
     <row r="144">
-      <c s="7" r="A144"/>
+      <c s="8" r="A144"/>
     </row>
     <row r="145">
-      <c s="7" r="A145"/>
+      <c s="8" r="A145"/>
     </row>
     <row r="146">
-      <c s="7" r="A146"/>
+      <c s="8" r="A146"/>
     </row>
     <row r="147">
-      <c s="7" r="A147"/>
+      <c s="8" r="A147"/>
     </row>
     <row r="148">
-      <c s="7" r="A148"/>
+      <c s="8" r="A148"/>
     </row>
     <row r="149">
-      <c s="7" r="A149"/>
+      <c s="8" r="A149"/>
     </row>
     <row r="150">
-      <c s="7" r="A150"/>
+      <c s="8" r="A150"/>
     </row>
     <row r="151">
-      <c s="7" r="A151"/>
+      <c s="8" r="A151"/>
     </row>
     <row r="152">
-      <c s="7" r="A152"/>
+      <c s="8" r="A152"/>
     </row>
     <row r="153">
-      <c s="7" r="A153"/>
+      <c s="8" r="A153"/>
     </row>
     <row r="154">
-      <c s="7" r="A154"/>
+      <c s="8" r="A154"/>
     </row>
     <row r="155">
-      <c s="7" r="A155"/>
+      <c s="8" r="A155"/>
     </row>
     <row r="156">
-      <c s="7" r="A156"/>
+      <c s="8" r="A156"/>
     </row>
     <row r="157">
-      <c s="7" r="A157"/>
+      <c s="8" r="A157"/>
     </row>
     <row r="158">
-      <c s="7" r="A158"/>
+      <c s="8" r="A158"/>
     </row>
     <row r="159">
-      <c s="7" r="A159"/>
+      <c s="8" r="A159"/>
     </row>
     <row r="160">
-      <c s="7" r="A160"/>
+      <c s="8" r="A160"/>
     </row>
     <row r="161">
-      <c s="7" r="A161"/>
+      <c s="8" r="A161"/>
     </row>
     <row r="162">
-      <c s="7" r="A162"/>
+      <c s="8" r="A162"/>
     </row>
     <row r="163">
-      <c s="7" r="A163"/>
+      <c s="8" r="A163"/>
     </row>
     <row r="164">
-      <c s="7" r="A164"/>
+      <c s="8" r="A164"/>
     </row>
     <row r="165">
-      <c s="7" r="A165"/>
+      <c s="8" r="A165"/>
     </row>
     <row r="166">
-      <c s="7" r="A166"/>
+      <c s="8" r="A166"/>
     </row>
     <row r="167">
-      <c s="7" r="A167"/>
+      <c s="8" r="A167"/>
     </row>
     <row r="168">
-      <c s="7" r="A168"/>
+      <c s="8" r="A168"/>
     </row>
     <row r="169">
-      <c s="7" r="A169"/>
+      <c s="8" r="A169"/>
     </row>
     <row r="170">
-      <c s="7" r="A170"/>
+      <c s="8" r="A170"/>
     </row>
     <row r="171">
-      <c s="7" r="A171"/>
+      <c s="8" r="A171"/>
     </row>
     <row r="172">
-      <c s="7" r="A172"/>
+      <c s="8" r="A172"/>
     </row>
     <row r="173">
-      <c s="7" r="A173"/>
+      <c s="8" r="A173"/>
     </row>
     <row r="174">
-      <c s="7" r="A174"/>
+      <c s="8" r="A174"/>
     </row>
     <row r="175">
-      <c s="7" r="A175"/>
+      <c s="8" r="A175"/>
     </row>
     <row r="176">
-      <c s="7" r="A176"/>
+      <c s="8" r="A176"/>
     </row>
     <row r="177">
-      <c s="7" r="A177"/>
+      <c s="8" r="A177"/>
     </row>
     <row r="178">
-      <c s="7" r="A178"/>
+      <c s="8" r="A178"/>
     </row>
     <row r="179">
-      <c s="7" r="A179"/>
+      <c s="8" r="A179"/>
     </row>
     <row r="180">
-      <c s="7" r="A180"/>
+      <c s="8" r="A180"/>
     </row>
     <row r="181">
-      <c s="7" r="A181"/>
+      <c s="8" r="A181"/>
     </row>
     <row r="182">
-      <c s="7" r="A182"/>
+      <c s="8" r="A182"/>
     </row>
     <row r="183">
-      <c s="7" r="A183"/>
+      <c s="8" r="A183"/>
     </row>
     <row r="184">
-      <c s="7" r="A184"/>
+      <c s="8" r="A184"/>
     </row>
     <row r="185">
-      <c s="7" r="A185"/>
+      <c s="8" r="A185"/>
     </row>
     <row r="186">
-      <c s="7" r="A186"/>
+      <c s="8" r="A186"/>
     </row>
     <row r="187">
-      <c s="7" r="A187"/>
+      <c s="8" r="A187"/>
     </row>
     <row r="188">
-      <c s="7" r="A188"/>
+      <c s="8" r="A188"/>
     </row>
     <row r="189">
-      <c s="7" r="A189"/>
+      <c s="8" r="A189"/>
     </row>
     <row r="190">
-      <c s="7" r="A190"/>
+      <c s="8" r="A190"/>
     </row>
     <row r="191">
-      <c s="7" r="A191"/>
+      <c s="8" r="A191"/>
     </row>
     <row r="192">
-      <c s="7" r="A192"/>
+      <c s="8" r="A192"/>
     </row>
     <row r="193">
-      <c s="7" r="A193"/>
+      <c s="8" r="A193"/>
     </row>
     <row r="194">
-      <c s="7" r="A194"/>
+      <c s="8" r="A194"/>
     </row>
     <row r="195">
-      <c s="7" r="A195"/>
+      <c s="8" r="A195"/>
     </row>
     <row r="196">
-      <c s="7" r="A196"/>
+      <c s="8" r="A196"/>
     </row>
     <row r="197">
-      <c s="7" r="A197"/>
+      <c s="8" r="A197"/>
     </row>
     <row r="198">
-      <c s="7" r="A198"/>
+      <c s="8" r="A198"/>
     </row>
     <row r="199">
-      <c s="7" r="A199"/>
+      <c s="8" r="A199"/>
     </row>
     <row r="200">
-      <c s="7" r="A200"/>
+      <c s="8" r="A200"/>
     </row>
     <row r="201">
-      <c s="7" r="A201"/>
+      <c s="8" r="A201"/>
     </row>
     <row r="202">
-      <c s="7" r="A202"/>
+      <c s="8" r="A202"/>
     </row>
     <row r="203">
-      <c s="7" r="A203"/>
+      <c s="8" r="A203"/>
     </row>
     <row r="204">
-      <c s="7" r="A204"/>
+      <c s="8" r="A204"/>
     </row>
     <row r="205">
-      <c s="7" r="A205"/>
+      <c s="8" r="A205"/>
     </row>
     <row r="206">
-      <c s="7" r="A206"/>
+      <c s="8" r="A206"/>
     </row>
     <row r="207">
-      <c s="7" r="A207"/>
+      <c s="8" r="A207"/>
     </row>
     <row r="208">
-      <c s="7" r="A208"/>
+      <c s="8" r="A208"/>
     </row>
     <row r="209">
-      <c s="7" r="A209"/>
+      <c s="8" r="A209"/>
     </row>
     <row r="210">
-      <c s="7" r="A210"/>
+      <c s="8" r="A210"/>
     </row>
     <row r="211">
-      <c s="7" r="A211"/>
+      <c s="8" r="A211"/>
     </row>
     <row r="212">
-      <c s="7" r="A212"/>
+      <c s="8" r="A212"/>
     </row>
     <row r="213">
-      <c s="7" r="A213"/>
+      <c s="8" r="A213"/>
     </row>
     <row r="214">
-      <c s="7" r="A214"/>
+      <c s="8" r="A214"/>
     </row>
     <row r="215">
-      <c s="7" r="A215"/>
+      <c s="8" r="A215"/>
     </row>
     <row r="216">
-      <c s="7" r="A216"/>
+      <c s="8" r="A216"/>
     </row>
     <row r="217">
-      <c s="7" r="A217"/>
+      <c s="8" r="A217"/>
     </row>
     <row r="218">
-      <c s="7" r="A218"/>
+      <c s="8" r="A218"/>
     </row>
     <row r="219">
-      <c s="7" r="A219"/>
+      <c s="8" r="A219"/>
     </row>
     <row r="220">
-      <c s="7" r="A220"/>
+      <c s="8" r="A220"/>
     </row>
     <row r="221">
-      <c s="7" r="A221"/>
+      <c s="8" r="A221"/>
     </row>
     <row r="222">
-      <c s="7" r="A222"/>
+      <c s="8" r="A222"/>
     </row>
     <row r="223">
-      <c s="7" r="A223"/>
+      <c s="8" r="A223"/>
     </row>
     <row r="224">
-      <c s="7" r="A224"/>
+      <c s="8" r="A224"/>
     </row>
     <row r="225">
-      <c s="7" r="A225"/>
+      <c s="8" r="A225"/>
     </row>
     <row r="226">
-      <c s="7" r="A226"/>
+      <c s="8" r="A226"/>
     </row>
     <row r="227">
-      <c s="7" r="A227"/>
+      <c s="8" r="A227"/>
     </row>
     <row r="228">
-      <c s="7" r="A228"/>
+      <c s="8" r="A228"/>
     </row>
     <row r="229">
-      <c s="7" r="A229"/>
+      <c s="8" r="A229"/>
     </row>
     <row r="230">
-      <c s="7" r="A230"/>
+      <c s="8" r="A230"/>
     </row>
     <row r="231">
-      <c s="7" r="A231"/>
+      <c s="8" r="A231"/>
     </row>
     <row r="232">
-      <c s="7" r="A232"/>
+      <c s="8" r="A232"/>
     </row>
     <row r="233">
-      <c s="7" r="A233"/>
+      <c s="8" r="A233"/>
     </row>
     <row r="234">
-      <c s="7" r="A234"/>
+      <c s="8" r="A234"/>
     </row>
     <row r="235">
-      <c s="7" r="A235"/>
+      <c s="8" r="A235"/>
     </row>
     <row r="236">
-      <c s="7" r="A236"/>
+      <c s="8" r="A236"/>
     </row>
     <row r="237">
-      <c s="7" r="A237"/>
+      <c s="8" r="A237"/>
     </row>
     <row r="238">
-      <c s="7" r="A238"/>
+      <c s="8" r="A238"/>
     </row>
     <row r="239">
-      <c s="7" r="A239"/>
+      <c s="8" r="A239"/>
     </row>
     <row r="240">
-      <c s="7" r="A240"/>
+      <c s="8" r="A240"/>
     </row>
     <row r="241">
-      <c s="7" r="A241"/>
+      <c s="8" r="A241"/>
     </row>
     <row r="242">
-      <c s="7" r="A242"/>
+      <c s="8" r="A242"/>
     </row>
     <row r="243">
-      <c s="7" r="A243"/>
+      <c s="8" r="A243"/>
     </row>
     <row r="244">
-      <c s="7" r="A244"/>
+      <c s="8" r="A244"/>
     </row>
     <row r="245">
-      <c s="7" r="A245"/>
+      <c s="8" r="A245"/>
     </row>
     <row r="246">
-      <c s="7" r="A246"/>
+      <c s="8" r="A246"/>
     </row>
     <row r="247">
-      <c s="7" r="A247"/>
+      <c s="8" r="A247"/>
     </row>
     <row r="248">
-      <c s="7" r="A248"/>
+      <c s="8" r="A248"/>
     </row>
     <row r="249">
-      <c s="7" r="A249"/>
+      <c s="8" r="A249"/>
     </row>
     <row r="250">
-      <c s="7" r="A250"/>
+      <c s="8" r="A250"/>
     </row>
     <row r="251">
-      <c s="7" r="A251"/>
+      <c s="8" r="A251"/>
     </row>
     <row r="252">
-      <c s="7" r="A252"/>
+      <c s="8" r="A252"/>
     </row>
     <row r="253">
-      <c s="7" r="A253"/>
+      <c s="8" r="A253"/>
     </row>
     <row r="254">
-      <c s="7" r="A254"/>
+      <c s="8" r="A254"/>
     </row>
     <row r="255">
-      <c s="7" r="A255"/>
+      <c s="8" r="A255"/>
     </row>
     <row r="256">
-      <c s="7" r="A256"/>
+      <c s="8" r="A256"/>
     </row>
     <row r="257">
-      <c s="7" r="A257"/>
+      <c s="8" r="A257"/>
     </row>
     <row r="258">
-      <c s="7" r="A258"/>
+      <c s="8" r="A258"/>
     </row>
     <row r="259">
-      <c s="7" r="A259"/>
+      <c s="8" r="A259"/>
     </row>
     <row r="260">
-      <c s="7" r="A260"/>
+      <c s="8" r="A260"/>
     </row>
     <row r="261">
-      <c s="7" r="A261"/>
+      <c s="8" r="A261"/>
     </row>
     <row r="262">
-      <c s="7" r="A262"/>
+      <c s="8" r="A262"/>
     </row>
     <row r="263">
-      <c s="7" r="A263"/>
+      <c s="8" r="A263"/>
     </row>
     <row r="264">
-      <c s="7" r="A264"/>
+      <c s="8" r="A264"/>
     </row>
     <row r="265">
-      <c s="7" r="A265"/>
+      <c s="8" r="A265"/>
     </row>
     <row r="266">
-      <c s="7" r="A266"/>
+      <c s="8" r="A266"/>
     </row>
     <row r="267">
-      <c s="7" r="A267"/>
+      <c s="8" r="A267"/>
     </row>
     <row r="268">
-      <c s="7" r="A268"/>
+      <c s="8" r="A268"/>
     </row>
     <row r="269">
-      <c s="7" r="A269"/>
+      <c s="8" r="A269"/>
     </row>
     <row r="270">
-      <c s="7" r="A270"/>
+      <c s="8" r="A270"/>
     </row>
     <row r="271">
-      <c s="7" r="A271"/>
+      <c s="8" r="A271"/>
     </row>
     <row r="272">
-      <c s="7" r="A272"/>
+      <c s="8" r="A272"/>
     </row>
     <row r="273">
-      <c s="7" r="A273"/>
+      <c s="8" r="A273"/>
     </row>
     <row r="274">
-      <c s="7" r="A274"/>
+      <c s="8" r="A274"/>
     </row>
     <row r="275">
-      <c s="7" r="A275"/>
+      <c s="8" r="A275"/>
     </row>
     <row r="276">
-      <c s="7" r="A276"/>
+      <c s="8" r="A276"/>
     </row>
     <row r="277">
-      <c s="7" r="A277"/>
+      <c s="8" r="A277"/>
     </row>
     <row r="278">
-      <c s="7" r="A278"/>
+      <c s="8" r="A278"/>
     </row>
     <row r="279">
-      <c s="7" r="A279"/>
+      <c s="8" r="A279"/>
     </row>
     <row r="280">
-      <c s="7" r="A280"/>
+      <c s="8" r="A280"/>
     </row>
     <row r="281">
-      <c s="7" r="A281"/>
+      <c s="8" r="A281"/>
     </row>
     <row r="282">
-      <c s="7" r="A282"/>
+      <c s="8" r="A282"/>
     </row>
     <row r="283">
-      <c s="7" r="A283"/>
+      <c s="8" r="A283"/>
     </row>
     <row r="284">
-      <c s="7" r="A284"/>
+      <c s="8" r="A284"/>
     </row>
     <row r="285">
-      <c s="7" r="A285"/>
+      <c s="8" r="A285"/>
     </row>
     <row r="286">
-      <c s="7" r="A286"/>
+      <c s="8" r="A286"/>
     </row>
     <row r="287">
-      <c s="7" r="A287"/>
+      <c s="8" r="A287"/>
     </row>
     <row r="288">
-      <c s="7" r="A288"/>
+      <c s="8" r="A288"/>
     </row>
     <row r="289">
-      <c s="7" r="A289"/>
+      <c s="8" r="A289"/>
     </row>
     <row r="290">
-      <c s="7" r="A290"/>
+      <c s="8" r="A290"/>
     </row>
     <row r="291">
-      <c s="7" r="A291"/>
+      <c s="8" r="A291"/>
     </row>
     <row r="292">
-      <c s="7" r="A292"/>
+      <c s="8" r="A292"/>
     </row>
     <row r="293">
-      <c s="7" r="A293"/>
+      <c s="8" r="A293"/>
     </row>
     <row r="294">
-      <c s="7" r="A294"/>
+      <c s="8" r="A294"/>
     </row>
     <row r="295">
-      <c s="7" r="A295"/>
+      <c s="8" r="A295"/>
     </row>
     <row r="296">
-      <c s="7" r="A296"/>
+      <c s="8" r="A296"/>
     </row>
     <row r="297">
-      <c s="7" r="A297"/>
+      <c s="8" r="A297"/>
     </row>
     <row r="298">
-      <c s="7" r="A298"/>
+      <c s="8" r="A298"/>
     </row>
     <row r="299">
-      <c s="7" r="A299"/>
+      <c s="8" r="A299"/>
     </row>
     <row r="300">
-      <c s="7" r="A300"/>
+      <c s="8" r="A300"/>
     </row>
     <row r="301">
-      <c s="7" r="A301"/>
+      <c s="8" r="A301"/>
     </row>
     <row r="302">
-      <c s="7" r="A302"/>
+      <c s="8" r="A302"/>
     </row>
     <row r="303">
-      <c s="7" r="A303"/>
+      <c s="8" r="A303"/>
     </row>
     <row r="304">
-      <c s="7" r="A304"/>
+      <c s="8" r="A304"/>
     </row>
     <row r="305">
-      <c s="7" r="A305"/>
+      <c s="8" r="A305"/>
     </row>
     <row r="306">
-      <c s="7" r="A306"/>
+      <c s="8" r="A306"/>
     </row>
     <row r="307">
-      <c s="7" r="A307"/>
+      <c s="8" r="A307"/>
     </row>
     <row r="308">
-      <c s="7" r="A308"/>
+      <c s="8" r="A308"/>
     </row>
     <row r="309">
-      <c s="7" r="A309"/>
+      <c s="8" r="A309"/>
     </row>
     <row r="310">
-      <c s="7" r="A310"/>
+      <c s="8" r="A310"/>
     </row>
     <row r="311">
-      <c s="7" r="A311"/>
+      <c s="8" r="A311"/>
     </row>
     <row r="312">
-      <c s="7" r="A312"/>
+      <c s="8" r="A312"/>
     </row>
     <row r="313">
-      <c s="7" r="A313"/>
+      <c s="8" r="A313"/>
     </row>
     <row r="314">
-      <c s="7" r="A314"/>
+      <c s="8" r="A314"/>
     </row>
     <row r="315">
-      <c s="7" r="A315"/>
+      <c s="8" r="A315"/>
     </row>
     <row r="316">
-      <c s="7" r="A316"/>
+      <c s="8" r="A316"/>
     </row>
     <row r="317">
-      <c s="7" r="A317"/>
+      <c s="8" r="A317"/>
     </row>
     <row r="318">
-      <c s="7" r="A318"/>
+      <c s="8" r="A318"/>
     </row>
     <row r="319">
-      <c s="7" r="A319"/>
+      <c s="8" r="A319"/>
     </row>
     <row r="320">
-      <c s="7" r="A320"/>
+      <c s="8" r="A320"/>
     </row>
     <row r="321">
-      <c s="7" r="A321"/>
+      <c s="8" r="A321"/>
     </row>
     <row r="322">
-      <c s="7" r="A322"/>
+      <c s="8" r="A322"/>
     </row>
     <row r="323">
-      <c s="7" r="A323"/>
+      <c s="8" r="A323"/>
     </row>
     <row r="324">
-      <c s="7" r="A324"/>
+      <c s="8" r="A324"/>
     </row>
     <row r="325">
-      <c s="7" r="A325"/>
+      <c s="8" r="A325"/>
     </row>
     <row r="326">
-      <c s="7" r="A326"/>
+      <c s="8" r="A326"/>
     </row>
     <row r="327">
-      <c s="7" r="A327"/>
+      <c s="8" r="A327"/>
     </row>
     <row r="328">
-      <c s="7" r="A328"/>
+      <c s="8" r="A328"/>
     </row>
     <row r="329">
-      <c s="7" r="A329"/>
+      <c s="8" r="A329"/>
     </row>
     <row r="330">
-      <c s="7" r="A330"/>
+      <c s="8" r="A330"/>
     </row>
     <row r="331">
-      <c s="7" r="A331"/>
+      <c s="8" r="A331"/>
     </row>
     <row r="332">
-      <c s="7" r="A332"/>
+      <c s="8" r="A332"/>
     </row>
     <row r="333">
-      <c s="7" r="A333"/>
+      <c s="8" r="A333"/>
     </row>
     <row r="334">
-      <c s="7" r="A334"/>
+      <c s="8" r="A334"/>
     </row>
     <row r="335">
-      <c s="7" r="A335"/>
+      <c s="8" r="A335"/>
     </row>
     <row r="336">
-      <c s="7" r="A336"/>
+      <c s="8" r="A336"/>
     </row>
     <row r="337">
-      <c s="7" r="A337"/>
+      <c s="8" r="A337"/>
     </row>
     <row r="338">
-      <c s="7" r="A338"/>
+      <c s="8" r="A338"/>
     </row>
     <row r="339">
-      <c s="7" r="A339"/>
+      <c s="8" r="A339"/>
     </row>
     <row r="340">
-      <c s="7" r="A340"/>
+      <c s="8" r="A340"/>
     </row>
     <row r="341">
-      <c s="7" r="A341"/>
+      <c s="8" r="A341"/>
     </row>
     <row r="342">
-      <c s="7" r="A342"/>
+      <c s="8" r="A342"/>
     </row>
     <row r="343">
-      <c s="7" r="A343"/>
+      <c s="8" r="A343"/>
     </row>
     <row r="344">
-      <c s="7" r="A344"/>
+      <c s="8" r="A344"/>
     </row>
     <row r="345">
-      <c s="7" r="A345"/>
+      <c s="8" r="A345"/>
     </row>
     <row r="346">
-      <c s="7" r="A346"/>
+      <c s="8" r="A346"/>
     </row>
     <row r="347">
-      <c s="7" r="A347"/>
+      <c s="8" r="A347"/>
     </row>
     <row r="348">
-      <c s="7" r="A348"/>
+      <c s="8" r="A348"/>
     </row>
     <row r="349">
-      <c s="7" r="A349"/>
+      <c s="8" r="A349"/>
     </row>
     <row r="350">
-      <c s="7" r="A350"/>
+      <c s="8" r="A350"/>
     </row>
     <row r="351">
-      <c s="7" r="A351"/>
+      <c s="8" r="A351"/>
     </row>
     <row r="352">
-      <c s="7" r="A352"/>
+      <c s="8" r="A352"/>
     </row>
     <row r="353">
-      <c s="7" r="A353"/>
+      <c s="8" r="A353"/>
     </row>
     <row r="354">
-      <c s="7" r="A354"/>
+      <c s="8" r="A354"/>
     </row>
     <row r="355">
-      <c s="7" r="A355"/>
+      <c s="8" r="A355"/>
     </row>
     <row r="356">
-      <c s="7" r="A356"/>
+      <c s="8" r="A356"/>
     </row>
     <row r="357">
-      <c s="7" r="A357"/>
+      <c s="8" r="A357"/>
     </row>
     <row r="358">
-      <c s="7" r="A358"/>
+      <c s="8" r="A358"/>
     </row>
     <row r="359">
-      <c s="7" r="A359"/>
+      <c s="8" r="A359"/>
     </row>
     <row r="360">
-      <c s="7" r="A360"/>
+      <c s="8" r="A360"/>
     </row>
     <row r="361">
-      <c s="7" r="A361"/>
+      <c s="8" r="A361"/>
     </row>
     <row r="362">
-      <c s="7" r="A362"/>
+      <c s="8" r="A362"/>
     </row>
     <row r="363">
-      <c s="7" r="A363"/>
+      <c s="8" r="A363"/>
     </row>
     <row r="364">
-      <c s="7" r="A364"/>
+      <c s="8" r="A364"/>
     </row>
     <row r="365">
-      <c s="7" r="A365"/>
+      <c s="8" r="A365"/>
     </row>
     <row r="366">
-      <c s="7" r="A366"/>
+      <c s="8" r="A366"/>
     </row>
     <row r="367">
-      <c s="7" r="A367"/>
+      <c s="8" r="A367"/>
     </row>
     <row r="368">
-      <c s="7" r="A368"/>
+      <c s="8" r="A368"/>
     </row>
     <row r="369">
-      <c s="7" r="A369"/>
+      <c s="8" r="A369"/>
     </row>
     <row r="370">
-      <c s="7" r="A370"/>
+      <c s="8" r="A370"/>
     </row>
     <row r="371">
-      <c s="7" r="A371"/>
+      <c s="8" r="A371"/>
     </row>
     <row r="372">
-      <c s="7" r="A372"/>
+      <c s="8" r="A372"/>
     </row>
     <row r="373">
-      <c s="7" r="A373"/>
+      <c s="8" r="A373"/>
     </row>
     <row r="374">
-      <c s="7" r="A374"/>
+      <c s="8" r="A374"/>
     </row>
     <row r="375">
-      <c s="7" r="A375"/>
+      <c s="8" r="A375"/>
     </row>
     <row r="376">
-      <c s="7" r="A376"/>
+      <c s="8" r="A376"/>
     </row>
     <row r="377">
-      <c s="7" r="A377"/>
+      <c s="8" r="A377"/>
     </row>
     <row r="378">
-      <c s="7" r="A378"/>
+      <c s="8" r="A378"/>
     </row>
     <row r="379">
-      <c s="7" r="A379"/>
+      <c s="8" r="A379"/>
     </row>
     <row r="380">
-      <c s="7" r="A380"/>
+      <c s="8" r="A380"/>
     </row>
     <row r="381">
-      <c s="7" r="A381"/>
+      <c s="8" r="A381"/>
     </row>
     <row r="382">
-      <c s="7" r="A382"/>
+      <c s="8" r="A382"/>
     </row>
     <row r="383">
-      <c s="7" r="A383"/>
+      <c s="8" r="A383"/>
     </row>
     <row r="384">
-      <c s="7" r="A384"/>
+      <c s="8" r="A384"/>
     </row>
     <row r="385">
-      <c s="7" r="A385"/>
+      <c s="8" r="A385"/>
     </row>
     <row r="386">
-      <c s="7" r="A386"/>
+      <c s="8" r="A386"/>
     </row>
     <row r="387">
-      <c s="7" r="A387"/>
+      <c s="8" r="A387"/>
     </row>
     <row r="388">
-      <c s="7" r="A388"/>
+      <c s="8" r="A388"/>
     </row>
     <row r="389">
-      <c s="7" r="A389"/>
+      <c s="8" r="A389"/>
     </row>
     <row r="390">
-      <c s="7" r="A390"/>
+      <c s="8" r="A390"/>
     </row>
     <row r="391">
-      <c s="7" r="A391"/>
+      <c s="8" r="A391"/>
     </row>
     <row r="392">
-      <c s="7" r="A392"/>
+      <c s="8" r="A392"/>
     </row>
     <row r="393">
-      <c s="7" r="A393"/>
+      <c s="8" r="A393"/>
     </row>
     <row r="394">
-      <c s="7" r="A394"/>
+      <c s="8" r="A394"/>
     </row>
     <row r="395">
-      <c s="7" r="A395"/>
+      <c s="8" r="A395"/>
     </row>
     <row r="396">
-      <c s="7" r="A396"/>
+      <c s="8" r="A396"/>
     </row>
     <row r="397">
-      <c s="7" r="A397"/>
+      <c s="8" r="A397"/>
     </row>
     <row r="398">
-      <c s="7" r="A398"/>
+      <c s="8" r="A398"/>
     </row>
     <row r="399">
-      <c s="7" r="A399"/>
+      <c s="8" r="A399"/>
     </row>
     <row r="400">
-      <c s="7" r="A400"/>
+      <c s="8" r="A400"/>
     </row>
     <row r="401">
-      <c s="7" r="A401"/>
+      <c s="8" r="A401"/>
     </row>
     <row r="402">
-      <c s="7" r="A402"/>
+      <c s="8" r="A402"/>
     </row>
     <row r="403">
-      <c s="7" r="A403"/>
+      <c s="8" r="A403"/>
     </row>
     <row r="404">
-      <c s="7" r="A404"/>
+      <c s="8" r="A404"/>
     </row>
     <row r="405">
-      <c s="7" r="A405"/>
+      <c s="8" r="A405"/>
     </row>
     <row r="406">
-      <c s="7" r="A406"/>
+      <c s="8" r="A406"/>
     </row>
     <row r="407">
-      <c s="7" r="A407"/>
+      <c s="8" r="A407"/>
     </row>
     <row r="408">
-      <c s="7" r="A408"/>
+      <c s="8" r="A408"/>
     </row>
     <row r="409">
-      <c s="7" r="A409"/>
+      <c s="8" r="A409"/>
     </row>
     <row r="410">
-      <c s="7" r="A410"/>
+      <c s="8" r="A410"/>
     </row>
     <row r="411">
-      <c s="7" r="A411"/>
+      <c s="8" r="A411"/>
     </row>
     <row r="412">
-      <c s="7" r="A412"/>
+      <c s="8" r="A412"/>
     </row>
     <row r="413">
-      <c s="7" r="A413"/>
+      <c s="8" r="A413"/>
     </row>
     <row r="414">
-      <c s="7" r="A414"/>
+      <c s="8" r="A414"/>
     </row>
     <row r="415">
-      <c s="7" r="A415"/>
+      <c s="8" r="A415"/>
     </row>
     <row r="416">
-      <c s="7" r="A416"/>
+      <c s="8" r="A416"/>
     </row>
     <row r="417">
-      <c s="7" r="A417"/>
+      <c s="8" r="A417"/>
     </row>
     <row r="418">
-      <c s="7" r="A418"/>
+      <c s="8" r="A418"/>
     </row>
     <row r="419">
-      <c s="7" r="A419"/>
+      <c s="8" r="A419"/>
     </row>
     <row r="420">
-      <c s="7" r="A420"/>
+      <c s="8" r="A420"/>
     </row>
     <row r="421">
-      <c s="7" r="A421"/>
+      <c s="8" r="A421"/>
     </row>
     <row r="422">
-      <c s="7" r="A422"/>
+      <c s="8" r="A422"/>
     </row>
     <row r="423">
-      <c s="7" r="A423"/>
+      <c s="8" r="A423"/>
     </row>
     <row r="424">
-      <c s="7" r="A424"/>
+      <c s="8" r="A424"/>
     </row>
     <row r="425">
-      <c s="7" r="A425"/>
+      <c s="8" r="A425"/>
     </row>
     <row r="426">
-      <c s="7" r="A426"/>
+      <c s="8" r="A426"/>
     </row>
     <row r="427">
-      <c s="7" r="A427"/>
+      <c s="8" r="A427"/>
     </row>
     <row r="428">
-      <c s="7" r="A428"/>
+      <c s="8" r="A428"/>
     </row>
     <row r="429">
-      <c s="7" r="A429"/>
+      <c s="8" r="A429"/>
     </row>
     <row r="430">
-      <c s="7" r="A430"/>
+      <c s="8" r="A430"/>
     </row>
     <row r="431">
-      <c s="7" r="A431"/>
+      <c s="8" r="A431"/>
     </row>
     <row r="432">
-      <c s="7" r="A432"/>
+      <c s="8" r="A432"/>
     </row>
     <row r="433">
-      <c s="7" r="A433"/>
+      <c s="8" r="A433"/>
     </row>
     <row r="434">
-      <c s="7" r="A434"/>
+      <c s="8" r="A434"/>
     </row>
     <row r="435">
-      <c s="7" r="A435"/>
+      <c s="8" r="A435"/>
     </row>
     <row r="436">
-      <c s="7" r="A436"/>
+      <c s="8" r="A436"/>
     </row>
     <row r="437">
-      <c s="7" r="A437"/>
+      <c s="8" r="A437"/>
     </row>
     <row r="438">
-      <c s="7" r="A438"/>
+      <c s="8" r="A438"/>
     </row>
     <row r="439">
-      <c s="7" r="A439"/>
+      <c s="8" r="A439"/>
     </row>
     <row r="440">
-      <c s="7" r="A440"/>
+      <c s="8" r="A440"/>
     </row>
     <row r="441">
-      <c s="7" r="A441"/>
+      <c s="8" r="A441"/>
     </row>
     <row r="442">
-      <c s="7" r="A442"/>
+      <c s="8" r="A442"/>
     </row>
     <row r="443">
-      <c s="7" r="A443"/>
+      <c s="8" r="A443"/>
     </row>
     <row r="444">
-      <c s="7" r="A444"/>
+      <c s="8" r="A444"/>
     </row>
     <row r="445">
-      <c s="7" r="A445"/>
+      <c s="8" r="A445"/>
     </row>
     <row r="446">
-      <c s="7" r="A446"/>
+      <c s="8" r="A446"/>
     </row>
     <row r="447">
-      <c s="7" r="A447"/>
+      <c s="8" r="A447"/>
     </row>
     <row r="448">
-      <c s="7" r="A448"/>
+      <c s="8" r="A448"/>
     </row>
     <row r="449">
-      <c s="7" r="A449"/>
+      <c s="8" r="A449"/>
     </row>
     <row r="450">
-      <c s="7" r="A450"/>
+      <c s="8" r="A450"/>
     </row>
     <row r="451">
-      <c s="7" r="A451"/>
+      <c s="8" r="A451"/>
     </row>
     <row r="452">
-      <c s="7" r="A452"/>
+      <c s="8" r="A452"/>
     </row>
     <row r="453">
-      <c s="7" r="A453"/>
+      <c s="8" r="A453"/>
     </row>
     <row r="454">
-      <c s="7" r="A454"/>
+      <c s="8" r="A454"/>
     </row>
     <row r="455">
-      <c s="7" r="A455"/>
+      <c s="8" r="A455"/>
     </row>
     <row r="456">
-      <c s="7" r="A456"/>
+      <c s="8" r="A456"/>
     </row>
     <row r="457">
-      <c s="7" r="A457"/>
+      <c s="8" r="A457"/>
     </row>
     <row r="458">
-      <c s="7" r="A458"/>
+      <c s="8" r="A458"/>
     </row>
     <row r="459">
-      <c s="7" r="A459"/>
+      <c s="8" r="A459"/>
     </row>
     <row r="460">
-      <c s="7" r="A460"/>
+      <c s="8" r="A460"/>
     </row>
     <row r="461">
-      <c s="7" r="A461"/>
+      <c s="8" r="A461"/>
     </row>
     <row r="462">
-      <c s="7" r="A462"/>
+      <c s="8" r="A462"/>
     </row>
     <row r="463">
-      <c s="7" r="A463"/>
+      <c s="8" r="A463"/>
     </row>
     <row r="464">
-      <c s="7" r="A464"/>
+      <c s="8" r="A464"/>
     </row>
     <row r="465">
-      <c s="7" r="A465"/>
+      <c s="8" r="A465"/>
     </row>
     <row r="466">
-      <c s="7" r="A466"/>
+      <c s="8" r="A466"/>
     </row>
     <row r="467">
-      <c s="7" r="A467"/>
+      <c s="8" r="A467"/>
     </row>
     <row r="468">
-      <c s="7" r="A468"/>
+      <c s="8" r="A468"/>
     </row>
     <row r="469">
-      <c s="7" r="A469"/>
+      <c s="8" r="A469"/>
     </row>
     <row r="470">
-      <c s="7" r="A470"/>
+      <c s="8" r="A470"/>
     </row>
     <row r="471">
-      <c s="7" r="A471"/>
+      <c s="8" r="A471"/>
     </row>
     <row r="472">
-      <c s="7" r="A472"/>
+      <c s="8" r="A472"/>
     </row>
     <row r="473">
-      <c s="7" r="A473"/>
+      <c s="8" r="A473"/>
     </row>
     <row r="474">
-      <c s="7" r="A474"/>
+      <c s="8" r="A474"/>
     </row>
     <row r="475">
-      <c s="7" r="A475"/>
+      <c s="8" r="A475"/>
     </row>
     <row r="476">
-      <c s="7" r="A476"/>
+      <c s="8" r="A476"/>
     </row>
     <row r="477">
-      <c s="7" r="A477"/>
+      <c s="8" r="A477"/>
     </row>
     <row r="478">
-      <c s="7" r="A478"/>
+      <c s="8" r="A478"/>
     </row>
     <row r="479">
-      <c s="7" r="A479"/>
+      <c s="8" r="A479"/>
     </row>
     <row r="480">
-      <c s="7" r="A480"/>
+      <c s="8" r="A480"/>
     </row>
     <row r="481">
-      <c s="7" r="A481"/>
+      <c s="8" r="A481"/>
     </row>
     <row r="482">
-      <c s="7" r="A482"/>
+      <c s="8" r="A482"/>
     </row>
     <row r="483">
-      <c s="7" r="A483"/>
+      <c s="8" r="A483"/>
     </row>
     <row r="484">
-      <c s="7" r="A484"/>
+      <c s="8" r="A484"/>
     </row>
     <row r="485">
-      <c s="7" r="A485"/>
+      <c s="8" r="A485"/>
     </row>
     <row r="486">
-      <c s="7" r="A486"/>
+      <c s="8" r="A486"/>
     </row>
     <row r="487">
-      <c s="7" r="A487"/>
+      <c s="8" r="A487"/>
     </row>
     <row r="488">
-      <c s="7" r="A488"/>
+      <c s="8" r="A488"/>
     </row>
     <row r="489">
-      <c s="7" r="A489"/>
+      <c s="8" r="A489"/>
     </row>
     <row r="490">
-      <c s="7" r="A490"/>
+      <c s="8" r="A490"/>
     </row>
     <row r="491">
-      <c s="7" r="A491"/>
+      <c s="8" r="A491"/>
     </row>
     <row r="492">
-      <c s="7" r="A492"/>
+      <c s="8" r="A492"/>
     </row>
     <row r="493">
-      <c s="7" r="A493"/>
+      <c s="8" r="A493"/>
     </row>
     <row r="494">
-      <c s="7" r="A494"/>
+      <c s="8" r="A494"/>
     </row>
     <row r="495">
-      <c s="7" r="A495"/>
+      <c s="8" r="A495"/>
     </row>
     <row r="496">
-      <c s="7" r="A496"/>
+      <c s="8" r="A496"/>
     </row>
     <row r="497">
-      <c s="7" r="A497"/>
+      <c s="8" r="A497"/>
     </row>
     <row r="498">
-      <c s="7" r="A498"/>
+      <c s="8" r="A498"/>
     </row>
     <row r="499">
-      <c s="7" r="A499"/>
+      <c s="8" r="A499"/>
     </row>
     <row r="500">
-      <c s="7" r="A500"/>
+      <c s="8" r="A500"/>
     </row>
     <row r="501">
-      <c s="7" r="A501"/>
+      <c s="8" r="A501"/>
     </row>
     <row r="502">
-      <c s="7" r="A502"/>
+      <c s="8" r="A502"/>
     </row>
     <row r="503">
-      <c s="7" r="A503"/>
+      <c s="8" r="A503"/>
     </row>
     <row r="504">
-      <c s="7" r="A504"/>
+      <c s="8" r="A504"/>
     </row>
     <row r="505">
-      <c s="7" r="A505"/>
+      <c s="8" r="A505"/>
     </row>
     <row r="506">
-      <c s="7" r="A506"/>
+      <c s="8" r="A506"/>
     </row>
     <row r="507">
-      <c s="7" r="A507"/>
+      <c s="8" r="A507"/>
     </row>
     <row r="508">
-      <c s="7" r="A508"/>
+      <c s="8" r="A508"/>
     </row>
     <row r="509">
-      <c s="7" r="A509"/>
+      <c s="8" r="A509"/>
     </row>
     <row r="510">
-      <c s="7" r="A510"/>
+      <c s="8" r="A510"/>
     </row>
     <row r="511">
-      <c s="7" r="A511"/>
+      <c s="8" r="A511"/>
     </row>
     <row r="512">
-      <c s="7" r="A512"/>
+      <c s="8" r="A512"/>
     </row>
     <row r="513">
-      <c s="7" r="A513"/>
+      <c s="8" r="A513"/>
     </row>
     <row r="514">
-      <c s="7" r="A514"/>
+      <c s="8" r="A514"/>
     </row>
     <row r="515">
-      <c s="7" r="A515"/>
+      <c s="8" r="A515"/>
     </row>
     <row r="516">
-      <c s="7" r="A516"/>
+      <c s="8" r="A516"/>
     </row>
     <row r="517">
-      <c s="7" r="A517"/>
+      <c s="8" r="A517"/>
     </row>
     <row r="518">
-      <c s="7" r="A518"/>
+      <c s="8" r="A518"/>
     </row>
     <row r="519">
-      <c s="7" r="A519"/>
+      <c s="8" r="A519"/>
     </row>
     <row r="520">
-      <c s="7" r="A520"/>
+      <c s="8" r="A520"/>
     </row>
     <row r="521">
-      <c s="7" r="A521"/>
+      <c s="8" r="A521"/>
     </row>
     <row r="522">
-      <c s="7" r="A522"/>
+      <c s="8" r="A522"/>
     </row>
     <row r="523">
-      <c s="7" r="A523"/>
+      <c s="8" r="A523"/>
     </row>
     <row r="524">
-      <c s="7" r="A524"/>
+      <c s="8" r="A524"/>
     </row>
     <row r="525">
-      <c s="7" r="A525"/>
+      <c s="8" r="A525"/>
     </row>
     <row r="526">
-      <c s="7" r="A526"/>
+      <c s="8" r="A526"/>
     </row>
     <row r="527">
-      <c s="7" r="A527"/>
+      <c s="8" r="A527"/>
     </row>
     <row r="528">
-      <c s="7" r="A528"/>
+      <c s="8" r="A528"/>
     </row>
     <row r="529">
-      <c s="7" r="A529"/>
+      <c s="8" r="A529"/>
     </row>
     <row r="530">
-      <c s="7" r="A530"/>
+      <c s="8" r="A530"/>
     </row>
     <row r="531">
-      <c s="7" r="A531"/>
+      <c s="8" r="A531"/>
     </row>
     <row r="532">
-      <c s="7" r="A532"/>
+      <c s="8" r="A532"/>
     </row>
     <row r="533">
-      <c s="7" r="A533"/>
+      <c s="8" r="A533"/>
     </row>
     <row r="534">
-      <c s="7" r="A534"/>
+      <c s="8" r="A534"/>
     </row>
     <row r="535">
-      <c s="7" r="A535"/>
+      <c s="8" r="A535"/>
     </row>
     <row r="536">
-      <c s="7" r="A536"/>
+      <c s="8" r="A536"/>
     </row>
     <row r="537">
-      <c s="7" r="A537"/>
+      <c s="8" r="A537"/>
     </row>
     <row r="538">
-      <c s="7" r="A538"/>
+      <c s="8" r="A538"/>
     </row>
     <row r="539">
-      <c s="7" r="A539"/>
+      <c s="8" r="A539"/>
     </row>
     <row r="540">
-      <c s="7" r="A540"/>
+      <c s="8" r="A540"/>
     </row>
     <row r="541">
-      <c s="7" r="A541"/>
+      <c s="8" r="A541"/>
     </row>
     <row r="542">
-      <c s="7" r="A542"/>
+      <c s="8" r="A542"/>
     </row>
     <row r="543">
-      <c s="7" r="A543"/>
+      <c s="8" r="A543"/>
     </row>
     <row r="544">
-      <c s="7" r="A544"/>
+      <c s="8" r="A544"/>
     </row>
     <row r="545">
-      <c s="7" r="A545"/>
+      <c s="8" r="A545"/>
     </row>
     <row r="546">
-      <c s="7" r="A546"/>
+      <c s="8" r="A546"/>
     </row>
     <row r="547">
-      <c s="7" r="A547"/>
+      <c s="8" r="A547"/>
     </row>
     <row r="548">
-      <c s="7" r="A548"/>
+      <c s="8" r="A548"/>
     </row>
     <row r="549">
-      <c s="7" r="A549"/>
+      <c s="8" r="A549"/>
     </row>
     <row r="550">
-      <c s="7" r="A550"/>
+      <c s="8" r="A550"/>
     </row>
     <row r="551">
-      <c s="7" r="A551"/>
+      <c s="8" r="A551"/>
     </row>
     <row r="552">
-      <c s="7" r="A552"/>
+      <c s="8" r="A552"/>
     </row>
     <row r="553">
-      <c s="7" r="A553"/>
+      <c s="8" r="A553"/>
     </row>
     <row r="554">
-      <c s="7" r="A554"/>
+      <c s="8" r="A554"/>
     </row>
     <row r="555">
-      <c s="7" r="A555"/>
+      <c s="8" r="A555"/>
     </row>
     <row r="556">
-      <c s="7" r="A556"/>
+      <c s="8" r="A556"/>
     </row>
     <row r="557">
-      <c s="7" r="A557"/>
+      <c s="8" r="A557"/>
     </row>
     <row r="558">
-      <c s="7" r="A558"/>
+      <c s="8" r="A558"/>
     </row>
     <row r="559">
-      <c s="7" r="A559"/>
+      <c s="8" r="A559"/>
     </row>
     <row r="560">
-      <c s="7" r="A560"/>
+      <c s="8" r="A560"/>
     </row>
     <row r="561">
-      <c s="7" r="A561"/>
+      <c s="8" r="A561"/>
     </row>
     <row r="562">
-      <c s="7" r="A562"/>
+      <c s="8" r="A562"/>
     </row>
     <row r="563">
-      <c s="7" r="A563"/>
+      <c s="8" r="A563"/>
     </row>
     <row r="564">
-      <c s="7" r="A564"/>
+      <c s="8" r="A564"/>
     </row>
     <row r="565">
-      <c s="7" r="A565"/>
+      <c s="8" r="A565"/>
     </row>
     <row r="566">
-      <c s="7" r="A566"/>
+      <c s="8" r="A566"/>
     </row>
     <row r="567">
-      <c s="7" r="A567"/>
+      <c s="8" r="A567"/>
     </row>
     <row r="568">
-      <c s="7" r="A568"/>
+      <c s="8" r="A568"/>
     </row>
     <row r="569">
-      <c s="7" r="A569"/>
+      <c s="8" r="A569"/>
     </row>
     <row r="570">
-      <c s="7" r="A570"/>
+      <c s="8" r="A570"/>
     </row>
     <row r="571">
-      <c s="7" r="A571"/>
+      <c s="8" r="A571"/>
     </row>
     <row r="572">
-      <c s="7" r="A572"/>
+      <c s="8" r="A572"/>
     </row>
     <row r="573">
-      <c s="7" r="A573"/>
+      <c s="8" r="A573"/>
     </row>
     <row r="574">
-      <c s="7" r="A574"/>
+      <c s="8" r="A574"/>
     </row>
     <row r="575">
-      <c s="7" r="A575"/>
+      <c s="8" r="A575"/>
     </row>
     <row r="576">
-      <c s="7" r="A576"/>
+      <c s="8" r="A576"/>
     </row>
     <row r="577">
-      <c s="7" r="A577"/>
+      <c s="8" r="A577"/>
     </row>
     <row r="578">
-      <c s="7" r="A578"/>
+      <c s="8" r="A578"/>
     </row>
     <row r="579">
-      <c s="7" r="A579"/>
+      <c s="8" r="A579"/>
     </row>
     <row r="580">
-      <c s="7" r="A580"/>
+      <c s="8" r="A580"/>
     </row>
     <row r="581">
-      <c s="7" r="A581"/>
+      <c s="8" r="A581"/>
     </row>
     <row r="582">
-      <c s="7" r="A582"/>
+      <c s="8" r="A582"/>
     </row>
     <row r="583">
-      <c s="7" r="A583"/>
+      <c s="8" r="A583"/>
     </row>
     <row r="584">
-      <c s="7" r="A584"/>
+      <c s="8" r="A584"/>
     </row>
     <row r="585">
-      <c s="7" r="A585"/>
+      <c s="8" r="A585"/>
     </row>
     <row r="586">
-      <c s="7" r="A586"/>
+      <c s="8" r="A586"/>
     </row>
     <row r="587">
-      <c s="7" r="A587"/>
+      <c s="8" r="A587"/>
     </row>
     <row r="588">
-      <c s="7" r="A588"/>
+      <c s="8" r="A588"/>
     </row>
     <row r="589">
-      <c s="7" r="A589"/>
+      <c s="8" r="A589"/>
     </row>
     <row r="590">
-      <c s="7" r="A590"/>
+      <c s="8" r="A590"/>
     </row>
     <row r="591">
-      <c s="7" r="A591"/>
+      <c s="8" r="A591"/>
     </row>
     <row r="592">
-      <c s="7" r="A592"/>
+      <c s="8" r="A592"/>
     </row>
     <row r="593">
-      <c s="7" r="A593"/>
+      <c s="8" r="A593"/>
     </row>
     <row r="594">
-      <c s="7" r="A594"/>
+      <c s="8" r="A594"/>
     </row>
     <row r="595">
-      <c s="7" r="A595"/>
+      <c s="8" r="A595"/>
     </row>
     <row r="596">
-      <c s="7" r="A596"/>
+      <c s="8" r="A596"/>
     </row>
     <row r="597">
-      <c s="7" r="A597"/>
+      <c s="8" r="A597"/>
     </row>
     <row r="598">
-      <c s="7" r="A598"/>
+      <c s="8" r="A598"/>
     </row>
     <row r="599">
-      <c s="7" r="A599"/>
+      <c s="8" r="A599"/>
     </row>
     <row r="600">
-      <c s="7" r="A600"/>
+      <c s="8" r="A600"/>
     </row>
     <row r="601">
-      <c s="7" r="A601"/>
+      <c s="8" r="A601"/>
     </row>
     <row r="602">
-      <c s="7" r="A602"/>
+      <c s="8" r="A602"/>
     </row>
     <row r="603">
-      <c s="7" r="A603"/>
+      <c s="8" r="A603"/>
     </row>
     <row r="604">
-      <c s="7" r="A604"/>
+      <c s="8" r="A604"/>
     </row>
     <row r="605">
-      <c s="7" r="A605"/>
+      <c s="8" r="A605"/>
     </row>
     <row r="606">
-      <c s="7" r="A606"/>
+      <c s="8" r="A606"/>
     </row>
     <row r="607">
-      <c s="7" r="A607"/>
+      <c s="8" r="A607"/>
     </row>
     <row r="608">
-      <c s="7" r="A608"/>
+      <c s="8" r="A608"/>
     </row>
     <row r="609">
-      <c s="7" r="A609"/>
+      <c s="8" r="A609"/>
     </row>
     <row r="610">
-      <c s="7" r="A610"/>
+      <c s="8" r="A610"/>
     </row>
     <row r="611">
-      <c s="7" r="A611"/>
+      <c s="8" r="A611"/>
     </row>
     <row r="612">
-      <c s="7" r="A612"/>
+      <c s="8" r="A612"/>
     </row>
     <row r="613">
-      <c s="7" r="A613"/>
+      <c s="8" r="A613"/>
     </row>
     <row r="614">
-      <c s="7" r="A614"/>
+      <c s="8" r="A614"/>
     </row>
     <row r="615">
-      <c s="7" r="A615"/>
+      <c s="8" r="A615"/>
     </row>
     <row r="616">
-      <c s="7" r="A616"/>
+      <c s="8" r="A616"/>
     </row>
     <row r="617">
-      <c s="7" r="A617"/>
+      <c s="8" r="A617"/>
     </row>
     <row r="618">
-      <c s="7" r="A618"/>
+      <c s="8" r="A618"/>
     </row>
     <row r="619">
-      <c s="7" r="A619"/>
+      <c s="8" r="A619"/>
     </row>
     <row r="620">
-      <c s="7" r="A620"/>
+      <c s="8" r="A620"/>
     </row>
     <row r="621">
-      <c s="7" r="A621"/>
+      <c s="8" r="A621"/>
     </row>
     <row r="622">
-      <c s="7" r="A622"/>
+      <c s="8" r="A622"/>
     </row>
     <row r="623">
-      <c s="7" r="A623"/>
+      <c s="8" r="A623"/>
     </row>
     <row r="624">
-      <c s="7" r="A624"/>
+      <c s="8" r="A624"/>
     </row>
     <row r="625">
-      <c s="7" r="A625"/>
+      <c s="8" r="A625"/>
     </row>
     <row r="626">
-      <c s="7" r="A626"/>
+      <c s="8" r="A626"/>
     </row>
     <row r="627">
-      <c s="7" r="A627"/>
+      <c s="8" r="A627"/>
     </row>
     <row r="628">
-      <c s="7" r="A628"/>
+      <c s="8" r="A628"/>
     </row>
     <row r="629">
-      <c s="7" r="A629"/>
+      <c s="8" r="A629"/>
     </row>
     <row r="630">
-      <c s="7" r="A630"/>
+      <c s="8" r="A630"/>
     </row>
     <row r="631">
-      <c s="7" r="A631"/>
+      <c s="8" r="A631"/>
     </row>
     <row r="632">
-      <c s="7" r="A632"/>
+      <c s="8" r="A632"/>
     </row>
     <row r="633">
-      <c s="7" r="A633"/>
+      <c s="8" r="A633"/>
     </row>
     <row r="634">
-      <c s="7" r="A634"/>
+      <c s="8" r="A634"/>
     </row>
     <row r="635">
-      <c s="7" r="A635"/>
+      <c s="8" r="A635"/>
     </row>
     <row r="636">
-      <c s="7" r="A636"/>
+      <c s="8" r="A636"/>
     </row>
     <row r="637">
-      <c s="7" r="A637"/>
+      <c s="8" r="A637"/>
     </row>
     <row r="638">
-      <c s="7" r="A638"/>
+      <c s="8" r="A638"/>
     </row>
     <row r="639">
-      <c s="7" r="A639"/>
+      <c s="8" r="A639"/>
     </row>
     <row r="640">
-      <c s="7" r="A640"/>
+      <c s="8" r="A640"/>
     </row>
     <row r="641">
-      <c s="7" r="A641"/>
+      <c s="8" r="A641"/>
     </row>
     <row r="642">
-      <c s="7" r="A642"/>
+      <c s="8" r="A642"/>
     </row>
     <row r="643">
-      <c s="7" r="A643"/>
+      <c s="8" r="A643"/>
     </row>
     <row r="644">
-      <c s="7" r="A644"/>
+      <c s="8" r="A644"/>
     </row>
     <row r="645">
-      <c s="7" r="A645"/>
+      <c s="8" r="A645"/>
     </row>
     <row r="646">
-      <c s="7" r="A646"/>
+      <c s="8" r="A646"/>
     </row>
     <row r="647">
-      <c s="7" r="A647"/>
+      <c s="8" r="A647"/>
     </row>
     <row r="648">
-      <c s="7" r="A648"/>
+      <c s="8" r="A648"/>
     </row>
     <row r="649">
-      <c s="7" r="A649"/>
+      <c s="8" r="A649"/>
     </row>
     <row r="650">
-      <c s="7" r="A650"/>
+      <c s="8" r="A650"/>
     </row>
     <row r="651">
-      <c s="7" r="A651"/>
+      <c s="8" r="A651"/>
     </row>
     <row r="652">
-      <c s="7" r="A652"/>
+      <c s="8" r="A652"/>
     </row>
     <row r="653">
-      <c s="7" r="A653"/>
+      <c s="8" r="A653"/>
     </row>
     <row r="654">
-      <c s="7" r="A654"/>
+      <c s="8" r="A654"/>
     </row>
     <row r="655">
-      <c s="7" r="A655"/>
+      <c s="8" r="A655"/>
     </row>
     <row r="656">
-      <c s="7" r="A656"/>
+      <c s="8" r="A656"/>
     </row>
     <row r="657">
-      <c s="7" r="A657"/>
+      <c s="8" r="A657"/>
     </row>
     <row r="658">
-      <c s="7" r="A658"/>
+      <c s="8" r="A658"/>
     </row>
     <row r="659">
-      <c s="7" r="A659"/>
+      <c s="8" r="A659"/>
     </row>
     <row r="660">
-      <c s="7" r="A660"/>
+      <c s="8" r="A660"/>
     </row>
     <row r="661">
-      <c s="7" r="A661"/>
+      <c s="8" r="A661"/>
     </row>
     <row r="662">
-      <c s="7" r="A662"/>
+      <c s="8" r="A662"/>
     </row>
     <row r="663">
-      <c s="7" r="A663"/>
+      <c s="8" r="A663"/>
     </row>
     <row r="664">
-      <c s="7" r="A664"/>
+      <c s="8" r="A664"/>
     </row>
     <row r="665">
-      <c s="7" r="A665"/>
+      <c s="8" r="A665"/>
     </row>
     <row r="666">
-      <c s="7" r="A666"/>
+      <c s="8" r="A666"/>
     </row>
     <row r="667">
-      <c s="7" r="A667"/>
+      <c s="8" r="A667"/>
     </row>
     <row r="668">
-      <c s="7" r="A668"/>
+      <c s="8" r="A668"/>
     </row>
     <row r="669">
-      <c s="7" r="A669"/>
+      <c s="8" r="A669"/>
     </row>
     <row r="670">
-      <c s="7" r="A670"/>
+      <c s="8" r="A670"/>
     </row>
     <row r="671">
-      <c s="7" r="A671"/>
+      <c s="8" r="A671"/>
     </row>
     <row r="672">
-      <c s="7" r="A672"/>
+      <c s="8" r="A672"/>
     </row>
     <row r="673">
-      <c s="7" r="A673"/>
+      <c s="8" r="A673"/>
     </row>
     <row r="674">
-      <c s="7" r="A674"/>
+      <c s="8" r="A674"/>
     </row>
     <row r="675">
-      <c s="7" r="A675"/>
+      <c s="8" r="A675"/>
     </row>
     <row r="676">
-      <c s="7" r="A676"/>
+      <c s="8" r="A676"/>
     </row>
     <row r="677">
-      <c s="7" r="A677"/>
+      <c s="8" r="A677"/>
     </row>
     <row r="678">
-      <c s="7" r="A678"/>
+      <c s="8" r="A678"/>
     </row>
     <row r="679">
-      <c s="7" r="A679"/>
+      <c s="8" r="A679"/>
     </row>
     <row r="680">
-      <c s="7" r="A680"/>
+      <c s="8" r="A680"/>
     </row>
     <row r="681">
-      <c s="7" r="A681"/>
+      <c s="8" r="A681"/>
     </row>
     <row r="682">
-      <c s="7" r="A682"/>
+      <c s="8" r="A682"/>
     </row>
     <row r="683">
-      <c s="7" r="A683"/>
+      <c s="8" r="A683"/>
     </row>
     <row r="684">
-      <c s="7" r="A684"/>
+      <c s="8" r="A684"/>
     </row>
     <row r="685">
-      <c s="7" r="A685"/>
+      <c s="8" r="A685"/>
     </row>
     <row r="686">
-      <c s="7" r="A686"/>
+      <c s="8" r="A686"/>
     </row>
     <row r="687">
-      <c s="7" r="A687"/>
+      <c s="8" r="A687"/>
     </row>
     <row r="688">
-      <c s="7" r="A688"/>
+      <c s="8" r="A688"/>
     </row>
     <row r="689">
-      <c s="7" r="A689"/>
+      <c s="8" r="A689"/>
     </row>
     <row r="690">
-      <c s="7" r="A690"/>
+      <c s="8" r="A690"/>
     </row>
     <row r="691">
-      <c s="7" r="A691"/>
+      <c s="8" r="A691"/>
     </row>
     <row r="692">
-      <c s="7" r="A692"/>
+      <c s="8" r="A692"/>
     </row>
     <row r="693">
-      <c s="7" r="A693"/>
+      <c s="8" r="A693"/>
     </row>
     <row r="694">
-      <c s="7" r="A694"/>
+      <c s="8" r="A694"/>
     </row>
     <row r="695">
-      <c s="7" r="A695"/>
+      <c s="8" r="A695"/>
     </row>
     <row r="696">
-      <c s="7" r="A696"/>
+      <c s="8" r="A696"/>
     </row>
     <row r="697">
-      <c s="7" r="A697"/>
+      <c s="8" r="A697"/>
     </row>
     <row r="698">
-      <c s="7" r="A698"/>
+      <c s="8" r="A698"/>
     </row>
     <row r="699">
-      <c s="7" r="A699"/>
+      <c s="8" r="A699"/>
     </row>
     <row r="700">
-      <c s="7" r="A700"/>
+      <c s="8" r="A700"/>
     </row>
     <row r="701">
-      <c s="7" r="A701"/>
+      <c s="8" r="A701"/>
     </row>
     <row r="702">
-      <c s="7" r="A702"/>
+      <c s="8" r="A702"/>
     </row>
     <row r="703">
-      <c s="7" r="A703"/>
+      <c s="8" r="A703"/>
     </row>
     <row r="704">
-      <c s="7" r="A704"/>
+      <c s="8" r="A704"/>
     </row>
     <row r="705">
-      <c s="7" r="A705"/>
+      <c s="8" r="A705"/>
     </row>
     <row r="706">
-      <c s="7" r="A706"/>
+      <c s="8" r="A706"/>
     </row>
     <row r="707">
-      <c s="7" r="A707"/>
+      <c s="8" r="A707"/>
     </row>
     <row r="708">
-      <c s="7" r="A708"/>
+      <c s="8" r="A708"/>
     </row>
     <row r="709">
-      <c s="7" r="A709"/>
+      <c s="8" r="A709"/>
     </row>
     <row r="710">
-      <c s="7" r="A710"/>
+      <c s="8" r="A710"/>
     </row>
     <row r="711">
-      <c s="7" r="A711"/>
+      <c s="8" r="A711"/>
     </row>
     <row r="712">
-      <c s="7" r="A712"/>
+      <c s="8" r="A712"/>
     </row>
     <row r="713">
-      <c s="7" r="A713"/>
+      <c s="8" r="A713"/>
     </row>
     <row r="714">
-      <c s="7" r="A714"/>
+      <c s="8" r="A714"/>
     </row>
     <row r="715">
-      <c s="7" r="A715"/>
+      <c s="8" r="A715"/>
     </row>
     <row r="716">
-      <c s="7" r="A716"/>
+      <c s="8" r="A716"/>
     </row>
     <row r="717">
-      <c s="7" r="A717"/>
+      <c s="8" r="A717"/>
     </row>
     <row r="718">
-      <c s="7" r="A718"/>
+      <c s="8" r="A718"/>
     </row>
     <row r="719">
-      <c s="7" r="A719"/>
+      <c s="8" r="A719"/>
     </row>
     <row r="720">
-      <c s="7" r="A720"/>
+      <c s="8" r="A720"/>
     </row>
     <row r="721">
-      <c s="7" r="A721"/>
+      <c s="8" r="A721"/>
     </row>
     <row r="722">
-      <c s="7" r="A722"/>
+      <c s="8" r="A722"/>
     </row>
     <row r="723">
-      <c s="7" r="A723"/>
+      <c s="8" r="A723"/>
     </row>
     <row r="724">
-      <c s="7" r="A724"/>
+      <c s="8" r="A724"/>
     </row>
     <row r="725">
-      <c s="7" r="A725"/>
+      <c s="8" r="A725"/>
     </row>
     <row r="726">
-      <c s="7" r="A726"/>
+      <c s="8" r="A726"/>
     </row>
     <row r="727">
-      <c s="7" r="A727"/>
+      <c s="8" r="A727"/>
     </row>
     <row r="728">
-      <c s="7" r="A728"/>
+      <c s="8" r="A728"/>
     </row>
     <row r="729">
-      <c s="7" r="A729"/>
+      <c s="8" r="A729"/>
     </row>
     <row r="730">
-      <c s="7" r="A730"/>
+      <c s="8" r="A730"/>
     </row>
     <row r="731">
-      <c s="7" r="A731"/>
+      <c s="8" r="A731"/>
     </row>
     <row r="732">
-      <c s="7" r="A732"/>
+      <c s="8" r="A732"/>
     </row>
     <row r="733">
-      <c s="7" r="A733"/>
+      <c s="8" r="A733"/>
     </row>
     <row r="734">
-      <c s="7" r="A734"/>
+      <c s="8" r="A734"/>
     </row>
     <row r="735">
-      <c s="7" r="A735"/>
+      <c s="8" r="A735"/>
     </row>
     <row r="736">
-      <c s="7" r="A736"/>
+      <c s="8" r="A736"/>
     </row>
     <row r="737">
-      <c s="7" r="A737"/>
+      <c s="8" r="A737"/>
     </row>
     <row r="738">
-      <c s="7" r="A738"/>
+      <c s="8" r="A738"/>
     </row>
     <row r="739">
-      <c s="7" r="A739"/>
+      <c s="8" r="A739"/>
     </row>
     <row r="740">
-      <c s="7" r="A740"/>
+      <c s="8" r="A740"/>
     </row>
     <row r="741">
-      <c s="7" r="A741"/>
+      <c s="8" r="A741"/>
     </row>
     <row r="742">
-      <c s="7" r="A742"/>
+      <c s="8" r="A742"/>
     </row>
     <row r="743">
-      <c s="7" r="A743"/>
+      <c s="8" r="A743"/>
     </row>
     <row r="744">
-      <c s="7" r="A744"/>
+      <c s="8" r="A744"/>
     </row>
     <row r="745">
-      <c s="7" r="A745"/>
+      <c s="8" r="A745"/>
     </row>
     <row r="746">
-      <c s="7" r="A746"/>
+      <c s="8" r="A746"/>
     </row>
     <row r="747">
-      <c s="7" r="A747"/>
+      <c s="8" r="A747"/>
     </row>
     <row r="748">
-      <c s="7" r="A748"/>
+      <c s="8" r="A748"/>
     </row>
     <row r="749">
-      <c s="7" r="A749"/>
+      <c s="8" r="A749"/>
     </row>
     <row r="750">
-      <c s="7" r="A750"/>
+      <c s="8" r="A750"/>
     </row>
     <row r="751">
-      <c s="7" r="A751"/>
+      <c s="8" r="A751"/>
     </row>
     <row r="752">
-      <c s="7" r="A752"/>
+      <c s="8" r="A752"/>
     </row>
     <row r="753">
-      <c s="7" r="A753"/>
+      <c s="8" r="A753"/>
     </row>
     <row r="754">
-      <c s="7" r="A754"/>
+      <c s="8" r="A754"/>
     </row>
     <row r="755">
-      <c s="7" r="A755"/>
+      <c s="8" r="A755"/>
     </row>
     <row r="756">
-      <c s="7" r="A756"/>
+      <c s="8" r="A756"/>
     </row>
     <row r="757">
-      <c s="7" r="A757"/>
+      <c s="8" r="A757"/>
     </row>
     <row r="758">
-      <c s="7" r="A758"/>
+      <c s="8" r="A758"/>
     </row>
     <row r="759">
-      <c s="7" r="A759"/>
+      <c s="8" r="A759"/>
     </row>
     <row r="760">
-      <c s="7" r="A760"/>
+      <c s="8" r="A760"/>
     </row>
     <row r="761">
-      <c s="7" r="A761"/>
+      <c s="8" r="A761"/>
     </row>
     <row r="762">
-      <c s="7" r="A762"/>
+      <c s="8" r="A762"/>
     </row>
     <row r="763">
-      <c s="7" r="A763"/>
+      <c s="8" r="A763"/>
     </row>
     <row r="764">
-      <c s="7" r="A764"/>
+      <c s="8" r="A764"/>
     </row>
     <row r="765">
-      <c s="7" r="A765"/>
+      <c s="8" r="A765"/>
     </row>
     <row r="766">
-      <c s="7" r="A766"/>
+      <c s="8" r="A766"/>
     </row>
     <row r="767">
-      <c s="7" r="A767"/>
+      <c s="8" r="A767"/>
     </row>
     <row r="768">
-      <c s="7" r="A768"/>
+      <c s="8" r="A768"/>
     </row>
     <row r="769">
-      <c s="7" r="A769"/>
+      <c s="8" r="A769"/>
     </row>
     <row r="770">
-      <c s="7" r="A770"/>
+      <c s="8" r="A770"/>
     </row>
     <row r="771">
-      <c s="7" r="A771"/>
+      <c s="8" r="A771"/>
     </row>
     <row r="772">
-      <c s="7" r="A772"/>
+      <c s="8" r="A772"/>
     </row>
     <row r="773">
-      <c s="7" r="A773"/>
+      <c s="8" r="A773"/>
     </row>
     <row r="774">
-      <c s="7" r="A774"/>
+      <c s="8" r="A774"/>
     </row>
     <row r="775">
-      <c s="7" r="A775"/>
+      <c s="8" r="A775"/>
     </row>
     <row r="776">
-      <c s="7" r="A776"/>
+      <c s="8" r="A776"/>
     </row>
     <row r="777">
-      <c s="7" r="A777"/>
+      <c s="8" r="A777"/>
     </row>
     <row r="778">
-      <c s="7" r="A778"/>
+      <c s="8" r="A778"/>
     </row>
     <row r="779">
-      <c s="7" r="A779"/>
+      <c s="8" r="A779"/>
     </row>
     <row r="780">
-      <c s="7" r="A780"/>
+      <c s="8" r="A780"/>
     </row>
     <row r="781">
-      <c s="7" r="A781"/>
+      <c s="8" r="A781"/>
     </row>
     <row r="782">
-      <c s="7" r="A782"/>
+      <c s="8" r="A782"/>
     </row>
     <row r="783">
-      <c s="7" r="A783"/>
+      <c s="8" r="A783"/>
     </row>
     <row r="784">
-      <c s="7" r="A784"/>
+      <c s="8" r="A784"/>
     </row>
     <row r="785">
-      <c s="7" r="A785"/>
+      <c s="8" r="A785"/>
     </row>
     <row r="786">
-      <c s="7" r="A786"/>
+      <c s="8" r="A786"/>
     </row>
     <row r="787">
-      <c s="7" r="A787"/>
+      <c s="8" r="A787"/>
     </row>
     <row r="788">
-      <c s="7" r="A788"/>
+      <c s="8" r="A788"/>
     </row>
     <row r="789">
-      <c s="7" r="A789"/>
+      <c s="8" r="A789"/>
     </row>
     <row r="790">
-      <c s="7" r="A790"/>
+      <c s="8" r="A790"/>
     </row>
     <row r="791">
-      <c s="7" r="A791"/>
+      <c s="8" r="A791"/>
     </row>
     <row r="792">
-      <c s="7" r="A792"/>
+      <c s="8" r="A792"/>
     </row>
     <row r="793">
-      <c s="7" r="A793"/>
+      <c s="8" r="A793"/>
     </row>
     <row r="794">
-      <c s="7" r="A794"/>
+      <c s="8" r="A794"/>
     </row>
     <row r="795">
-      <c s="7" r="A795"/>
+      <c s="8" r="A795"/>
     </row>
     <row r="796">
-      <c s="7" r="A796"/>
+      <c s="8" r="A796"/>
     </row>
     <row r="797">
-      <c s="7" r="A797"/>
+      <c s="8" r="A797"/>
     </row>
     <row r="798">
-      <c s="7" r="A798"/>
+      <c s="8" r="A798"/>
     </row>
     <row r="799">
-      <c s="7" r="A799"/>
+      <c s="8" r="A799"/>
     </row>
     <row r="800">
-      <c s="7" r="A800"/>
+      <c s="8" r="A800"/>
     </row>
     <row r="801">
-      <c s="7" r="A801"/>
+      <c s="8" r="A801"/>
     </row>
     <row r="802">
-      <c s="7" r="A802"/>
+      <c s="8" r="A802"/>
     </row>
     <row r="803">
-      <c s="7" r="A803"/>
+      <c s="8" r="A803"/>
     </row>
     <row r="804">
-      <c s="7" r="A804"/>
+      <c s="8" r="A804"/>
     </row>
     <row r="805">
-      <c s="7" r="A805"/>
+      <c s="8" r="A805"/>
     </row>
     <row r="806">
-      <c s="7" r="A806"/>
+      <c s="8" r="A806"/>
     </row>
     <row r="807">
-      <c s="7" r="A807"/>
+      <c s="8" r="A807"/>
     </row>
     <row r="808">
-      <c s="7" r="A808"/>
+      <c s="8" r="A808"/>
     </row>
     <row r="809">
-      <c s="7" r="A809"/>
+      <c s="8" r="A809"/>
     </row>
     <row r="810">
-      <c s="7" r="A810"/>
+      <c s="8" r="A810"/>
     </row>
     <row r="811">
-      <c s="7" r="A811"/>
+      <c s="8" r="A811"/>
     </row>
     <row r="812">
-      <c s="7" r="A812"/>
+      <c s="8" r="A812"/>
     </row>
     <row r="813">
-      <c s="7" r="A813"/>
+      <c s="8" r="A813"/>
     </row>
     <row r="814">
-      <c s="7" r="A814"/>
+      <c s="8" r="A814"/>
     </row>
     <row r="815">
-      <c s="7" r="A815"/>
+      <c s="8" r="A815"/>
     </row>
     <row r="816">
-      <c s="7" r="A816"/>
+      <c s="8" r="A816"/>
     </row>
     <row r="817">
-      <c s="7" r="A817"/>
+      <c s="8" r="A817"/>
     </row>
     <row r="818">
-      <c s="7" r="A818"/>
+      <c s="8" r="A818"/>
     </row>
     <row r="819">
-      <c s="7" r="A819"/>
+      <c s="8" r="A819"/>
     </row>
     <row r="820">
-      <c s="7" r="A820"/>
+      <c s="8" r="A820"/>
     </row>
     <row r="821">
-      <c s="7" r="A821"/>
+      <c s="8" r="A821"/>
     </row>
     <row r="822">
-      <c s="7" r="A822"/>
+      <c s="8" r="A822"/>
     </row>
     <row r="823">
-      <c s="7" r="A823"/>
+      <c s="8" r="A823"/>
     </row>
     <row r="824">
-      <c s="7" r="A824"/>
+      <c s="8" r="A824"/>
     </row>
     <row r="825">
-      <c s="7" r="A825"/>
+      <c s="8" r="A825"/>
     </row>
     <row r="826">
-      <c s="7" r="A826"/>
+      <c s="8" r="A826"/>
     </row>
     <row r="827">
-      <c s="7" r="A827"/>
+      <c s="8" r="A827"/>
     </row>
     <row r="828">
-      <c s="7" r="A828"/>
+      <c s="8" r="A828"/>
     </row>
     <row r="829">
-      <c s="7" r="A829"/>
+      <c s="8" r="A829"/>
     </row>
     <row r="830">
-      <c s="7" r="A830"/>
+      <c s="8" r="A830"/>
     </row>
     <row r="831">
-      <c s="7" r="A831"/>
+      <c s="8" r="A831"/>
     </row>
     <row r="832">
-      <c s="7" r="A832"/>
+      <c s="8" r="A832"/>
     </row>
     <row r="833">
-      <c s="7" r="A833"/>
+      <c s="8" r="A833"/>
     </row>
     <row r="834">
-      <c s="7" r="A834"/>
+      <c s="8" r="A834"/>
     </row>
     <row r="835">
-      <c s="7" r="A835"/>
+      <c s="8" r="A835"/>
     </row>
     <row r="836">
-      <c s="7" r="A836"/>
+      <c s="8" r="A836"/>
     </row>
     <row r="837">
-      <c s="7" r="A837"/>
+      <c s="8" r="A837"/>
     </row>
     <row r="838">
-      <c s="7" r="A838"/>
+      <c s="8" r="A838"/>
     </row>
     <row r="839">
-      <c s="7" r="A839"/>
+      <c s="8" r="A839"/>
     </row>
     <row r="840">
-      <c s="7" r="A840"/>
+      <c s="8" r="A840"/>
     </row>
     <row r="841">
-      <c s="7" r="A841"/>
+      <c s="8" r="A841"/>
     </row>
     <row r="842">
-      <c s="7" r="A842"/>
+      <c s="8" r="A842"/>
     </row>
     <row r="843">
-      <c s="7" r="A843"/>
+      <c s="8" r="A843"/>
     </row>
     <row r="844">
-      <c s="7" r="A844"/>
+      <c s="8" r="A844"/>
     </row>
     <row r="845">
-      <c s="7" r="A845"/>
+      <c s="8" r="A845"/>
     </row>
     <row r="846">
-      <c s="7" r="A846"/>
+      <c s="8" r="A846"/>
     </row>
     <row r="847">
-      <c s="7" r="A847"/>
+      <c s="8" r="A847"/>
     </row>
     <row r="848">
-      <c s="7" r="A848"/>
+      <c s="8" r="A848"/>
     </row>
     <row r="849">
-      <c s="7" r="A849"/>
+      <c s="8" r="A849"/>
     </row>
     <row r="850">
-      <c s="7" r="A850"/>
+      <c s="8" r="A850"/>
     </row>
     <row r="851">
-      <c s="7" r="A851"/>
+      <c s="8" r="A851"/>
     </row>
     <row r="852">
-      <c s="7" r="A852"/>
+      <c s="8" r="A852"/>
     </row>
     <row r="853">
-      <c s="7" r="A853"/>
+      <c s="8" r="A853"/>
     </row>
     <row r="854">
-      <c s="7" r="A854"/>
+      <c s="8" r="A854"/>
     </row>
     <row r="855">
-      <c s="7" r="A855"/>
+      <c s="8" r="A855"/>
     </row>
     <row r="856">
-      <c s="7" r="A856"/>
+      <c s="8" r="A856"/>
     </row>
     <row r="857">
-      <c s="7" r="A857"/>
+      <c s="8" r="A857"/>
     </row>
     <row r="858">
-      <c s="7" r="A858"/>
+      <c s="8" r="A858"/>
     </row>
     <row r="859">
-      <c s="7" r="A859"/>
+      <c s="8" r="A859"/>
     </row>
     <row r="860">
-      <c s="7" r="A860"/>
+      <c s="8" r="A860"/>
     </row>
     <row r="861">
-      <c s="7" r="A861"/>
+      <c s="8" r="A861"/>
     </row>
     <row r="862">
-      <c s="7" r="A862"/>
+      <c s="8" r="A862"/>
     </row>
     <row r="863">
-      <c s="7" r="A863"/>
+      <c s="8" r="A863"/>
     </row>
     <row r="864">
-      <c s="7" r="A864"/>
+      <c s="8" r="A864"/>
     </row>
     <row r="865">
-      <c s="7" r="A865"/>
+      <c s="8" r="A865"/>
     </row>
     <row r="866">
-      <c s="7" r="A866"/>
+      <c s="8" r="A866"/>
     </row>
     <row r="867">
-      <c s="7" r="A867"/>
+      <c s="8" r="A867"/>
     </row>
     <row r="868">
-      <c s="7" r="A868"/>
+      <c s="8" r="A868"/>
     </row>
     <row r="869">
-      <c s="7" r="A869"/>
+      <c s="8" r="A869"/>
     </row>
     <row r="870">
-      <c s="7" r="A870"/>
+      <c s="8" r="A870"/>
     </row>
     <row r="871">
-      <c s="7" r="A871"/>
+      <c s="8" r="A871"/>
     </row>
     <row r="872">
-      <c s="7" r="A872"/>
+      <c s="8" r="A872"/>
     </row>
     <row r="873">
-      <c s="7" r="A873"/>
+      <c s="8" r="A873"/>
     </row>
     <row r="874">
-      <c s="7" r="A874"/>
+      <c s="8" r="A874"/>
     </row>
     <row r="875">
-      <c s="7" r="A875"/>
+      <c s="8" r="A875"/>
     </row>
     <row r="876">
-      <c s="7" r="A876"/>
+      <c s="8" r="A876"/>
     </row>
     <row r="877">
-      <c s="7" r="A877"/>
+      <c s="8" r="A877"/>
     </row>
     <row r="878">
-      <c s="7" r="A878"/>
+      <c s="8" r="A878"/>
     </row>
     <row r="879">
-      <c s="7" r="A879"/>
+      <c s="8" r="A879"/>
     </row>
     <row r="880">
-      <c s="7" r="A880"/>
+      <c s="8" r="A880"/>
     </row>
     <row r="881">
-      <c s="7" r="A881"/>
+      <c s="8" r="A881"/>
     </row>
     <row r="882">
-      <c s="7" r="A882"/>
+      <c s="8" r="A882"/>
     </row>
     <row r="883">
-      <c s="7" r="A883"/>
+      <c s="8" r="A883"/>
     </row>
     <row r="884">
-      <c s="7" r="A884"/>
+      <c s="8" r="A884"/>
     </row>
     <row r="885">
-      <c s="7" r="A885"/>
+      <c s="8" r="A885"/>
     </row>
     <row r="886">
-      <c s="7" r="A886"/>
+      <c s="8" r="A886"/>
     </row>
     <row r="887">
-      <c s="7" r="A887"/>
+      <c s="8" r="A887"/>
     </row>
     <row r="888">
-      <c s="7" r="A888"/>
+      <c s="8" r="A888"/>
     </row>
     <row r="889">
-      <c s="7" r="A889"/>
+      <c s="8" r="A889"/>
     </row>
     <row r="890">
-      <c s="7" r="A890"/>
+      <c s="8" r="A890"/>
     </row>
     <row r="891">
-      <c s="7" r="A891"/>
+      <c s="8" r="A891"/>
     </row>
     <row r="892">
-      <c s="7" r="A892"/>
+      <c s="8" r="A892"/>
     </row>
     <row r="893">
-      <c s="7" r="A893"/>
+      <c s="8" r="A893"/>
     </row>
     <row r="894">
-      <c s="7" r="A894"/>
+      <c s="8" r="A894"/>
     </row>
     <row r="895">
-      <c s="7" r="A895"/>
+      <c s="8" r="A895"/>
     </row>
     <row r="896">
-      <c s="7" r="A896"/>
+      <c s="8" r="A896"/>
     </row>
     <row r="897">
-      <c s="7" r="A897"/>
+      <c s="8" r="A897"/>
     </row>
     <row r="898">
-      <c s="7" r="A898"/>
+      <c s="8" r="A898"/>
     </row>
     <row r="899">
-      <c s="7" r="A899"/>
+      <c s="8" r="A899"/>
     </row>
     <row r="900">
-      <c s="7" r="A900"/>
+      <c s="8" r="A900"/>
     </row>
     <row r="901">
-      <c s="7" r="A901"/>
+      <c s="8" r="A901"/>
     </row>
     <row r="902">
-      <c s="7" r="A902"/>
+      <c s="8" r="A902"/>
     </row>
     <row r="903">
-      <c s="7" r="A903"/>
+      <c s="8" r="A903"/>
     </row>
     <row r="904">
-      <c s="7" r="A904"/>
+      <c s="8" r="A904"/>
     </row>
     <row r="905">
-      <c s="7" r="A905"/>
+      <c s="8" r="A905"/>
     </row>
     <row r="906">
-      <c s="7" r="A906"/>
+      <c s="8" r="A906"/>
     </row>
     <row r="907">
-      <c s="7" r="A907"/>
+      <c s="8" r="A907"/>
     </row>
     <row r="908">
-      <c s="7" r="A908"/>
+      <c s="8" r="A908"/>
     </row>
     <row r="909">
-      <c s="7" r="A909"/>
+      <c s="8" r="A909"/>
     </row>
     <row r="910">
-      <c s="7" r="A910"/>
+      <c s="8" r="A910"/>
     </row>
     <row r="911">
-      <c s="7" r="A911"/>
+      <c s="8" r="A911"/>
     </row>
     <row r="912">
-      <c s="7" r="A912"/>
+      <c s="8" r="A912"/>
     </row>
     <row r="913">
-      <c s="7" r="A913"/>
+      <c s="8" r="A913"/>
     </row>
     <row r="914">
-      <c s="7" r="A914"/>
+      <c s="8" r="A914"/>
     </row>
     <row r="915">
-      <c s="7" r="A915"/>
+      <c s="8" r="A915"/>
     </row>
     <row r="916">
-      <c s="7" r="A916"/>
+      <c s="8" r="A916"/>
     </row>
     <row r="917">
-      <c s="7" r="A917"/>
+      <c s="8" r="A917"/>
     </row>
     <row r="918">
-      <c s="7" r="A918"/>
+      <c s="8" r="A918"/>
     </row>
     <row r="919">
-      <c s="7" r="A919"/>
+      <c s="8" r="A919"/>
     </row>
     <row r="920">
-      <c s="7" r="A920"/>
+      <c s="8" r="A920"/>
     </row>
     <row r="921">
-      <c s="7" r="A921"/>
+      <c s="8" r="A921"/>
     </row>
     <row r="922">
-      <c s="7" r="A922"/>
+      <c s="8" r="A922"/>
     </row>
     <row r="923">
-      <c s="7" r="A923"/>
+      <c s="8" r="A923"/>
     </row>
     <row r="924">
-      <c s="7" r="A924"/>
+      <c s="8" r="A924"/>
     </row>
     <row r="925">
-      <c s="7" r="A925"/>
+      <c s="8" r="A925"/>
     </row>
     <row r="926">
-      <c s="7" r="A926"/>
+      <c s="8" r="A926"/>
     </row>
     <row r="927">
-      <c s="7" r="A927"/>
+      <c s="8" r="A927"/>
     </row>
     <row r="928">
-      <c s="7" r="A928"/>
+      <c s="8" r="A928"/>
     </row>
     <row r="929">
-      <c s="7" r="A929"/>
+      <c s="8" r="A929"/>
     </row>
     <row r="930">
-      <c s="7" r="A930"/>
+      <c s="8" r="A930"/>
     </row>
     <row r="931">
-      <c s="7" r="A931"/>
+      <c s="8" r="A931"/>
     </row>
     <row r="932">
-      <c s="7" r="A932"/>
+      <c s="8" r="A932"/>
     </row>
     <row r="933">
-      <c s="7" r="A933"/>
+      <c s="8" r="A933"/>
     </row>
     <row r="934">
-      <c s="7" r="A934"/>
+      <c s="8" r="A934"/>
     </row>
     <row r="935">
-      <c s="7" r="A935"/>
+      <c s="8" r="A935"/>
     </row>
     <row r="936">
-      <c s="7" r="A936"/>
+      <c s="8" r="A936"/>
     </row>
     <row r="937">
-      <c s="7" r="A937"/>
+      <c s="8" r="A937"/>
     </row>
     <row r="938">
-      <c s="7" r="A938"/>
+      <c s="8" r="A938"/>
     </row>
     <row r="939">
-      <c s="7" r="A939"/>
+      <c s="8" r="A939"/>
     </row>
     <row r="940">
-      <c s="7" r="A940"/>
+      <c s="8" r="A940"/>
     </row>
     <row r="941">
-      <c s="7" r="A941"/>
+      <c s="8" r="A941"/>
     </row>
     <row r="942">
-      <c s="7" r="A942"/>
+      <c s="8" r="A942"/>
     </row>
     <row r="943">
-      <c s="7" r="A943"/>
+      <c s="8" r="A943"/>
     </row>
     <row r="944">
-      <c s="7" r="A944"/>
+      <c s="8" r="A944"/>
     </row>
     <row r="945">
-      <c s="7" r="A945"/>
+      <c s="8" r="A945"/>
     </row>
     <row r="946">
-      <c s="7" r="A946"/>
+      <c s="8" r="A946"/>
     </row>
     <row r="947">
-      <c s="7" r="A947"/>
+      <c s="8" r="A947"/>
     </row>
     <row r="948">
-      <c s="7" r="A948"/>
+      <c s="8" r="A948"/>
     </row>
     <row r="949">
-      <c s="7" r="A949"/>
+      <c s="8" r="A949"/>
     </row>
     <row r="950">
-      <c s="7" r="A950"/>
+      <c s="8" r="A950"/>
     </row>
     <row r="951">
-      <c s="7" r="A951"/>
+      <c s="8" r="A951"/>
     </row>
     <row r="952">
-      <c s="7" r="A952"/>
+      <c s="8" r="A952"/>
     </row>
     <row r="953">
-      <c s="7" r="A953"/>
+      <c s="8" r="A953"/>
     </row>
     <row r="954">
-      <c s="7" r="A954"/>
+      <c s="8" r="A954"/>
     </row>
     <row r="955">
-      <c s="7" r="A955"/>
+      <c s="8" r="A955"/>
     </row>
     <row r="956">
-      <c s="7" r="A956"/>
+      <c s="8" r="A956"/>
     </row>
     <row r="957">
-      <c s="7" r="A957"/>
+      <c s="8" r="A957"/>
     </row>
     <row r="958">
-      <c s="7" r="A958"/>
+      <c s="8" r="A958"/>
     </row>
     <row r="959">
-      <c s="7" r="A959"/>
+      <c s="8" r="A959"/>
     </row>
     <row r="960">
-      <c s="7" r="A960"/>
+      <c s="8" r="A960"/>
     </row>
     <row r="961">
-      <c s="7" r="A961"/>
+      <c s="8" r="A961"/>
     </row>
     <row r="962">
-      <c s="7" r="A962"/>
+      <c s="8" r="A962"/>
     </row>
     <row r="963">
-      <c s="7" r="A963"/>
+      <c s="8" r="A963"/>
     </row>
     <row r="964">
-      <c s="7" r="A964"/>
+      <c s="8" r="A964"/>
     </row>
     <row r="965">
-      <c s="7" r="A965"/>
+      <c s="8" r="A965"/>
     </row>
     <row r="966">
-      <c s="7" r="A966"/>
+      <c s="8" r="A966"/>
     </row>
     <row r="967">
-      <c s="7" r="A967"/>
+      <c s="8" r="A967"/>
     </row>
     <row r="968">
-      <c s="7" r="A968"/>
+      <c s="8" r="A968"/>
     </row>
     <row r="969">
-      <c s="7" r="A969"/>
+      <c s="8" r="A969"/>
     </row>
     <row r="970">
-      <c s="7" r="A970"/>
+      <c s="8" r="A970"/>
     </row>
     <row r="971">
-      <c s="7" r="A971"/>
+      <c s="8" r="A971"/>
     </row>
     <row r="972">
-      <c s="7" r="A972"/>
+      <c s="8" r="A972"/>
     </row>
     <row r="973">
-      <c s="7" r="A973"/>
+      <c s="8" r="A973"/>
     </row>
     <row r="974">
-      <c s="7" r="A974"/>
+      <c s="8" r="A974"/>
     </row>
     <row r="975">
-      <c s="7" r="A975"/>
+      <c s="8" r="A975"/>
     </row>
     <row r="976">
-      <c s="7" r="A976"/>
+      <c s="8" r="A976"/>
     </row>
     <row r="977">
-      <c s="7" r="A977"/>
+      <c s="8" r="A977"/>
     </row>
     <row r="978">
-      <c s="7" r="A978"/>
+      <c s="8" r="A978"/>
     </row>
     <row r="979">
-      <c s="7" r="A979"/>
+      <c s="8" r="A979"/>
     </row>
     <row r="980">
-      <c s="7" r="A980"/>
+      <c s="8" r="A980"/>
     </row>
     <row r="981">
-      <c s="7" r="A981"/>
+      <c s="8" r="A981"/>
     </row>
     <row r="982">
-      <c s="7" r="A982"/>
+      <c s="8" r="A982"/>
     </row>
     <row r="983">
-      <c s="7" r="A983"/>
+      <c s="8" r="A983"/>
     </row>
     <row r="984">
-      <c s="7" r="A984"/>
+      <c s="8" r="A984"/>
     </row>
     <row r="985">
-      <c s="7" r="A985"/>
+      <c s="8" r="A985"/>
     </row>
     <row r="986">
-      <c s="7" r="A986"/>
+      <c s="8" r="A986"/>
     </row>
     <row r="987">
-      <c s="7" r="A987"/>
+      <c s="8" r="A987"/>
     </row>
     <row r="988">
-      <c s="7" r="A988"/>
+      <c s="8" r="A988"/>
     </row>
     <row r="989">
-      <c s="7" r="A989"/>
+      <c s="8" r="A989"/>
     </row>
     <row r="990">
-      <c s="7" r="A990"/>
+      <c s="8" r="A990"/>
     </row>
     <row r="991">
-      <c s="7" r="A991"/>
+      <c s="8" r="A991"/>
     </row>
     <row r="992">
-      <c s="7" r="A992"/>
+      <c s="8" r="A992"/>
     </row>
     <row r="993">
-      <c s="7" r="A993"/>
+      <c s="8" r="A993"/>
     </row>
     <row r="994">
-      <c s="7" r="A994"/>
+      <c s="8" r="A994"/>
     </row>
     <row r="995">
-      <c s="7" r="A995"/>
+      <c s="8" r="A995"/>
     </row>
     <row r="996">
-      <c s="7" r="A996"/>
+      <c s="8" r="A996"/>
     </row>
     <row r="997">
-      <c s="7" r="A997"/>
+      <c s="8" r="A997"/>
     </row>
     <row r="998">
-      <c s="7" r="A998"/>
+      <c s="8" r="A998"/>
     </row>
     <row r="999">
-      <c s="7" r="A999"/>
+      <c s="8" r="A999"/>
     </row>
     <row r="1000">
-      <c s="7" r="A1000"/>
+      <c s="8" r="A1000"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
style tweaks and removed view all btn
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -40,7 +40,10 @@
     <t>imgOK</t>
   </si>
   <si>
-    <t>"You know how long that takes in Texas at 75 miles an hour? That's a particularly flat highway."</t>
+    <t>imgDir</t>
+  </si>
+  <si>
+    <t>You know how long that takes in Texas at 75 miles an hour? That's a particularly flat highway.</t>
   </si>
   <si>
     <t>Judge Edith Jones</t>
@@ -64,7 +67,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>“MARRIAGE = ONE MAN &amp; ONE MAN. Enough of these activist judges. FAVORITE if you agree. I know the silent majority out there is with us!”</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>MARRIAGE = ONE MAN &amp; ONE MAN. Enough of these activist judges. FAVORITE if you agree. I know the silent majority out there is with us!</t>
   </si>
   <si>
     <t>State Sen. Dan Patrick</t>
@@ -88,7 +94,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>"Apparently I’ve outfoxed the campaign deal, so maybe I need to be a consultant. I’m not going to run all over the state. I work."</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Apparently I’ve outfoxed the campaign deal, so maybe I need to be a consultant. I’m not going to run all over the state. I work.</t>
   </si>
   <si>
     <t>Jim Hogan</t>
@@ -112,7 +121,10 @@
     <t>n</t>
   </si>
   <si>
-    <t>"Out there on Twitter, in front of the Alamo in your campaign, you know, you’ve been huffing and puffing like the big bad wolf and now you’re dancing around, tiptoeing like Little Red Riding Hood on this issue."</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Out there on Twitter, in front of the Alamo in your campaign, you know, you’ve been huffing and puffing like the big bad wolf and now you’re dancing around, tiptoeing like Little Red Riding Hood on this issue.</t>
   </si>
   <si>
     <t>San Antonio Mayor Julián Castro</t>
@@ -136,7 +148,10 @@
     <t>n</t>
   </si>
   <si>
-    <t>"Dewhurst has asked me to cease distribution of this information. He also asked me not to run against him for Lt. Gov. I didn't really give a damn what David wanted then, and I don't give a damn now. The voters of Texas need to know."</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Dewhurst has asked me to cease distribution of this information. He also asked me not to run against him for Lt. Gov. I didn't really give a damn what David wanted then, and I don't give a damn now. The voters of Texas need to know.</t>
   </si>
   <si>
     <t>Jerry Patterson</t>
@@ -160,7 +175,10 @@
     <t>n</t>
   </si>
   <si>
-    <t>"Some Democrats have said they wanted me to be the nominee. Well, they’ve got me and I’m coming."</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Some Democrats have said they wanted me to be the nominee. Well, they’ve got me and I’m coming.</t>
   </si>
   <si>
     <t>State Sen. Dan Patrick</t>
@@ -184,7 +202,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>"The uninformed opinions of a Washington, D.C., desk jockey who's never stepped foot in Texas couldn't be less relevant to what's actually happening on the ground."</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>The uninformed opinions of a Washington, D.C., desk jockey who's never stepped foot in Texas couldn't be less relevant to what's actually happening on the ground.</t>
   </si>
   <si>
     <t>Karin Johanson</t>
@@ -208,7 +229,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>“We need to look at the states, which are lavatories of innovation and democracy.”</t>
+    <t>l</t>
+  </si>
+  <si>
+    <t>We need to look at the states, which are lavatories of innovation and democracy.</t>
   </si>
   <si>
     <t>Gov. Rick Perry</t>
@@ -232,7 +256,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>"We don't settle political differences with indictments in this country. It is outrageous that some would use partisan political theatrics to rip away at the very fabric of our state's constitution."</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>We don't settle political differences with indictments in this country. It is outrageous that some would use partisan political theatrics to rip away at the very fabric of our state's constitution.</t>
   </si>
   <si>
     <t>Gov. Rick Perry</t>
@@ -256,7 +283,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>“And all I can do is deal with the issues that are before me. … The job of attorney general is to represent and defend in court the laws of their client, which is the state Legislature, unless and until a court strikes it down.”</t>
+    <t>l</t>
+  </si>
+  <si>
+    <t>And all I can do is deal with the issues that are before me. … The job of attorney general is to represent and defend in court the laws of their client, which is the state Legislature, unless and until a court strikes it down.</t>
   </si>
   <si>
     <t>Attorney General Greg Abbott</t>
@@ -280,7 +310,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>"If that dog has to be The Boy in the Plastic Bubble, we're going to take good care of that dog."</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>If that dog has to be The Boy in the Plastic Bubble, we're going to take good care of that dog.</t>
   </si>
   <si>
     <t>Judge Clay Jenkins</t>
@@ -304,7 +337,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>"The only way we will have lost tonight is if we stop fighting. I am so proud of all that we have accomplished."</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>The only way we will have lost tonight is if we stop fighting. I am so proud of all that we have accomplished.</t>
   </si>
   <si>
     <t>Wendy Davis</t>
@@ -328,7 +364,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>“We were elected to govern. If we blow it by not governing, then shame on us.”</t>
+    <t>l</t>
+  </si>
+  <si>
+    <t>We were elected to govern. If we blow it by not governing, then shame on us.</t>
   </si>
   <si>
     <t>U.S. Rep. Michael McCaul</t>
@@ -347,6 +386,9 @@
   </si>
   <si>
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/MichaelMcCaul_1_jpg_75x75_crop_q100.jpg</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
   <si>
     <t>n</t>
@@ -356,7 +398,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -365,10 +407,13 @@
       <b/>
       <sz val="10.0"/>
     </font>
-    <font/>
+    <font>
+      <b/>
+    </font>
     <font>
       <sz val="10.0"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -402,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -422,8 +467,14 @@
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
       <alignment/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+      <alignment/>
+    </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
+      <alignment/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -477,34 +528,40 @@
       <c t="s" s="3" r="I1">
         <v>8</v>
       </c>
+      <c t="s" s="3" r="J1">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c s="4" r="A2">
         <v>0.0</v>
       </c>
       <c t="s" s="5" r="B2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c t="s" s="6" r="C2">
-        <v>10</v>
-      </c>
-      <c t="s" s="5" r="D2">
         <v>11</v>
       </c>
-      <c t="s" s="5" r="E2">
+      <c t="s" s="7" r="D2">
         <v>12</v>
       </c>
-      <c t="s" s="5" r="F2">
+      <c t="s" s="7" r="E2">
         <v>13</v>
       </c>
-      <c t="s" s="7" r="G2">
+      <c t="s" s="7" r="F2">
         <v>14</v>
       </c>
-      <c t="s" s="7" r="H2">
+      <c t="s" s="8" r="G2">
         <v>15</v>
       </c>
-      <c t="s" s="3" r="I2">
+      <c t="s" s="8" r="H2">
         <v>16</v>
+      </c>
+      <c t="s" s="9" r="I2">
+        <v>17</v>
+      </c>
+      <c t="s" s="9" r="J2">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -512,28 +569,31 @@
         <v>1.0</v>
       </c>
       <c t="s" s="5" r="B3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c t="s" s="6" r="C3">
-        <v>18</v>
-      </c>
-      <c t="s" s="5" r="D3">
-        <v>19</v>
-      </c>
-      <c t="s" s="5" r="E3">
         <v>20</v>
       </c>
-      <c t="s" s="5" r="F3">
+      <c t="s" s="7" r="D3">
         <v>21</v>
       </c>
-      <c t="s" s="7" r="G3">
+      <c t="s" s="7" r="E3">
         <v>22</v>
       </c>
-      <c t="s" s="5" r="H3">
+      <c t="s" s="7" r="F3">
         <v>23</v>
       </c>
-      <c t="s" s="3" r="I3">
+      <c t="s" s="8" r="G3">
         <v>24</v>
+      </c>
+      <c t="s" s="7" r="H3">
+        <v>25</v>
+      </c>
+      <c t="s" s="9" r="I3">
+        <v>26</v>
+      </c>
+      <c t="s" s="9" r="J3">
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -541,28 +601,31 @@
         <v>2.0</v>
       </c>
       <c t="s" s="5" r="B4">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c t="s" s="6" r="C4">
-        <v>26</v>
-      </c>
-      <c t="s" s="5" r="D4">
-        <v>27</v>
-      </c>
-      <c t="s" s="5" r="E4">
-        <v>28</v>
-      </c>
-      <c t="s" s="5" r="F4">
         <v>29</v>
       </c>
-      <c t="s" s="7" r="G4">
+      <c t="s" s="7" r="D4">
         <v>30</v>
       </c>
-      <c t="s" s="7" r="H4">
+      <c t="s" s="7" r="E4">
         <v>31</v>
       </c>
-      <c t="s" s="3" r="I4">
+      <c t="s" s="7" r="F4">
         <v>32</v>
+      </c>
+      <c t="s" s="8" r="G4">
+        <v>33</v>
+      </c>
+      <c t="s" s="8" r="H4">
+        <v>34</v>
+      </c>
+      <c t="s" s="9" r="I4">
+        <v>35</v>
+      </c>
+      <c t="s" s="9" r="J4">
+        <v>36</v>
       </c>
     </row>
     <row r="5">
@@ -570,28 +633,31 @@
         <v>3.0</v>
       </c>
       <c t="s" s="5" r="B5">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c t="s" s="6" r="C5">
-        <v>34</v>
-      </c>
-      <c t="s" s="5" r="D5">
-        <v>35</v>
-      </c>
-      <c t="s" s="5" r="E5">
-        <v>36</v>
-      </c>
-      <c t="s" s="5" r="F5">
-        <v>37</v>
-      </c>
-      <c t="s" s="7" r="G5">
         <v>38</v>
       </c>
-      <c t="s" s="7" r="H5">
+      <c t="s" s="7" r="D5">
         <v>39</v>
       </c>
-      <c t="s" s="3" r="I5">
+      <c t="s" s="7" r="E5">
         <v>40</v>
+      </c>
+      <c t="s" s="7" r="F5">
+        <v>41</v>
+      </c>
+      <c t="s" s="8" r="G5">
+        <v>42</v>
+      </c>
+      <c t="s" s="8" r="H5">
+        <v>43</v>
+      </c>
+      <c t="s" s="9" r="I5">
+        <v>44</v>
+      </c>
+      <c t="s" s="9" r="J5">
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -599,28 +665,31 @@
         <v>4.0</v>
       </c>
       <c t="s" s="5" r="B6">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c t="s" s="6" r="C6">
-        <v>42</v>
-      </c>
-      <c t="s" s="5" r="D6">
-        <v>43</v>
-      </c>
-      <c t="s" s="5" r="E6">
-        <v>44</v>
-      </c>
-      <c t="s" s="5" r="F6">
-        <v>45</v>
-      </c>
-      <c t="s" s="7" r="G6">
-        <v>46</v>
-      </c>
-      <c t="s" s="7" r="H6">
         <v>47</v>
       </c>
-      <c t="s" s="3" r="I6">
+      <c t="s" s="7" r="D6">
         <v>48</v>
+      </c>
+      <c t="s" s="7" r="E6">
+        <v>49</v>
+      </c>
+      <c t="s" s="7" r="F6">
+        <v>50</v>
+      </c>
+      <c t="s" s="8" r="G6">
+        <v>51</v>
+      </c>
+      <c t="s" s="8" r="H6">
+        <v>52</v>
+      </c>
+      <c t="s" s="9" r="I6">
+        <v>53</v>
+      </c>
+      <c t="s" s="9" r="J6">
+        <v>54</v>
       </c>
     </row>
     <row r="7">
@@ -628,28 +697,31 @@
         <v>5.0</v>
       </c>
       <c t="s" s="5" r="B7">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c t="s" s="6" r="C7">
-        <v>50</v>
-      </c>
-      <c t="s" s="5" r="D7">
-        <v>51</v>
-      </c>
-      <c t="s" s="5" r="E7">
-        <v>52</v>
-      </c>
-      <c t="s" s="5" r="F7">
-        <v>53</v>
-      </c>
-      <c t="s" s="7" r="G7">
-        <v>54</v>
-      </c>
-      <c t="s" s="7" r="H7">
-        <v>55</v>
-      </c>
-      <c t="s" s="3" r="I7">
         <v>56</v>
+      </c>
+      <c t="s" s="7" r="D7">
+        <v>57</v>
+      </c>
+      <c t="s" s="7" r="E7">
+        <v>58</v>
+      </c>
+      <c t="s" s="7" r="F7">
+        <v>59</v>
+      </c>
+      <c t="s" s="8" r="G7">
+        <v>60</v>
+      </c>
+      <c t="s" s="8" r="H7">
+        <v>61</v>
+      </c>
+      <c t="s" s="9" r="I7">
+        <v>62</v>
+      </c>
+      <c t="s" s="9" r="J7">
+        <v>63</v>
       </c>
     </row>
     <row r="8">
@@ -657,28 +729,31 @@
         <v>6.0</v>
       </c>
       <c t="s" s="5" r="B8">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c t="s" s="6" r="C8">
-        <v>58</v>
-      </c>
-      <c t="s" s="5" r="D8">
-        <v>59</v>
-      </c>
-      <c t="s" s="5" r="E8">
-        <v>60</v>
-      </c>
-      <c t="s" s="5" r="F8">
-        <v>61</v>
-      </c>
-      <c t="s" s="7" r="G8">
-        <v>62</v>
-      </c>
-      <c t="s" s="7" r="H8">
-        <v>63</v>
-      </c>
-      <c t="s" s="3" r="I8">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c t="s" s="7" r="D8">
+        <v>66</v>
+      </c>
+      <c t="s" s="7" r="E8">
+        <v>67</v>
+      </c>
+      <c t="s" s="7" r="F8">
+        <v>68</v>
+      </c>
+      <c t="s" s="8" r="G8">
+        <v>69</v>
+      </c>
+      <c t="s" s="8" r="H8">
+        <v>70</v>
+      </c>
+      <c t="s" s="9" r="I8">
+        <v>71</v>
+      </c>
+      <c t="s" s="9" r="J8">
+        <v>72</v>
       </c>
     </row>
     <row r="9">
@@ -686,28 +761,31 @@
         <v>7.0</v>
       </c>
       <c t="s" s="5" r="B9">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c t="s" s="6" r="C9">
-        <v>66</v>
-      </c>
-      <c t="s" s="5" r="D9">
-        <v>67</v>
-      </c>
-      <c t="s" s="5" r="E9">
-        <v>68</v>
-      </c>
-      <c t="s" s="5" r="F9">
-        <v>69</v>
-      </c>
-      <c t="s" s="7" r="G9">
-        <v>70</v>
-      </c>
-      <c t="s" s="7" r="H9">
-        <v>71</v>
-      </c>
-      <c t="s" s="3" r="I9">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c t="s" s="7" r="D9">
+        <v>75</v>
+      </c>
+      <c t="s" s="7" r="E9">
+        <v>76</v>
+      </c>
+      <c t="s" s="7" r="F9">
+        <v>77</v>
+      </c>
+      <c t="s" s="8" r="G9">
+        <v>78</v>
+      </c>
+      <c t="s" s="8" r="H9">
+        <v>79</v>
+      </c>
+      <c t="s" s="9" r="I9">
+        <v>80</v>
+      </c>
+      <c t="s" s="9" r="J9">
+        <v>81</v>
       </c>
     </row>
     <row r="10">
@@ -715,28 +793,31 @@
         <v>8.0</v>
       </c>
       <c t="s" s="5" r="B10">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c t="s" s="6" r="C10">
-        <v>74</v>
-      </c>
-      <c t="s" s="5" r="D10">
-        <v>75</v>
-      </c>
-      <c t="s" s="5" r="E10">
-        <v>76</v>
-      </c>
-      <c t="s" s="5" r="F10">
-        <v>77</v>
-      </c>
-      <c t="s" s="7" r="G10">
-        <v>78</v>
-      </c>
-      <c t="s" s="7" r="H10">
-        <v>79</v>
-      </c>
-      <c t="s" s="3" r="I10">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c t="s" s="7" r="D10">
+        <v>84</v>
+      </c>
+      <c t="s" s="7" r="E10">
+        <v>85</v>
+      </c>
+      <c t="s" s="7" r="F10">
+        <v>86</v>
+      </c>
+      <c t="s" s="8" r="G10">
+        <v>87</v>
+      </c>
+      <c t="s" s="8" r="H10">
+        <v>88</v>
+      </c>
+      <c t="s" s="9" r="I10">
+        <v>89</v>
+      </c>
+      <c t="s" s="9" r="J10">
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -744,28 +825,31 @@
         <v>9.0</v>
       </c>
       <c t="s" s="5" r="B11">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c t="s" s="6" r="C11">
-        <v>82</v>
-      </c>
-      <c t="s" s="5" r="D11">
-        <v>83</v>
-      </c>
-      <c t="s" s="5" r="E11">
-        <v>84</v>
-      </c>
-      <c t="s" s="5" r="F11">
-        <v>85</v>
-      </c>
-      <c t="s" s="7" r="G11">
-        <v>86</v>
-      </c>
-      <c t="s" s="7" r="H11">
-        <v>87</v>
-      </c>
-      <c t="s" s="3" r="I11">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c t="s" s="7" r="D11">
+        <v>93</v>
+      </c>
+      <c t="s" s="7" r="E11">
+        <v>94</v>
+      </c>
+      <c t="s" s="7" r="F11">
+        <v>95</v>
+      </c>
+      <c t="s" s="8" r="G11">
+        <v>96</v>
+      </c>
+      <c t="s" s="8" r="H11">
+        <v>97</v>
+      </c>
+      <c t="s" s="9" r="I11">
+        <v>98</v>
+      </c>
+      <c t="s" s="9" r="J11">
+        <v>99</v>
       </c>
     </row>
     <row r="12">
@@ -773,28 +857,31 @@
         <v>10.0</v>
       </c>
       <c t="s" s="5" r="B12">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c t="s" s="6" r="C12">
-        <v>90</v>
-      </c>
-      <c t="s" s="5" r="D12">
-        <v>91</v>
-      </c>
-      <c t="s" s="5" r="E12">
-        <v>92</v>
-      </c>
-      <c t="s" s="5" r="F12">
-        <v>93</v>
-      </c>
-      <c t="s" s="7" r="G12">
-        <v>94</v>
-      </c>
-      <c t="s" s="7" r="H12">
-        <v>95</v>
-      </c>
-      <c t="s" s="3" r="I12">
-        <v>96</v>
+        <v>101</v>
+      </c>
+      <c t="s" s="7" r="D12">
+        <v>102</v>
+      </c>
+      <c t="s" s="7" r="E12">
+        <v>103</v>
+      </c>
+      <c t="s" s="7" r="F12">
+        <v>104</v>
+      </c>
+      <c t="s" s="8" r="G12">
+        <v>105</v>
+      </c>
+      <c t="s" s="8" r="H12">
+        <v>106</v>
+      </c>
+      <c t="s" s="9" r="I12">
+        <v>107</v>
+      </c>
+      <c t="s" s="9" r="J12">
+        <v>108</v>
       </c>
     </row>
     <row r="13">
@@ -802,28 +889,31 @@
         <v>11.0</v>
       </c>
       <c t="s" s="5" r="B13">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c t="s" s="6" r="C13">
-        <v>98</v>
-      </c>
-      <c t="s" s="5" r="D13">
-        <v>99</v>
-      </c>
-      <c t="s" s="5" r="E13">
-        <v>100</v>
-      </c>
-      <c t="s" s="5" r="F13">
-        <v>101</v>
-      </c>
-      <c t="s" s="7" r="G13">
-        <v>102</v>
-      </c>
-      <c t="s" s="7" r="H13">
-        <v>103</v>
-      </c>
-      <c t="s" s="3" r="I13">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c t="s" s="7" r="D13">
+        <v>111</v>
+      </c>
+      <c t="s" s="7" r="E13">
+        <v>112</v>
+      </c>
+      <c t="s" s="7" r="F13">
+        <v>113</v>
+      </c>
+      <c t="s" s="8" r="G13">
+        <v>114</v>
+      </c>
+      <c t="s" s="8" r="H13">
+        <v>115</v>
+      </c>
+      <c t="s" s="9" r="I13">
+        <v>116</v>
+      </c>
+      <c t="s" s="9" r="J13">
+        <v>117</v>
       </c>
     </row>
     <row r="14">
@@ -831,2987 +921,2990 @@
         <v>12.0</v>
       </c>
       <c t="s" s="5" r="B14">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c t="s" s="6" r="C14">
-        <v>106</v>
-      </c>
-      <c t="s" s="5" r="D14">
-        <v>107</v>
-      </c>
-      <c t="s" s="5" r="E14">
-        <v>108</v>
-      </c>
-      <c t="s" s="5" r="F14">
-        <v>109</v>
-      </c>
-      <c t="s" s="7" r="G14">
-        <v>110</v>
-      </c>
-      <c t="s" s="7" r="H14">
-        <v>111</v>
-      </c>
-      <c t="s" s="3" r="I14">
-        <v>112</v>
+        <v>119</v>
+      </c>
+      <c t="s" s="7" r="D14">
+        <v>120</v>
+      </c>
+      <c t="s" s="7" r="E14">
+        <v>121</v>
+      </c>
+      <c t="s" s="7" r="F14">
+        <v>122</v>
+      </c>
+      <c t="s" s="8" r="G14">
+        <v>123</v>
+      </c>
+      <c t="s" s="8" r="H14">
+        <v>124</v>
+      </c>
+      <c t="s" s="9" r="I14">
+        <v>125</v>
+      </c>
+      <c t="s" s="9" r="J14">
+        <v>126</v>
       </c>
     </row>
     <row r="15">
-      <c s="8" r="A15"/>
+      <c s="10" r="A15"/>
     </row>
     <row r="16">
-      <c s="8" r="A16"/>
+      <c s="10" r="A16"/>
     </row>
     <row r="17">
-      <c s="8" r="A17"/>
+      <c s="10" r="A17"/>
     </row>
     <row r="18">
-      <c s="8" r="A18"/>
+      <c s="10" r="A18"/>
     </row>
     <row r="19">
-      <c s="8" r="A19"/>
+      <c s="10" r="A19"/>
     </row>
     <row r="20">
-      <c s="8" r="A20"/>
+      <c s="10" r="A20"/>
     </row>
     <row r="21">
-      <c s="8" r="A21"/>
+      <c s="10" r="A21"/>
     </row>
     <row r="22">
-      <c s="8" r="A22"/>
+      <c s="10" r="A22"/>
     </row>
     <row r="23">
-      <c s="8" r="A23"/>
+      <c s="10" r="A23"/>
     </row>
     <row r="24">
-      <c s="8" r="A24"/>
+      <c s="10" r="A24"/>
     </row>
     <row r="25">
-      <c s="8" r="A25"/>
+      <c s="10" r="A25"/>
     </row>
     <row r="26">
-      <c s="8" r="A26"/>
+      <c s="10" r="A26"/>
     </row>
     <row r="27">
-      <c s="8" r="A27"/>
+      <c s="10" r="A27"/>
     </row>
     <row r="28">
-      <c s="8" r="A28"/>
+      <c s="10" r="A28"/>
     </row>
     <row r="29">
-      <c s="8" r="A29"/>
+      <c s="10" r="A29"/>
     </row>
     <row r="30">
-      <c s="8" r="A30"/>
+      <c s="10" r="A30"/>
     </row>
     <row r="31">
-      <c s="8" r="A31"/>
+      <c s="10" r="A31"/>
     </row>
     <row r="32">
-      <c s="8" r="A32"/>
+      <c s="10" r="A32"/>
     </row>
     <row r="33">
-      <c s="8" r="A33"/>
+      <c s="10" r="A33"/>
     </row>
     <row r="34">
-      <c s="8" r="A34"/>
+      <c s="10" r="A34"/>
     </row>
     <row r="35">
-      <c s="8" r="A35"/>
+      <c s="10" r="A35"/>
     </row>
     <row r="36">
-      <c s="8" r="A36"/>
+      <c s="10" r="A36"/>
     </row>
     <row r="37">
-      <c s="8" r="A37"/>
+      <c s="10" r="A37"/>
     </row>
     <row r="38">
-      <c s="8" r="A38"/>
+      <c s="10" r="A38"/>
     </row>
     <row r="39">
-      <c s="8" r="A39"/>
+      <c s="10" r="A39"/>
     </row>
     <row r="40">
-      <c s="8" r="A40"/>
+      <c s="10" r="A40"/>
     </row>
     <row r="41">
-      <c s="8" r="A41"/>
+      <c s="10" r="A41"/>
     </row>
     <row r="42">
-      <c s="8" r="A42"/>
+      <c s="10" r="A42"/>
     </row>
     <row r="43">
-      <c s="8" r="A43"/>
+      <c s="10" r="A43"/>
     </row>
     <row r="44">
-      <c s="8" r="A44"/>
+      <c s="10" r="A44"/>
     </row>
     <row r="45">
-      <c s="8" r="A45"/>
+      <c s="10" r="A45"/>
     </row>
     <row r="46">
-      <c s="8" r="A46"/>
+      <c s="10" r="A46"/>
     </row>
     <row r="47">
-      <c s="8" r="A47"/>
+      <c s="10" r="A47"/>
     </row>
     <row r="48">
-      <c s="8" r="A48"/>
+      <c s="10" r="A48"/>
     </row>
     <row r="49">
-      <c s="8" r="A49"/>
+      <c s="10" r="A49"/>
     </row>
     <row r="50">
-      <c s="8" r="A50"/>
+      <c s="10" r="A50"/>
     </row>
     <row r="51">
-      <c s="8" r="A51"/>
+      <c s="10" r="A51"/>
     </row>
     <row r="52">
-      <c s="8" r="A52"/>
+      <c s="10" r="A52"/>
     </row>
     <row r="53">
-      <c s="8" r="A53"/>
+      <c s="10" r="A53"/>
     </row>
     <row r="54">
-      <c s="8" r="A54"/>
+      <c s="10" r="A54"/>
     </row>
     <row r="55">
-      <c s="8" r="A55"/>
+      <c s="10" r="A55"/>
     </row>
     <row r="56">
-      <c s="8" r="A56"/>
+      <c s="10" r="A56"/>
     </row>
     <row r="57">
-      <c s="8" r="A57"/>
+      <c s="10" r="A57"/>
     </row>
     <row r="58">
-      <c s="8" r="A58"/>
+      <c s="10" r="A58"/>
     </row>
     <row r="59">
-      <c s="8" r="A59"/>
+      <c s="10" r="A59"/>
     </row>
     <row r="60">
-      <c s="8" r="A60"/>
+      <c s="10" r="A60"/>
     </row>
     <row r="61">
-      <c s="8" r="A61"/>
+      <c s="10" r="A61"/>
     </row>
     <row r="62">
-      <c s="8" r="A62"/>
+      <c s="10" r="A62"/>
     </row>
     <row r="63">
-      <c s="8" r="A63"/>
+      <c s="10" r="A63"/>
     </row>
     <row r="64">
-      <c s="8" r="A64"/>
+      <c s="10" r="A64"/>
     </row>
     <row r="65">
-      <c s="8" r="A65"/>
+      <c s="10" r="A65"/>
     </row>
     <row r="66">
-      <c s="8" r="A66"/>
+      <c s="10" r="A66"/>
     </row>
     <row r="67">
-      <c s="8" r="A67"/>
+      <c s="10" r="A67"/>
     </row>
     <row r="68">
-      <c s="8" r="A68"/>
+      <c s="10" r="A68"/>
     </row>
     <row r="69">
-      <c s="8" r="A69"/>
+      <c s="10" r="A69"/>
     </row>
     <row r="70">
-      <c s="8" r="A70"/>
+      <c s="10" r="A70"/>
     </row>
     <row r="71">
-      <c s="8" r="A71"/>
+      <c s="10" r="A71"/>
     </row>
     <row r="72">
-      <c s="8" r="A72"/>
+      <c s="10" r="A72"/>
     </row>
     <row r="73">
-      <c s="8" r="A73"/>
+      <c s="10" r="A73"/>
     </row>
     <row r="74">
-      <c s="8" r="A74"/>
+      <c s="10" r="A74"/>
     </row>
     <row r="75">
-      <c s="8" r="A75"/>
+      <c s="10" r="A75"/>
     </row>
     <row r="76">
-      <c s="8" r="A76"/>
+      <c s="10" r="A76"/>
     </row>
     <row r="77">
-      <c s="8" r="A77"/>
+      <c s="10" r="A77"/>
     </row>
     <row r="78">
-      <c s="8" r="A78"/>
+      <c s="10" r="A78"/>
     </row>
     <row r="79">
-      <c s="8" r="A79"/>
+      <c s="10" r="A79"/>
     </row>
     <row r="80">
-      <c s="8" r="A80"/>
+      <c s="10" r="A80"/>
     </row>
     <row r="81">
-      <c s="8" r="A81"/>
+      <c s="10" r="A81"/>
     </row>
     <row r="82">
-      <c s="8" r="A82"/>
+      <c s="10" r="A82"/>
     </row>
     <row r="83">
-      <c s="8" r="A83"/>
+      <c s="10" r="A83"/>
     </row>
     <row r="84">
-      <c s="8" r="A84"/>
+      <c s="10" r="A84"/>
     </row>
     <row r="85">
-      <c s="8" r="A85"/>
+      <c s="10" r="A85"/>
     </row>
     <row r="86">
-      <c s="8" r="A86"/>
+      <c s="10" r="A86"/>
     </row>
     <row r="87">
-      <c s="8" r="A87"/>
+      <c s="10" r="A87"/>
     </row>
     <row r="88">
-      <c s="8" r="A88"/>
+      <c s="10" r="A88"/>
     </row>
     <row r="89">
-      <c s="8" r="A89"/>
+      <c s="10" r="A89"/>
     </row>
     <row r="90">
-      <c s="8" r="A90"/>
+      <c s="10" r="A90"/>
     </row>
     <row r="91">
-      <c s="8" r="A91"/>
+      <c s="10" r="A91"/>
     </row>
     <row r="92">
-      <c s="8" r="A92"/>
+      <c s="10" r="A92"/>
     </row>
     <row r="93">
-      <c s="8" r="A93"/>
+      <c s="10" r="A93"/>
     </row>
     <row r="94">
-      <c s="8" r="A94"/>
+      <c s="10" r="A94"/>
     </row>
     <row r="95">
-      <c s="8" r="A95"/>
+      <c s="10" r="A95"/>
     </row>
     <row r="96">
-      <c s="8" r="A96"/>
+      <c s="10" r="A96"/>
     </row>
     <row r="97">
-      <c s="8" r="A97"/>
+      <c s="10" r="A97"/>
     </row>
     <row r="98">
-      <c s="8" r="A98"/>
+      <c s="10" r="A98"/>
     </row>
     <row r="99">
-      <c s="8" r="A99"/>
+      <c s="10" r="A99"/>
     </row>
     <row r="100">
-      <c s="8" r="A100"/>
+      <c s="10" r="A100"/>
     </row>
     <row r="101">
-      <c s="8" r="A101"/>
+      <c s="10" r="A101"/>
     </row>
     <row r="102">
-      <c s="8" r="A102"/>
+      <c s="10" r="A102"/>
     </row>
     <row r="103">
-      <c s="8" r="A103"/>
+      <c s="10" r="A103"/>
     </row>
     <row r="104">
-      <c s="8" r="A104"/>
+      <c s="10" r="A104"/>
     </row>
     <row r="105">
-      <c s="8" r="A105"/>
+      <c s="10" r="A105"/>
     </row>
     <row r="106">
-      <c s="8" r="A106"/>
+      <c s="10" r="A106"/>
     </row>
     <row r="107">
-      <c s="8" r="A107"/>
+      <c s="10" r="A107"/>
     </row>
     <row r="108">
-      <c s="8" r="A108"/>
+      <c s="10" r="A108"/>
     </row>
     <row r="109">
-      <c s="8" r="A109"/>
+      <c s="10" r="A109"/>
     </row>
     <row r="110">
-      <c s="8" r="A110"/>
+      <c s="10" r="A110"/>
     </row>
     <row r="111">
-      <c s="8" r="A111"/>
+      <c s="10" r="A111"/>
     </row>
     <row r="112">
-      <c s="8" r="A112"/>
+      <c s="10" r="A112"/>
     </row>
     <row r="113">
-      <c s="8" r="A113"/>
+      <c s="10" r="A113"/>
     </row>
     <row r="114">
-      <c s="8" r="A114"/>
+      <c s="10" r="A114"/>
     </row>
     <row r="115">
-      <c s="8" r="A115"/>
+      <c s="10" r="A115"/>
     </row>
     <row r="116">
-      <c s="8" r="A116"/>
+      <c s="10" r="A116"/>
     </row>
     <row r="117">
-      <c s="8" r="A117"/>
+      <c s="10" r="A117"/>
     </row>
     <row r="118">
-      <c s="8" r="A118"/>
+      <c s="10" r="A118"/>
     </row>
     <row r="119">
-      <c s="8" r="A119"/>
+      <c s="10" r="A119"/>
     </row>
     <row r="120">
-      <c s="8" r="A120"/>
+      <c s="10" r="A120"/>
     </row>
     <row r="121">
-      <c s="8" r="A121"/>
+      <c s="10" r="A121"/>
     </row>
     <row r="122">
-      <c s="8" r="A122"/>
+      <c s="10" r="A122"/>
     </row>
     <row r="123">
-      <c s="8" r="A123"/>
+      <c s="10" r="A123"/>
     </row>
     <row r="124">
-      <c s="8" r="A124"/>
+      <c s="10" r="A124"/>
     </row>
     <row r="125">
-      <c s="8" r="A125"/>
+      <c s="10" r="A125"/>
     </row>
     <row r="126">
-      <c s="8" r="A126"/>
+      <c s="10" r="A126"/>
     </row>
     <row r="127">
-      <c s="8" r="A127"/>
+      <c s="10" r="A127"/>
     </row>
     <row r="128">
-      <c s="8" r="A128"/>
+      <c s="10" r="A128"/>
     </row>
     <row r="129">
-      <c s="8" r="A129"/>
+      <c s="10" r="A129"/>
     </row>
     <row r="130">
-      <c s="8" r="A130"/>
+      <c s="10" r="A130"/>
     </row>
     <row r="131">
-      <c s="8" r="A131"/>
+      <c s="10" r="A131"/>
     </row>
     <row r="132">
-      <c s="8" r="A132"/>
+      <c s="10" r="A132"/>
     </row>
     <row r="133">
-      <c s="8" r="A133"/>
+      <c s="10" r="A133"/>
     </row>
     <row r="134">
-      <c s="8" r="A134"/>
+      <c s="10" r="A134"/>
     </row>
     <row r="135">
-      <c s="8" r="A135"/>
+      <c s="10" r="A135"/>
     </row>
     <row r="136">
-      <c s="8" r="A136"/>
+      <c s="10" r="A136"/>
     </row>
     <row r="137">
-      <c s="8" r="A137"/>
+      <c s="10" r="A137"/>
     </row>
     <row r="138">
-      <c s="8" r="A138"/>
+      <c s="10" r="A138"/>
     </row>
     <row r="139">
-      <c s="8" r="A139"/>
+      <c s="10" r="A139"/>
     </row>
     <row r="140">
-      <c s="8" r="A140"/>
+      <c s="10" r="A140"/>
     </row>
     <row r="141">
-      <c s="8" r="A141"/>
+      <c s="10" r="A141"/>
     </row>
     <row r="142">
-      <c s="8" r="A142"/>
+      <c s="10" r="A142"/>
     </row>
     <row r="143">
-      <c s="8" r="A143"/>
+      <c s="10" r="A143"/>
     </row>
     <row r="144">
-      <c s="8" r="A144"/>
+      <c s="10" r="A144"/>
     </row>
     <row r="145">
-      <c s="8" r="A145"/>
+      <c s="10" r="A145"/>
     </row>
     <row r="146">
-      <c s="8" r="A146"/>
+      <c s="10" r="A146"/>
     </row>
     <row r="147">
-      <c s="8" r="A147"/>
+      <c s="10" r="A147"/>
     </row>
     <row r="148">
-      <c s="8" r="A148"/>
+      <c s="10" r="A148"/>
     </row>
     <row r="149">
-      <c s="8" r="A149"/>
+      <c s="10" r="A149"/>
     </row>
     <row r="150">
-      <c s="8" r="A150"/>
+      <c s="10" r="A150"/>
     </row>
     <row r="151">
-      <c s="8" r="A151"/>
+      <c s="10" r="A151"/>
     </row>
     <row r="152">
-      <c s="8" r="A152"/>
+      <c s="10" r="A152"/>
     </row>
     <row r="153">
-      <c s="8" r="A153"/>
+      <c s="10" r="A153"/>
     </row>
     <row r="154">
-      <c s="8" r="A154"/>
+      <c s="10" r="A154"/>
     </row>
     <row r="155">
-      <c s="8" r="A155"/>
+      <c s="10" r="A155"/>
     </row>
     <row r="156">
-      <c s="8" r="A156"/>
+      <c s="10" r="A156"/>
     </row>
     <row r="157">
-      <c s="8" r="A157"/>
+      <c s="10" r="A157"/>
     </row>
     <row r="158">
-      <c s="8" r="A158"/>
+      <c s="10" r="A158"/>
     </row>
     <row r="159">
-      <c s="8" r="A159"/>
+      <c s="10" r="A159"/>
     </row>
     <row r="160">
-      <c s="8" r="A160"/>
+      <c s="10" r="A160"/>
     </row>
     <row r="161">
-      <c s="8" r="A161"/>
+      <c s="10" r="A161"/>
     </row>
     <row r="162">
-      <c s="8" r="A162"/>
+      <c s="10" r="A162"/>
     </row>
     <row r="163">
-      <c s="8" r="A163"/>
+      <c s="10" r="A163"/>
     </row>
     <row r="164">
-      <c s="8" r="A164"/>
+      <c s="10" r="A164"/>
     </row>
     <row r="165">
-      <c s="8" r="A165"/>
+      <c s="10" r="A165"/>
     </row>
     <row r="166">
-      <c s="8" r="A166"/>
+      <c s="10" r="A166"/>
     </row>
     <row r="167">
-      <c s="8" r="A167"/>
+      <c s="10" r="A167"/>
     </row>
     <row r="168">
-      <c s="8" r="A168"/>
+      <c s="10" r="A168"/>
     </row>
     <row r="169">
-      <c s="8" r="A169"/>
+      <c s="10" r="A169"/>
     </row>
     <row r="170">
-      <c s="8" r="A170"/>
+      <c s="10" r="A170"/>
     </row>
     <row r="171">
-      <c s="8" r="A171"/>
+      <c s="10" r="A171"/>
     </row>
     <row r="172">
-      <c s="8" r="A172"/>
+      <c s="10" r="A172"/>
     </row>
     <row r="173">
-      <c s="8" r="A173"/>
+      <c s="10" r="A173"/>
     </row>
     <row r="174">
-      <c s="8" r="A174"/>
+      <c s="10" r="A174"/>
     </row>
     <row r="175">
-      <c s="8" r="A175"/>
+      <c s="10" r="A175"/>
     </row>
     <row r="176">
-      <c s="8" r="A176"/>
+      <c s="10" r="A176"/>
     </row>
     <row r="177">
-      <c s="8" r="A177"/>
+      <c s="10" r="A177"/>
     </row>
     <row r="178">
-      <c s="8" r="A178"/>
+      <c s="10" r="A178"/>
     </row>
     <row r="179">
-      <c s="8" r="A179"/>
+      <c s="10" r="A179"/>
     </row>
     <row r="180">
-      <c s="8" r="A180"/>
+      <c s="10" r="A180"/>
     </row>
     <row r="181">
-      <c s="8" r="A181"/>
+      <c s="10" r="A181"/>
     </row>
     <row r="182">
-      <c s="8" r="A182"/>
+      <c s="10" r="A182"/>
     </row>
     <row r="183">
-      <c s="8" r="A183"/>
+      <c s="10" r="A183"/>
     </row>
     <row r="184">
-      <c s="8" r="A184"/>
+      <c s="10" r="A184"/>
     </row>
     <row r="185">
-      <c s="8" r="A185"/>
+      <c s="10" r="A185"/>
     </row>
     <row r="186">
-      <c s="8" r="A186"/>
+      <c s="10" r="A186"/>
     </row>
     <row r="187">
-      <c s="8" r="A187"/>
+      <c s="10" r="A187"/>
     </row>
     <row r="188">
-      <c s="8" r="A188"/>
+      <c s="10" r="A188"/>
     </row>
     <row r="189">
-      <c s="8" r="A189"/>
+      <c s="10" r="A189"/>
     </row>
     <row r="190">
-      <c s="8" r="A190"/>
+      <c s="10" r="A190"/>
     </row>
     <row r="191">
-      <c s="8" r="A191"/>
+      <c s="10" r="A191"/>
     </row>
     <row r="192">
-      <c s="8" r="A192"/>
+      <c s="10" r="A192"/>
     </row>
     <row r="193">
-      <c s="8" r="A193"/>
+      <c s="10" r="A193"/>
     </row>
     <row r="194">
-      <c s="8" r="A194"/>
+      <c s="10" r="A194"/>
     </row>
     <row r="195">
-      <c s="8" r="A195"/>
+      <c s="10" r="A195"/>
     </row>
     <row r="196">
-      <c s="8" r="A196"/>
+      <c s="10" r="A196"/>
     </row>
     <row r="197">
-      <c s="8" r="A197"/>
+      <c s="10" r="A197"/>
     </row>
     <row r="198">
-      <c s="8" r="A198"/>
+      <c s="10" r="A198"/>
     </row>
     <row r="199">
-      <c s="8" r="A199"/>
+      <c s="10" r="A199"/>
     </row>
     <row r="200">
-      <c s="8" r="A200"/>
+      <c s="10" r="A200"/>
     </row>
     <row r="201">
-      <c s="8" r="A201"/>
+      <c s="10" r="A201"/>
     </row>
     <row r="202">
-      <c s="8" r="A202"/>
+      <c s="10" r="A202"/>
     </row>
     <row r="203">
-      <c s="8" r="A203"/>
+      <c s="10" r="A203"/>
     </row>
     <row r="204">
-      <c s="8" r="A204"/>
+      <c s="10" r="A204"/>
     </row>
     <row r="205">
-      <c s="8" r="A205"/>
+      <c s="10" r="A205"/>
     </row>
     <row r="206">
-      <c s="8" r="A206"/>
+      <c s="10" r="A206"/>
     </row>
     <row r="207">
-      <c s="8" r="A207"/>
+      <c s="10" r="A207"/>
     </row>
     <row r="208">
-      <c s="8" r="A208"/>
+      <c s="10" r="A208"/>
     </row>
     <row r="209">
-      <c s="8" r="A209"/>
+      <c s="10" r="A209"/>
     </row>
     <row r="210">
-      <c s="8" r="A210"/>
+      <c s="10" r="A210"/>
     </row>
     <row r="211">
-      <c s="8" r="A211"/>
+      <c s="10" r="A211"/>
     </row>
     <row r="212">
-      <c s="8" r="A212"/>
+      <c s="10" r="A212"/>
     </row>
     <row r="213">
-      <c s="8" r="A213"/>
+      <c s="10" r="A213"/>
     </row>
     <row r="214">
-      <c s="8" r="A214"/>
+      <c s="10" r="A214"/>
     </row>
     <row r="215">
-      <c s="8" r="A215"/>
+      <c s="10" r="A215"/>
     </row>
     <row r="216">
-      <c s="8" r="A216"/>
+      <c s="10" r="A216"/>
     </row>
     <row r="217">
-      <c s="8" r="A217"/>
+      <c s="10" r="A217"/>
     </row>
     <row r="218">
-      <c s="8" r="A218"/>
+      <c s="10" r="A218"/>
     </row>
     <row r="219">
-      <c s="8" r="A219"/>
+      <c s="10" r="A219"/>
     </row>
     <row r="220">
-      <c s="8" r="A220"/>
+      <c s="10" r="A220"/>
     </row>
     <row r="221">
-      <c s="8" r="A221"/>
+      <c s="10" r="A221"/>
     </row>
     <row r="222">
-      <c s="8" r="A222"/>
+      <c s="10" r="A222"/>
     </row>
     <row r="223">
-      <c s="8" r="A223"/>
+      <c s="10" r="A223"/>
     </row>
     <row r="224">
-      <c s="8" r="A224"/>
+      <c s="10" r="A224"/>
     </row>
     <row r="225">
-      <c s="8" r="A225"/>
+      <c s="10" r="A225"/>
     </row>
     <row r="226">
-      <c s="8" r="A226"/>
+      <c s="10" r="A226"/>
     </row>
     <row r="227">
-      <c s="8" r="A227"/>
+      <c s="10" r="A227"/>
     </row>
     <row r="228">
-      <c s="8" r="A228"/>
+      <c s="10" r="A228"/>
     </row>
     <row r="229">
-      <c s="8" r="A229"/>
+      <c s="10" r="A229"/>
     </row>
     <row r="230">
-      <c s="8" r="A230"/>
+      <c s="10" r="A230"/>
     </row>
     <row r="231">
-      <c s="8" r="A231"/>
+      <c s="10" r="A231"/>
     </row>
     <row r="232">
-      <c s="8" r="A232"/>
+      <c s="10" r="A232"/>
     </row>
     <row r="233">
-      <c s="8" r="A233"/>
+      <c s="10" r="A233"/>
     </row>
     <row r="234">
-      <c s="8" r="A234"/>
+      <c s="10" r="A234"/>
     </row>
     <row r="235">
-      <c s="8" r="A235"/>
+      <c s="10" r="A235"/>
     </row>
     <row r="236">
-      <c s="8" r="A236"/>
+      <c s="10" r="A236"/>
     </row>
     <row r="237">
-      <c s="8" r="A237"/>
+      <c s="10" r="A237"/>
     </row>
     <row r="238">
-      <c s="8" r="A238"/>
+      <c s="10" r="A238"/>
     </row>
     <row r="239">
-      <c s="8" r="A239"/>
+      <c s="10" r="A239"/>
     </row>
     <row r="240">
-      <c s="8" r="A240"/>
+      <c s="10" r="A240"/>
     </row>
     <row r="241">
-      <c s="8" r="A241"/>
+      <c s="10" r="A241"/>
     </row>
     <row r="242">
-      <c s="8" r="A242"/>
+      <c s="10" r="A242"/>
     </row>
     <row r="243">
-      <c s="8" r="A243"/>
+      <c s="10" r="A243"/>
     </row>
     <row r="244">
-      <c s="8" r="A244"/>
+      <c s="10" r="A244"/>
     </row>
     <row r="245">
-      <c s="8" r="A245"/>
+      <c s="10" r="A245"/>
     </row>
     <row r="246">
-      <c s="8" r="A246"/>
+      <c s="10" r="A246"/>
     </row>
     <row r="247">
-      <c s="8" r="A247"/>
+      <c s="10" r="A247"/>
     </row>
     <row r="248">
-      <c s="8" r="A248"/>
+      <c s="10" r="A248"/>
     </row>
     <row r="249">
-      <c s="8" r="A249"/>
+      <c s="10" r="A249"/>
     </row>
     <row r="250">
-      <c s="8" r="A250"/>
+      <c s="10" r="A250"/>
     </row>
     <row r="251">
-      <c s="8" r="A251"/>
+      <c s="10" r="A251"/>
     </row>
     <row r="252">
-      <c s="8" r="A252"/>
+      <c s="10" r="A252"/>
     </row>
     <row r="253">
-      <c s="8" r="A253"/>
+      <c s="10" r="A253"/>
     </row>
     <row r="254">
-      <c s="8" r="A254"/>
+      <c s="10" r="A254"/>
     </row>
     <row r="255">
-      <c s="8" r="A255"/>
+      <c s="10" r="A255"/>
     </row>
     <row r="256">
-      <c s="8" r="A256"/>
+      <c s="10" r="A256"/>
     </row>
     <row r="257">
-      <c s="8" r="A257"/>
+      <c s="10" r="A257"/>
     </row>
     <row r="258">
-      <c s="8" r="A258"/>
+      <c s="10" r="A258"/>
     </row>
     <row r="259">
-      <c s="8" r="A259"/>
+      <c s="10" r="A259"/>
     </row>
     <row r="260">
-      <c s="8" r="A260"/>
+      <c s="10" r="A260"/>
     </row>
     <row r="261">
-      <c s="8" r="A261"/>
+      <c s="10" r="A261"/>
     </row>
     <row r="262">
-      <c s="8" r="A262"/>
+      <c s="10" r="A262"/>
     </row>
     <row r="263">
-      <c s="8" r="A263"/>
+      <c s="10" r="A263"/>
     </row>
     <row r="264">
-      <c s="8" r="A264"/>
+      <c s="10" r="A264"/>
     </row>
     <row r="265">
-      <c s="8" r="A265"/>
+      <c s="10" r="A265"/>
     </row>
     <row r="266">
-      <c s="8" r="A266"/>
+      <c s="10" r="A266"/>
     </row>
     <row r="267">
-      <c s="8" r="A267"/>
+      <c s="10" r="A267"/>
     </row>
     <row r="268">
-      <c s="8" r="A268"/>
+      <c s="10" r="A268"/>
     </row>
     <row r="269">
-      <c s="8" r="A269"/>
+      <c s="10" r="A269"/>
     </row>
     <row r="270">
-      <c s="8" r="A270"/>
+      <c s="10" r="A270"/>
     </row>
     <row r="271">
-      <c s="8" r="A271"/>
+      <c s="10" r="A271"/>
     </row>
     <row r="272">
-      <c s="8" r="A272"/>
+      <c s="10" r="A272"/>
     </row>
     <row r="273">
-      <c s="8" r="A273"/>
+      <c s="10" r="A273"/>
     </row>
     <row r="274">
-      <c s="8" r="A274"/>
+      <c s="10" r="A274"/>
     </row>
     <row r="275">
-      <c s="8" r="A275"/>
+      <c s="10" r="A275"/>
     </row>
     <row r="276">
-      <c s="8" r="A276"/>
+      <c s="10" r="A276"/>
     </row>
     <row r="277">
-      <c s="8" r="A277"/>
+      <c s="10" r="A277"/>
     </row>
     <row r="278">
-      <c s="8" r="A278"/>
+      <c s="10" r="A278"/>
     </row>
     <row r="279">
-      <c s="8" r="A279"/>
+      <c s="10" r="A279"/>
     </row>
     <row r="280">
-      <c s="8" r="A280"/>
+      <c s="10" r="A280"/>
     </row>
     <row r="281">
-      <c s="8" r="A281"/>
+      <c s="10" r="A281"/>
     </row>
     <row r="282">
-      <c s="8" r="A282"/>
+      <c s="10" r="A282"/>
     </row>
     <row r="283">
-      <c s="8" r="A283"/>
+      <c s="10" r="A283"/>
     </row>
     <row r="284">
-      <c s="8" r="A284"/>
+      <c s="10" r="A284"/>
     </row>
     <row r="285">
-      <c s="8" r="A285"/>
+      <c s="10" r="A285"/>
     </row>
     <row r="286">
-      <c s="8" r="A286"/>
+      <c s="10" r="A286"/>
     </row>
     <row r="287">
-      <c s="8" r="A287"/>
+      <c s="10" r="A287"/>
     </row>
     <row r="288">
-      <c s="8" r="A288"/>
+      <c s="10" r="A288"/>
     </row>
     <row r="289">
-      <c s="8" r="A289"/>
+      <c s="10" r="A289"/>
     </row>
     <row r="290">
-      <c s="8" r="A290"/>
+      <c s="10" r="A290"/>
     </row>
     <row r="291">
-      <c s="8" r="A291"/>
+      <c s="10" r="A291"/>
     </row>
     <row r="292">
-      <c s="8" r="A292"/>
+      <c s="10" r="A292"/>
     </row>
     <row r="293">
-      <c s="8" r="A293"/>
+      <c s="10" r="A293"/>
     </row>
     <row r="294">
-      <c s="8" r="A294"/>
+      <c s="10" r="A294"/>
     </row>
     <row r="295">
-      <c s="8" r="A295"/>
+      <c s="10" r="A295"/>
     </row>
     <row r="296">
-      <c s="8" r="A296"/>
+      <c s="10" r="A296"/>
     </row>
     <row r="297">
-      <c s="8" r="A297"/>
+      <c s="10" r="A297"/>
     </row>
     <row r="298">
-      <c s="8" r="A298"/>
+      <c s="10" r="A298"/>
     </row>
     <row r="299">
-      <c s="8" r="A299"/>
+      <c s="10" r="A299"/>
     </row>
     <row r="300">
-      <c s="8" r="A300"/>
+      <c s="10" r="A300"/>
     </row>
     <row r="301">
-      <c s="8" r="A301"/>
+      <c s="10" r="A301"/>
     </row>
     <row r="302">
-      <c s="8" r="A302"/>
+      <c s="10" r="A302"/>
     </row>
     <row r="303">
-      <c s="8" r="A303"/>
+      <c s="10" r="A303"/>
     </row>
     <row r="304">
-      <c s="8" r="A304"/>
+      <c s="10" r="A304"/>
     </row>
     <row r="305">
-      <c s="8" r="A305"/>
+      <c s="10" r="A305"/>
     </row>
     <row r="306">
-      <c s="8" r="A306"/>
+      <c s="10" r="A306"/>
     </row>
     <row r="307">
-      <c s="8" r="A307"/>
+      <c s="10" r="A307"/>
     </row>
     <row r="308">
-      <c s="8" r="A308"/>
+      <c s="10" r="A308"/>
     </row>
     <row r="309">
-      <c s="8" r="A309"/>
+      <c s="10" r="A309"/>
     </row>
     <row r="310">
-      <c s="8" r="A310"/>
+      <c s="10" r="A310"/>
     </row>
     <row r="311">
-      <c s="8" r="A311"/>
+      <c s="10" r="A311"/>
     </row>
     <row r="312">
-      <c s="8" r="A312"/>
+      <c s="10" r="A312"/>
     </row>
     <row r="313">
-      <c s="8" r="A313"/>
+      <c s="10" r="A313"/>
     </row>
     <row r="314">
-      <c s="8" r="A314"/>
+      <c s="10" r="A314"/>
     </row>
     <row r="315">
-      <c s="8" r="A315"/>
+      <c s="10" r="A315"/>
     </row>
     <row r="316">
-      <c s="8" r="A316"/>
+      <c s="10" r="A316"/>
     </row>
     <row r="317">
-      <c s="8" r="A317"/>
+      <c s="10" r="A317"/>
     </row>
     <row r="318">
-      <c s="8" r="A318"/>
+      <c s="10" r="A318"/>
     </row>
     <row r="319">
-      <c s="8" r="A319"/>
+      <c s="10" r="A319"/>
     </row>
     <row r="320">
-      <c s="8" r="A320"/>
+      <c s="10" r="A320"/>
     </row>
     <row r="321">
-      <c s="8" r="A321"/>
+      <c s="10" r="A321"/>
     </row>
     <row r="322">
-      <c s="8" r="A322"/>
+      <c s="10" r="A322"/>
     </row>
     <row r="323">
-      <c s="8" r="A323"/>
+      <c s="10" r="A323"/>
     </row>
     <row r="324">
-      <c s="8" r="A324"/>
+      <c s="10" r="A324"/>
     </row>
     <row r="325">
-      <c s="8" r="A325"/>
+      <c s="10" r="A325"/>
     </row>
     <row r="326">
-      <c s="8" r="A326"/>
+      <c s="10" r="A326"/>
     </row>
     <row r="327">
-      <c s="8" r="A327"/>
+      <c s="10" r="A327"/>
     </row>
     <row r="328">
-      <c s="8" r="A328"/>
+      <c s="10" r="A328"/>
     </row>
     <row r="329">
-      <c s="8" r="A329"/>
+      <c s="10" r="A329"/>
     </row>
     <row r="330">
-      <c s="8" r="A330"/>
+      <c s="10" r="A330"/>
     </row>
     <row r="331">
-      <c s="8" r="A331"/>
+      <c s="10" r="A331"/>
     </row>
     <row r="332">
-      <c s="8" r="A332"/>
+      <c s="10" r="A332"/>
     </row>
     <row r="333">
-      <c s="8" r="A333"/>
+      <c s="10" r="A333"/>
     </row>
     <row r="334">
-      <c s="8" r="A334"/>
+      <c s="10" r="A334"/>
     </row>
     <row r="335">
-      <c s="8" r="A335"/>
+      <c s="10" r="A335"/>
     </row>
     <row r="336">
-      <c s="8" r="A336"/>
+      <c s="10" r="A336"/>
     </row>
     <row r="337">
-      <c s="8" r="A337"/>
+      <c s="10" r="A337"/>
     </row>
     <row r="338">
-      <c s="8" r="A338"/>
+      <c s="10" r="A338"/>
     </row>
     <row r="339">
-      <c s="8" r="A339"/>
+      <c s="10" r="A339"/>
     </row>
     <row r="340">
-      <c s="8" r="A340"/>
+      <c s="10" r="A340"/>
     </row>
     <row r="341">
-      <c s="8" r="A341"/>
+      <c s="10" r="A341"/>
     </row>
     <row r="342">
-      <c s="8" r="A342"/>
+      <c s="10" r="A342"/>
     </row>
     <row r="343">
-      <c s="8" r="A343"/>
+      <c s="10" r="A343"/>
     </row>
     <row r="344">
-      <c s="8" r="A344"/>
+      <c s="10" r="A344"/>
     </row>
     <row r="345">
-      <c s="8" r="A345"/>
+      <c s="10" r="A345"/>
     </row>
     <row r="346">
-      <c s="8" r="A346"/>
+      <c s="10" r="A346"/>
     </row>
     <row r="347">
-      <c s="8" r="A347"/>
+      <c s="10" r="A347"/>
     </row>
     <row r="348">
-      <c s="8" r="A348"/>
+      <c s="10" r="A348"/>
     </row>
     <row r="349">
-      <c s="8" r="A349"/>
+      <c s="10" r="A349"/>
     </row>
     <row r="350">
-      <c s="8" r="A350"/>
+      <c s="10" r="A350"/>
     </row>
     <row r="351">
-      <c s="8" r="A351"/>
+      <c s="10" r="A351"/>
     </row>
     <row r="352">
-      <c s="8" r="A352"/>
+      <c s="10" r="A352"/>
     </row>
     <row r="353">
-      <c s="8" r="A353"/>
+      <c s="10" r="A353"/>
     </row>
     <row r="354">
-      <c s="8" r="A354"/>
+      <c s="10" r="A354"/>
     </row>
     <row r="355">
-      <c s="8" r="A355"/>
+      <c s="10" r="A355"/>
     </row>
     <row r="356">
-      <c s="8" r="A356"/>
+      <c s="10" r="A356"/>
     </row>
     <row r="357">
-      <c s="8" r="A357"/>
+      <c s="10" r="A357"/>
     </row>
     <row r="358">
-      <c s="8" r="A358"/>
+      <c s="10" r="A358"/>
     </row>
     <row r="359">
-      <c s="8" r="A359"/>
+      <c s="10" r="A359"/>
     </row>
     <row r="360">
-      <c s="8" r="A360"/>
+      <c s="10" r="A360"/>
     </row>
     <row r="361">
-      <c s="8" r="A361"/>
+      <c s="10" r="A361"/>
     </row>
     <row r="362">
-      <c s="8" r="A362"/>
+      <c s="10" r="A362"/>
     </row>
     <row r="363">
-      <c s="8" r="A363"/>
+      <c s="10" r="A363"/>
     </row>
     <row r="364">
-      <c s="8" r="A364"/>
+      <c s="10" r="A364"/>
     </row>
     <row r="365">
-      <c s="8" r="A365"/>
+      <c s="10" r="A365"/>
     </row>
     <row r="366">
-      <c s="8" r="A366"/>
+      <c s="10" r="A366"/>
     </row>
     <row r="367">
-      <c s="8" r="A367"/>
+      <c s="10" r="A367"/>
     </row>
     <row r="368">
-      <c s="8" r="A368"/>
+      <c s="10" r="A368"/>
     </row>
     <row r="369">
-      <c s="8" r="A369"/>
+      <c s="10" r="A369"/>
     </row>
     <row r="370">
-      <c s="8" r="A370"/>
+      <c s="10" r="A370"/>
     </row>
     <row r="371">
-      <c s="8" r="A371"/>
+      <c s="10" r="A371"/>
     </row>
     <row r="372">
-      <c s="8" r="A372"/>
+      <c s="10" r="A372"/>
     </row>
     <row r="373">
-      <c s="8" r="A373"/>
+      <c s="10" r="A373"/>
     </row>
     <row r="374">
-      <c s="8" r="A374"/>
+      <c s="10" r="A374"/>
     </row>
     <row r="375">
-      <c s="8" r="A375"/>
+      <c s="10" r="A375"/>
     </row>
     <row r="376">
-      <c s="8" r="A376"/>
+      <c s="10" r="A376"/>
     </row>
     <row r="377">
-      <c s="8" r="A377"/>
+      <c s="10" r="A377"/>
     </row>
     <row r="378">
-      <c s="8" r="A378"/>
+      <c s="10" r="A378"/>
     </row>
     <row r="379">
-      <c s="8" r="A379"/>
+      <c s="10" r="A379"/>
     </row>
     <row r="380">
-      <c s="8" r="A380"/>
+      <c s="10" r="A380"/>
     </row>
     <row r="381">
-      <c s="8" r="A381"/>
+      <c s="10" r="A381"/>
     </row>
     <row r="382">
-      <c s="8" r="A382"/>
+      <c s="10" r="A382"/>
     </row>
     <row r="383">
-      <c s="8" r="A383"/>
+      <c s="10" r="A383"/>
     </row>
     <row r="384">
-      <c s="8" r="A384"/>
+      <c s="10" r="A384"/>
     </row>
     <row r="385">
-      <c s="8" r="A385"/>
+      <c s="10" r="A385"/>
     </row>
     <row r="386">
-      <c s="8" r="A386"/>
+      <c s="10" r="A386"/>
     </row>
     <row r="387">
-      <c s="8" r="A387"/>
+      <c s="10" r="A387"/>
     </row>
     <row r="388">
-      <c s="8" r="A388"/>
+      <c s="10" r="A388"/>
     </row>
     <row r="389">
-      <c s="8" r="A389"/>
+      <c s="10" r="A389"/>
     </row>
     <row r="390">
-      <c s="8" r="A390"/>
+      <c s="10" r="A390"/>
     </row>
     <row r="391">
-      <c s="8" r="A391"/>
+      <c s="10" r="A391"/>
     </row>
     <row r="392">
-      <c s="8" r="A392"/>
+      <c s="10" r="A392"/>
     </row>
     <row r="393">
-      <c s="8" r="A393"/>
+      <c s="10" r="A393"/>
     </row>
     <row r="394">
-      <c s="8" r="A394"/>
+      <c s="10" r="A394"/>
     </row>
     <row r="395">
-      <c s="8" r="A395"/>
+      <c s="10" r="A395"/>
     </row>
     <row r="396">
-      <c s="8" r="A396"/>
+      <c s="10" r="A396"/>
     </row>
     <row r="397">
-      <c s="8" r="A397"/>
+      <c s="10" r="A397"/>
     </row>
     <row r="398">
-      <c s="8" r="A398"/>
+      <c s="10" r="A398"/>
     </row>
     <row r="399">
-      <c s="8" r="A399"/>
+      <c s="10" r="A399"/>
     </row>
     <row r="400">
-      <c s="8" r="A400"/>
+      <c s="10" r="A400"/>
     </row>
     <row r="401">
-      <c s="8" r="A401"/>
+      <c s="10" r="A401"/>
     </row>
     <row r="402">
-      <c s="8" r="A402"/>
+      <c s="10" r="A402"/>
     </row>
     <row r="403">
-      <c s="8" r="A403"/>
+      <c s="10" r="A403"/>
     </row>
     <row r="404">
-      <c s="8" r="A404"/>
+      <c s="10" r="A404"/>
     </row>
     <row r="405">
-      <c s="8" r="A405"/>
+      <c s="10" r="A405"/>
     </row>
     <row r="406">
-      <c s="8" r="A406"/>
+      <c s="10" r="A406"/>
     </row>
     <row r="407">
-      <c s="8" r="A407"/>
+      <c s="10" r="A407"/>
     </row>
     <row r="408">
-      <c s="8" r="A408"/>
+      <c s="10" r="A408"/>
     </row>
     <row r="409">
-      <c s="8" r="A409"/>
+      <c s="10" r="A409"/>
     </row>
     <row r="410">
-      <c s="8" r="A410"/>
+      <c s="10" r="A410"/>
     </row>
     <row r="411">
-      <c s="8" r="A411"/>
+      <c s="10" r="A411"/>
     </row>
     <row r="412">
-      <c s="8" r="A412"/>
+      <c s="10" r="A412"/>
     </row>
     <row r="413">
-      <c s="8" r="A413"/>
+      <c s="10" r="A413"/>
     </row>
     <row r="414">
-      <c s="8" r="A414"/>
+      <c s="10" r="A414"/>
     </row>
     <row r="415">
-      <c s="8" r="A415"/>
+      <c s="10" r="A415"/>
     </row>
     <row r="416">
-      <c s="8" r="A416"/>
+      <c s="10" r="A416"/>
     </row>
     <row r="417">
-      <c s="8" r="A417"/>
+      <c s="10" r="A417"/>
     </row>
     <row r="418">
-      <c s="8" r="A418"/>
+      <c s="10" r="A418"/>
     </row>
     <row r="419">
-      <c s="8" r="A419"/>
+      <c s="10" r="A419"/>
     </row>
     <row r="420">
-      <c s="8" r="A420"/>
+      <c s="10" r="A420"/>
     </row>
     <row r="421">
-      <c s="8" r="A421"/>
+      <c s="10" r="A421"/>
     </row>
     <row r="422">
-      <c s="8" r="A422"/>
+      <c s="10" r="A422"/>
     </row>
     <row r="423">
-      <c s="8" r="A423"/>
+      <c s="10" r="A423"/>
     </row>
     <row r="424">
-      <c s="8" r="A424"/>
+      <c s="10" r="A424"/>
     </row>
     <row r="425">
-      <c s="8" r="A425"/>
+      <c s="10" r="A425"/>
     </row>
     <row r="426">
-      <c s="8" r="A426"/>
+      <c s="10" r="A426"/>
     </row>
     <row r="427">
-      <c s="8" r="A427"/>
+      <c s="10" r="A427"/>
     </row>
     <row r="428">
-      <c s="8" r="A428"/>
+      <c s="10" r="A428"/>
     </row>
     <row r="429">
-      <c s="8" r="A429"/>
+      <c s="10" r="A429"/>
     </row>
     <row r="430">
-      <c s="8" r="A430"/>
+      <c s="10" r="A430"/>
     </row>
     <row r="431">
-      <c s="8" r="A431"/>
+      <c s="10" r="A431"/>
     </row>
     <row r="432">
-      <c s="8" r="A432"/>
+      <c s="10" r="A432"/>
     </row>
     <row r="433">
-      <c s="8" r="A433"/>
+      <c s="10" r="A433"/>
     </row>
     <row r="434">
-      <c s="8" r="A434"/>
+      <c s="10" r="A434"/>
     </row>
     <row r="435">
-      <c s="8" r="A435"/>
+      <c s="10" r="A435"/>
     </row>
     <row r="436">
-      <c s="8" r="A436"/>
+      <c s="10" r="A436"/>
     </row>
     <row r="437">
-      <c s="8" r="A437"/>
+      <c s="10" r="A437"/>
     </row>
     <row r="438">
-      <c s="8" r="A438"/>
+      <c s="10" r="A438"/>
     </row>
     <row r="439">
-      <c s="8" r="A439"/>
+      <c s="10" r="A439"/>
     </row>
     <row r="440">
-      <c s="8" r="A440"/>
+      <c s="10" r="A440"/>
     </row>
     <row r="441">
-      <c s="8" r="A441"/>
+      <c s="10" r="A441"/>
     </row>
     <row r="442">
-      <c s="8" r="A442"/>
+      <c s="10" r="A442"/>
     </row>
     <row r="443">
-      <c s="8" r="A443"/>
+      <c s="10" r="A443"/>
     </row>
     <row r="444">
-      <c s="8" r="A444"/>
+      <c s="10" r="A444"/>
     </row>
     <row r="445">
-      <c s="8" r="A445"/>
+      <c s="10" r="A445"/>
     </row>
     <row r="446">
-      <c s="8" r="A446"/>
+      <c s="10" r="A446"/>
     </row>
     <row r="447">
-      <c s="8" r="A447"/>
+      <c s="10" r="A447"/>
     </row>
     <row r="448">
-      <c s="8" r="A448"/>
+      <c s="10" r="A448"/>
     </row>
     <row r="449">
-      <c s="8" r="A449"/>
+      <c s="10" r="A449"/>
     </row>
     <row r="450">
-      <c s="8" r="A450"/>
+      <c s="10" r="A450"/>
     </row>
     <row r="451">
-      <c s="8" r="A451"/>
+      <c s="10" r="A451"/>
     </row>
     <row r="452">
-      <c s="8" r="A452"/>
+      <c s="10" r="A452"/>
     </row>
     <row r="453">
-      <c s="8" r="A453"/>
+      <c s="10" r="A453"/>
     </row>
     <row r="454">
-      <c s="8" r="A454"/>
+      <c s="10" r="A454"/>
     </row>
     <row r="455">
-      <c s="8" r="A455"/>
+      <c s="10" r="A455"/>
     </row>
     <row r="456">
-      <c s="8" r="A456"/>
+      <c s="10" r="A456"/>
     </row>
     <row r="457">
-      <c s="8" r="A457"/>
+      <c s="10" r="A457"/>
     </row>
     <row r="458">
-      <c s="8" r="A458"/>
+      <c s="10" r="A458"/>
     </row>
     <row r="459">
-      <c s="8" r="A459"/>
+      <c s="10" r="A459"/>
     </row>
     <row r="460">
-      <c s="8" r="A460"/>
+      <c s="10" r="A460"/>
     </row>
     <row r="461">
-      <c s="8" r="A461"/>
+      <c s="10" r="A461"/>
     </row>
     <row r="462">
-      <c s="8" r="A462"/>
+      <c s="10" r="A462"/>
     </row>
     <row r="463">
-      <c s="8" r="A463"/>
+      <c s="10" r="A463"/>
     </row>
     <row r="464">
-      <c s="8" r="A464"/>
+      <c s="10" r="A464"/>
     </row>
     <row r="465">
-      <c s="8" r="A465"/>
+      <c s="10" r="A465"/>
     </row>
     <row r="466">
-      <c s="8" r="A466"/>
+      <c s="10" r="A466"/>
     </row>
     <row r="467">
-      <c s="8" r="A467"/>
+      <c s="10" r="A467"/>
     </row>
     <row r="468">
-      <c s="8" r="A468"/>
+      <c s="10" r="A468"/>
     </row>
     <row r="469">
-      <c s="8" r="A469"/>
+      <c s="10" r="A469"/>
     </row>
     <row r="470">
-      <c s="8" r="A470"/>
+      <c s="10" r="A470"/>
     </row>
     <row r="471">
-      <c s="8" r="A471"/>
+      <c s="10" r="A471"/>
     </row>
     <row r="472">
-      <c s="8" r="A472"/>
+      <c s="10" r="A472"/>
     </row>
     <row r="473">
-      <c s="8" r="A473"/>
+      <c s="10" r="A473"/>
     </row>
     <row r="474">
-      <c s="8" r="A474"/>
+      <c s="10" r="A474"/>
     </row>
     <row r="475">
-      <c s="8" r="A475"/>
+      <c s="10" r="A475"/>
     </row>
     <row r="476">
-      <c s="8" r="A476"/>
+      <c s="10" r="A476"/>
     </row>
     <row r="477">
-      <c s="8" r="A477"/>
+      <c s="10" r="A477"/>
     </row>
     <row r="478">
-      <c s="8" r="A478"/>
+      <c s="10" r="A478"/>
     </row>
     <row r="479">
-      <c s="8" r="A479"/>
+      <c s="10" r="A479"/>
     </row>
     <row r="480">
-      <c s="8" r="A480"/>
+      <c s="10" r="A480"/>
     </row>
     <row r="481">
-      <c s="8" r="A481"/>
+      <c s="10" r="A481"/>
     </row>
     <row r="482">
-      <c s="8" r="A482"/>
+      <c s="10" r="A482"/>
     </row>
     <row r="483">
-      <c s="8" r="A483"/>
+      <c s="10" r="A483"/>
     </row>
     <row r="484">
-      <c s="8" r="A484"/>
+      <c s="10" r="A484"/>
     </row>
     <row r="485">
-      <c s="8" r="A485"/>
+      <c s="10" r="A485"/>
     </row>
     <row r="486">
-      <c s="8" r="A486"/>
+      <c s="10" r="A486"/>
     </row>
     <row r="487">
-      <c s="8" r="A487"/>
+      <c s="10" r="A487"/>
     </row>
     <row r="488">
-      <c s="8" r="A488"/>
+      <c s="10" r="A488"/>
     </row>
     <row r="489">
-      <c s="8" r="A489"/>
+      <c s="10" r="A489"/>
     </row>
     <row r="490">
-      <c s="8" r="A490"/>
+      <c s="10" r="A490"/>
     </row>
     <row r="491">
-      <c s="8" r="A491"/>
+      <c s="10" r="A491"/>
     </row>
     <row r="492">
-      <c s="8" r="A492"/>
+      <c s="10" r="A492"/>
     </row>
     <row r="493">
-      <c s="8" r="A493"/>
+      <c s="10" r="A493"/>
     </row>
     <row r="494">
-      <c s="8" r="A494"/>
+      <c s="10" r="A494"/>
     </row>
     <row r="495">
-      <c s="8" r="A495"/>
+      <c s="10" r="A495"/>
     </row>
     <row r="496">
-      <c s="8" r="A496"/>
+      <c s="10" r="A496"/>
     </row>
     <row r="497">
-      <c s="8" r="A497"/>
+      <c s="10" r="A497"/>
     </row>
     <row r="498">
-      <c s="8" r="A498"/>
+      <c s="10" r="A498"/>
     </row>
     <row r="499">
-      <c s="8" r="A499"/>
+      <c s="10" r="A499"/>
     </row>
     <row r="500">
-      <c s="8" r="A500"/>
+      <c s="10" r="A500"/>
     </row>
     <row r="501">
-      <c s="8" r="A501"/>
+      <c s="10" r="A501"/>
     </row>
     <row r="502">
-      <c s="8" r="A502"/>
+      <c s="10" r="A502"/>
     </row>
     <row r="503">
-      <c s="8" r="A503"/>
+      <c s="10" r="A503"/>
     </row>
     <row r="504">
-      <c s="8" r="A504"/>
+      <c s="10" r="A504"/>
     </row>
     <row r="505">
-      <c s="8" r="A505"/>
+      <c s="10" r="A505"/>
     </row>
     <row r="506">
-      <c s="8" r="A506"/>
+      <c s="10" r="A506"/>
     </row>
     <row r="507">
-      <c s="8" r="A507"/>
+      <c s="10" r="A507"/>
     </row>
     <row r="508">
-      <c s="8" r="A508"/>
+      <c s="10" r="A508"/>
     </row>
     <row r="509">
-      <c s="8" r="A509"/>
+      <c s="10" r="A509"/>
     </row>
     <row r="510">
-      <c s="8" r="A510"/>
+      <c s="10" r="A510"/>
     </row>
     <row r="511">
-      <c s="8" r="A511"/>
+      <c s="10" r="A511"/>
     </row>
     <row r="512">
-      <c s="8" r="A512"/>
+      <c s="10" r="A512"/>
     </row>
     <row r="513">
-      <c s="8" r="A513"/>
+      <c s="10" r="A513"/>
     </row>
     <row r="514">
-      <c s="8" r="A514"/>
+      <c s="10" r="A514"/>
     </row>
     <row r="515">
-      <c s="8" r="A515"/>
+      <c s="10" r="A515"/>
     </row>
     <row r="516">
-      <c s="8" r="A516"/>
+      <c s="10" r="A516"/>
     </row>
     <row r="517">
-      <c s="8" r="A517"/>
+      <c s="10" r="A517"/>
     </row>
     <row r="518">
-      <c s="8" r="A518"/>
+      <c s="10" r="A518"/>
     </row>
     <row r="519">
-      <c s="8" r="A519"/>
+      <c s="10" r="A519"/>
     </row>
     <row r="520">
-      <c s="8" r="A520"/>
+      <c s="10" r="A520"/>
     </row>
     <row r="521">
-      <c s="8" r="A521"/>
+      <c s="10" r="A521"/>
     </row>
     <row r="522">
-      <c s="8" r="A522"/>
+      <c s="10" r="A522"/>
     </row>
     <row r="523">
-      <c s="8" r="A523"/>
+      <c s="10" r="A523"/>
     </row>
     <row r="524">
-      <c s="8" r="A524"/>
+      <c s="10" r="A524"/>
     </row>
     <row r="525">
-      <c s="8" r="A525"/>
+      <c s="10" r="A525"/>
     </row>
     <row r="526">
-      <c s="8" r="A526"/>
+      <c s="10" r="A526"/>
     </row>
     <row r="527">
-      <c s="8" r="A527"/>
+      <c s="10" r="A527"/>
     </row>
     <row r="528">
-      <c s="8" r="A528"/>
+      <c s="10" r="A528"/>
     </row>
     <row r="529">
-      <c s="8" r="A529"/>
+      <c s="10" r="A529"/>
     </row>
     <row r="530">
-      <c s="8" r="A530"/>
+      <c s="10" r="A530"/>
     </row>
     <row r="531">
-      <c s="8" r="A531"/>
+      <c s="10" r="A531"/>
     </row>
     <row r="532">
-      <c s="8" r="A532"/>
+      <c s="10" r="A532"/>
     </row>
     <row r="533">
-      <c s="8" r="A533"/>
+      <c s="10" r="A533"/>
     </row>
     <row r="534">
-      <c s="8" r="A534"/>
+      <c s="10" r="A534"/>
     </row>
     <row r="535">
-      <c s="8" r="A535"/>
+      <c s="10" r="A535"/>
     </row>
     <row r="536">
-      <c s="8" r="A536"/>
+      <c s="10" r="A536"/>
     </row>
     <row r="537">
-      <c s="8" r="A537"/>
+      <c s="10" r="A537"/>
     </row>
     <row r="538">
-      <c s="8" r="A538"/>
+      <c s="10" r="A538"/>
     </row>
     <row r="539">
-      <c s="8" r="A539"/>
+      <c s="10" r="A539"/>
     </row>
     <row r="540">
-      <c s="8" r="A540"/>
+      <c s="10" r="A540"/>
     </row>
     <row r="541">
-      <c s="8" r="A541"/>
+      <c s="10" r="A541"/>
     </row>
     <row r="542">
-      <c s="8" r="A542"/>
+      <c s="10" r="A542"/>
     </row>
     <row r="543">
-      <c s="8" r="A543"/>
+      <c s="10" r="A543"/>
     </row>
     <row r="544">
-      <c s="8" r="A544"/>
+      <c s="10" r="A544"/>
     </row>
     <row r="545">
-      <c s="8" r="A545"/>
+      <c s="10" r="A545"/>
     </row>
     <row r="546">
-      <c s="8" r="A546"/>
+      <c s="10" r="A546"/>
     </row>
     <row r="547">
-      <c s="8" r="A547"/>
+      <c s="10" r="A547"/>
     </row>
     <row r="548">
-      <c s="8" r="A548"/>
+      <c s="10" r="A548"/>
     </row>
     <row r="549">
-      <c s="8" r="A549"/>
+      <c s="10" r="A549"/>
     </row>
     <row r="550">
-      <c s="8" r="A550"/>
+      <c s="10" r="A550"/>
     </row>
     <row r="551">
-      <c s="8" r="A551"/>
+      <c s="10" r="A551"/>
     </row>
     <row r="552">
-      <c s="8" r="A552"/>
+      <c s="10" r="A552"/>
     </row>
     <row r="553">
-      <c s="8" r="A553"/>
+      <c s="10" r="A553"/>
     </row>
     <row r="554">
-      <c s="8" r="A554"/>
+      <c s="10" r="A554"/>
     </row>
     <row r="555">
-      <c s="8" r="A555"/>
+      <c s="10" r="A555"/>
     </row>
     <row r="556">
-      <c s="8" r="A556"/>
+      <c s="10" r="A556"/>
     </row>
     <row r="557">
-      <c s="8" r="A557"/>
+      <c s="10" r="A557"/>
     </row>
     <row r="558">
-      <c s="8" r="A558"/>
+      <c s="10" r="A558"/>
     </row>
     <row r="559">
-      <c s="8" r="A559"/>
+      <c s="10" r="A559"/>
     </row>
     <row r="560">
-      <c s="8" r="A560"/>
+      <c s="10" r="A560"/>
     </row>
     <row r="561">
-      <c s="8" r="A561"/>
+      <c s="10" r="A561"/>
     </row>
     <row r="562">
-      <c s="8" r="A562"/>
+      <c s="10" r="A562"/>
     </row>
     <row r="563">
-      <c s="8" r="A563"/>
+      <c s="10" r="A563"/>
     </row>
     <row r="564">
-      <c s="8" r="A564"/>
+      <c s="10" r="A564"/>
     </row>
     <row r="565">
-      <c s="8" r="A565"/>
+      <c s="10" r="A565"/>
     </row>
     <row r="566">
-      <c s="8" r="A566"/>
+      <c s="10" r="A566"/>
     </row>
     <row r="567">
-      <c s="8" r="A567"/>
+      <c s="10" r="A567"/>
     </row>
     <row r="568">
-      <c s="8" r="A568"/>
+      <c s="10" r="A568"/>
     </row>
     <row r="569">
-      <c s="8" r="A569"/>
+      <c s="10" r="A569"/>
     </row>
     <row r="570">
-      <c s="8" r="A570"/>
+      <c s="10" r="A570"/>
     </row>
     <row r="571">
-      <c s="8" r="A571"/>
+      <c s="10" r="A571"/>
     </row>
     <row r="572">
-      <c s="8" r="A572"/>
+      <c s="10" r="A572"/>
     </row>
     <row r="573">
-      <c s="8" r="A573"/>
+      <c s="10" r="A573"/>
     </row>
     <row r="574">
-      <c s="8" r="A574"/>
+      <c s="10" r="A574"/>
     </row>
     <row r="575">
-      <c s="8" r="A575"/>
+      <c s="10" r="A575"/>
     </row>
     <row r="576">
-      <c s="8" r="A576"/>
+      <c s="10" r="A576"/>
     </row>
     <row r="577">
-      <c s="8" r="A577"/>
+      <c s="10" r="A577"/>
     </row>
     <row r="578">
-      <c s="8" r="A578"/>
+      <c s="10" r="A578"/>
     </row>
     <row r="579">
-      <c s="8" r="A579"/>
+      <c s="10" r="A579"/>
     </row>
     <row r="580">
-      <c s="8" r="A580"/>
+      <c s="10" r="A580"/>
     </row>
     <row r="581">
-      <c s="8" r="A581"/>
+      <c s="10" r="A581"/>
     </row>
     <row r="582">
-      <c s="8" r="A582"/>
+      <c s="10" r="A582"/>
     </row>
     <row r="583">
-      <c s="8" r="A583"/>
+      <c s="10" r="A583"/>
     </row>
     <row r="584">
-      <c s="8" r="A584"/>
+      <c s="10" r="A584"/>
     </row>
     <row r="585">
-      <c s="8" r="A585"/>
+      <c s="10" r="A585"/>
     </row>
     <row r="586">
-      <c s="8" r="A586"/>
+      <c s="10" r="A586"/>
     </row>
     <row r="587">
-      <c s="8" r="A587"/>
+      <c s="10" r="A587"/>
     </row>
     <row r="588">
-      <c s="8" r="A588"/>
+      <c s="10" r="A588"/>
     </row>
     <row r="589">
-      <c s="8" r="A589"/>
+      <c s="10" r="A589"/>
     </row>
     <row r="590">
-      <c s="8" r="A590"/>
+      <c s="10" r="A590"/>
     </row>
     <row r="591">
-      <c s="8" r="A591"/>
+      <c s="10" r="A591"/>
     </row>
     <row r="592">
-      <c s="8" r="A592"/>
+      <c s="10" r="A592"/>
     </row>
     <row r="593">
-      <c s="8" r="A593"/>
+      <c s="10" r="A593"/>
     </row>
     <row r="594">
-      <c s="8" r="A594"/>
+      <c s="10" r="A594"/>
     </row>
     <row r="595">
-      <c s="8" r="A595"/>
+      <c s="10" r="A595"/>
     </row>
     <row r="596">
-      <c s="8" r="A596"/>
+      <c s="10" r="A596"/>
     </row>
     <row r="597">
-      <c s="8" r="A597"/>
+      <c s="10" r="A597"/>
     </row>
     <row r="598">
-      <c s="8" r="A598"/>
+      <c s="10" r="A598"/>
     </row>
     <row r="599">
-      <c s="8" r="A599"/>
+      <c s="10" r="A599"/>
     </row>
     <row r="600">
-      <c s="8" r="A600"/>
+      <c s="10" r="A600"/>
     </row>
     <row r="601">
-      <c s="8" r="A601"/>
+      <c s="10" r="A601"/>
     </row>
     <row r="602">
-      <c s="8" r="A602"/>
+      <c s="10" r="A602"/>
     </row>
     <row r="603">
-      <c s="8" r="A603"/>
+      <c s="10" r="A603"/>
     </row>
     <row r="604">
-      <c s="8" r="A604"/>
+      <c s="10" r="A604"/>
     </row>
     <row r="605">
-      <c s="8" r="A605"/>
+      <c s="10" r="A605"/>
     </row>
     <row r="606">
-      <c s="8" r="A606"/>
+      <c s="10" r="A606"/>
     </row>
     <row r="607">
-      <c s="8" r="A607"/>
+      <c s="10" r="A607"/>
     </row>
     <row r="608">
-      <c s="8" r="A608"/>
+      <c s="10" r="A608"/>
     </row>
     <row r="609">
-      <c s="8" r="A609"/>
+      <c s="10" r="A609"/>
     </row>
     <row r="610">
-      <c s="8" r="A610"/>
+      <c s="10" r="A610"/>
     </row>
     <row r="611">
-      <c s="8" r="A611"/>
+      <c s="10" r="A611"/>
     </row>
     <row r="612">
-      <c s="8" r="A612"/>
+      <c s="10" r="A612"/>
     </row>
     <row r="613">
-      <c s="8" r="A613"/>
+      <c s="10" r="A613"/>
     </row>
     <row r="614">
-      <c s="8" r="A614"/>
+      <c s="10" r="A614"/>
     </row>
     <row r="615">
-      <c s="8" r="A615"/>
+      <c s="10" r="A615"/>
     </row>
     <row r="616">
-      <c s="8" r="A616"/>
+      <c s="10" r="A616"/>
     </row>
     <row r="617">
-      <c s="8" r="A617"/>
+      <c s="10" r="A617"/>
     </row>
     <row r="618">
-      <c s="8" r="A618"/>
+      <c s="10" r="A618"/>
     </row>
     <row r="619">
-      <c s="8" r="A619"/>
+      <c s="10" r="A619"/>
     </row>
     <row r="620">
-      <c s="8" r="A620"/>
+      <c s="10" r="A620"/>
     </row>
     <row r="621">
-      <c s="8" r="A621"/>
+      <c s="10" r="A621"/>
     </row>
     <row r="622">
-      <c s="8" r="A622"/>
+      <c s="10" r="A622"/>
     </row>
     <row r="623">
-      <c s="8" r="A623"/>
+      <c s="10" r="A623"/>
     </row>
     <row r="624">
-      <c s="8" r="A624"/>
+      <c s="10" r="A624"/>
     </row>
     <row r="625">
-      <c s="8" r="A625"/>
+      <c s="10" r="A625"/>
     </row>
     <row r="626">
-      <c s="8" r="A626"/>
+      <c s="10" r="A626"/>
     </row>
     <row r="627">
-      <c s="8" r="A627"/>
+      <c s="10" r="A627"/>
     </row>
     <row r="628">
-      <c s="8" r="A628"/>
+      <c s="10" r="A628"/>
     </row>
     <row r="629">
-      <c s="8" r="A629"/>
+      <c s="10" r="A629"/>
     </row>
     <row r="630">
-      <c s="8" r="A630"/>
+      <c s="10" r="A630"/>
     </row>
     <row r="631">
-      <c s="8" r="A631"/>
+      <c s="10" r="A631"/>
     </row>
     <row r="632">
-      <c s="8" r="A632"/>
+      <c s="10" r="A632"/>
     </row>
     <row r="633">
-      <c s="8" r="A633"/>
+      <c s="10" r="A633"/>
     </row>
     <row r="634">
-      <c s="8" r="A634"/>
+      <c s="10" r="A634"/>
     </row>
     <row r="635">
-      <c s="8" r="A635"/>
+      <c s="10" r="A635"/>
     </row>
     <row r="636">
-      <c s="8" r="A636"/>
+      <c s="10" r="A636"/>
     </row>
     <row r="637">
-      <c s="8" r="A637"/>
+      <c s="10" r="A637"/>
     </row>
     <row r="638">
-      <c s="8" r="A638"/>
+      <c s="10" r="A638"/>
     </row>
     <row r="639">
-      <c s="8" r="A639"/>
+      <c s="10" r="A639"/>
     </row>
     <row r="640">
-      <c s="8" r="A640"/>
+      <c s="10" r="A640"/>
     </row>
     <row r="641">
-      <c s="8" r="A641"/>
+      <c s="10" r="A641"/>
     </row>
     <row r="642">
-      <c s="8" r="A642"/>
+      <c s="10" r="A642"/>
     </row>
     <row r="643">
-      <c s="8" r="A643"/>
+      <c s="10" r="A643"/>
     </row>
     <row r="644">
-      <c s="8" r="A644"/>
+      <c s="10" r="A644"/>
     </row>
     <row r="645">
-      <c s="8" r="A645"/>
+      <c s="10" r="A645"/>
     </row>
     <row r="646">
-      <c s="8" r="A646"/>
+      <c s="10" r="A646"/>
     </row>
     <row r="647">
-      <c s="8" r="A647"/>
+      <c s="10" r="A647"/>
     </row>
     <row r="648">
-      <c s="8" r="A648"/>
+      <c s="10" r="A648"/>
     </row>
     <row r="649">
-      <c s="8" r="A649"/>
+      <c s="10" r="A649"/>
     </row>
     <row r="650">
-      <c s="8" r="A650"/>
+      <c s="10" r="A650"/>
     </row>
     <row r="651">
-      <c s="8" r="A651"/>
+      <c s="10" r="A651"/>
     </row>
     <row r="652">
-      <c s="8" r="A652"/>
+      <c s="10" r="A652"/>
     </row>
     <row r="653">
-      <c s="8" r="A653"/>
+      <c s="10" r="A653"/>
     </row>
     <row r="654">
-      <c s="8" r="A654"/>
+      <c s="10" r="A654"/>
     </row>
     <row r="655">
-      <c s="8" r="A655"/>
+      <c s="10" r="A655"/>
     </row>
     <row r="656">
-      <c s="8" r="A656"/>
+      <c s="10" r="A656"/>
     </row>
     <row r="657">
-      <c s="8" r="A657"/>
+      <c s="10" r="A657"/>
     </row>
     <row r="658">
-      <c s="8" r="A658"/>
+      <c s="10" r="A658"/>
     </row>
     <row r="659">
-      <c s="8" r="A659"/>
+      <c s="10" r="A659"/>
     </row>
     <row r="660">
-      <c s="8" r="A660"/>
+      <c s="10" r="A660"/>
     </row>
     <row r="661">
-      <c s="8" r="A661"/>
+      <c s="10" r="A661"/>
     </row>
     <row r="662">
-      <c s="8" r="A662"/>
+      <c s="10" r="A662"/>
     </row>
     <row r="663">
-      <c s="8" r="A663"/>
+      <c s="10" r="A663"/>
     </row>
     <row r="664">
-      <c s="8" r="A664"/>
+      <c s="10" r="A664"/>
     </row>
     <row r="665">
-      <c s="8" r="A665"/>
+      <c s="10" r="A665"/>
     </row>
     <row r="666">
-      <c s="8" r="A666"/>
+      <c s="10" r="A666"/>
     </row>
     <row r="667">
-      <c s="8" r="A667"/>
+      <c s="10" r="A667"/>
     </row>
     <row r="668">
-      <c s="8" r="A668"/>
+      <c s="10" r="A668"/>
     </row>
     <row r="669">
-      <c s="8" r="A669"/>
+      <c s="10" r="A669"/>
     </row>
     <row r="670">
-      <c s="8" r="A670"/>
+      <c s="10" r="A670"/>
     </row>
     <row r="671">
-      <c s="8" r="A671"/>
+      <c s="10" r="A671"/>
     </row>
     <row r="672">
-      <c s="8" r="A672"/>
+      <c s="10" r="A672"/>
     </row>
     <row r="673">
-      <c s="8" r="A673"/>
+      <c s="10" r="A673"/>
     </row>
     <row r="674">
-      <c s="8" r="A674"/>
+      <c s="10" r="A674"/>
     </row>
     <row r="675">
-      <c s="8" r="A675"/>
+      <c s="10" r="A675"/>
     </row>
     <row r="676">
-      <c s="8" r="A676"/>
+      <c s="10" r="A676"/>
     </row>
     <row r="677">
-      <c s="8" r="A677"/>
+      <c s="10" r="A677"/>
     </row>
     <row r="678">
-      <c s="8" r="A678"/>
+      <c s="10" r="A678"/>
     </row>
     <row r="679">
-      <c s="8" r="A679"/>
+      <c s="10" r="A679"/>
     </row>
     <row r="680">
-      <c s="8" r="A680"/>
+      <c s="10" r="A680"/>
     </row>
     <row r="681">
-      <c s="8" r="A681"/>
+      <c s="10" r="A681"/>
     </row>
     <row r="682">
-      <c s="8" r="A682"/>
+      <c s="10" r="A682"/>
     </row>
     <row r="683">
-      <c s="8" r="A683"/>
+      <c s="10" r="A683"/>
     </row>
     <row r="684">
-      <c s="8" r="A684"/>
+      <c s="10" r="A684"/>
     </row>
     <row r="685">
-      <c s="8" r="A685"/>
+      <c s="10" r="A685"/>
     </row>
     <row r="686">
-      <c s="8" r="A686"/>
+      <c s="10" r="A686"/>
     </row>
     <row r="687">
-      <c s="8" r="A687"/>
+      <c s="10" r="A687"/>
     </row>
     <row r="688">
-      <c s="8" r="A688"/>
+      <c s="10" r="A688"/>
     </row>
     <row r="689">
-      <c s="8" r="A689"/>
+      <c s="10" r="A689"/>
     </row>
     <row r="690">
-      <c s="8" r="A690"/>
+      <c s="10" r="A690"/>
     </row>
     <row r="691">
-      <c s="8" r="A691"/>
+      <c s="10" r="A691"/>
     </row>
     <row r="692">
-      <c s="8" r="A692"/>
+      <c s="10" r="A692"/>
     </row>
     <row r="693">
-      <c s="8" r="A693"/>
+      <c s="10" r="A693"/>
     </row>
     <row r="694">
-      <c s="8" r="A694"/>
+      <c s="10" r="A694"/>
     </row>
     <row r="695">
-      <c s="8" r="A695"/>
+      <c s="10" r="A695"/>
     </row>
     <row r="696">
-      <c s="8" r="A696"/>
+      <c s="10" r="A696"/>
     </row>
     <row r="697">
-      <c s="8" r="A697"/>
+      <c s="10" r="A697"/>
     </row>
     <row r="698">
-      <c s="8" r="A698"/>
+      <c s="10" r="A698"/>
     </row>
     <row r="699">
-      <c s="8" r="A699"/>
+      <c s="10" r="A699"/>
     </row>
     <row r="700">
-      <c s="8" r="A700"/>
+      <c s="10" r="A700"/>
     </row>
     <row r="701">
-      <c s="8" r="A701"/>
+      <c s="10" r="A701"/>
     </row>
     <row r="702">
-      <c s="8" r="A702"/>
+      <c s="10" r="A702"/>
     </row>
     <row r="703">
-      <c s="8" r="A703"/>
+      <c s="10" r="A703"/>
     </row>
     <row r="704">
-      <c s="8" r="A704"/>
+      <c s="10" r="A704"/>
     </row>
     <row r="705">
-      <c s="8" r="A705"/>
+      <c s="10" r="A705"/>
     </row>
     <row r="706">
-      <c s="8" r="A706"/>
+      <c s="10" r="A706"/>
     </row>
     <row r="707">
-      <c s="8" r="A707"/>
+      <c s="10" r="A707"/>
     </row>
     <row r="708">
-      <c s="8" r="A708"/>
+      <c s="10" r="A708"/>
     </row>
     <row r="709">
-      <c s="8" r="A709"/>
+      <c s="10" r="A709"/>
     </row>
     <row r="710">
-      <c s="8" r="A710"/>
+      <c s="10" r="A710"/>
     </row>
     <row r="711">
-      <c s="8" r="A711"/>
+      <c s="10" r="A711"/>
     </row>
     <row r="712">
-      <c s="8" r="A712"/>
+      <c s="10" r="A712"/>
     </row>
     <row r="713">
-      <c s="8" r="A713"/>
+      <c s="10" r="A713"/>
     </row>
     <row r="714">
-      <c s="8" r="A714"/>
+      <c s="10" r="A714"/>
     </row>
     <row r="715">
-      <c s="8" r="A715"/>
+      <c s="10" r="A715"/>
     </row>
     <row r="716">
-      <c s="8" r="A716"/>
+      <c s="10" r="A716"/>
     </row>
     <row r="717">
-      <c s="8" r="A717"/>
+      <c s="10" r="A717"/>
     </row>
     <row r="718">
-      <c s="8" r="A718"/>
+      <c s="10" r="A718"/>
     </row>
     <row r="719">
-      <c s="8" r="A719"/>
+      <c s="10" r="A719"/>
     </row>
     <row r="720">
-      <c s="8" r="A720"/>
+      <c s="10" r="A720"/>
     </row>
     <row r="721">
-      <c s="8" r="A721"/>
+      <c s="10" r="A721"/>
     </row>
     <row r="722">
-      <c s="8" r="A722"/>
+      <c s="10" r="A722"/>
     </row>
     <row r="723">
-      <c s="8" r="A723"/>
+      <c s="10" r="A723"/>
     </row>
     <row r="724">
-      <c s="8" r="A724"/>
+      <c s="10" r="A724"/>
     </row>
     <row r="725">
-      <c s="8" r="A725"/>
+      <c s="10" r="A725"/>
     </row>
     <row r="726">
-      <c s="8" r="A726"/>
+      <c s="10" r="A726"/>
     </row>
     <row r="727">
-      <c s="8" r="A727"/>
+      <c s="10" r="A727"/>
     </row>
     <row r="728">
-      <c s="8" r="A728"/>
+      <c s="10" r="A728"/>
     </row>
     <row r="729">
-      <c s="8" r="A729"/>
+      <c s="10" r="A729"/>
     </row>
     <row r="730">
-      <c s="8" r="A730"/>
+      <c s="10" r="A730"/>
     </row>
     <row r="731">
-      <c s="8" r="A731"/>
+      <c s="10" r="A731"/>
     </row>
     <row r="732">
-      <c s="8" r="A732"/>
+      <c s="10" r="A732"/>
     </row>
     <row r="733">
-      <c s="8" r="A733"/>
+      <c s="10" r="A733"/>
     </row>
     <row r="734">
-      <c s="8" r="A734"/>
+      <c s="10" r="A734"/>
     </row>
     <row r="735">
-      <c s="8" r="A735"/>
+      <c s="10" r="A735"/>
     </row>
     <row r="736">
-      <c s="8" r="A736"/>
+      <c s="10" r="A736"/>
     </row>
     <row r="737">
-      <c s="8" r="A737"/>
+      <c s="10" r="A737"/>
     </row>
     <row r="738">
-      <c s="8" r="A738"/>
+      <c s="10" r="A738"/>
     </row>
     <row r="739">
-      <c s="8" r="A739"/>
+      <c s="10" r="A739"/>
     </row>
     <row r="740">
-      <c s="8" r="A740"/>
+      <c s="10" r="A740"/>
     </row>
     <row r="741">
-      <c s="8" r="A741"/>
+      <c s="10" r="A741"/>
     </row>
     <row r="742">
-      <c s="8" r="A742"/>
+      <c s="10" r="A742"/>
     </row>
     <row r="743">
-      <c s="8" r="A743"/>
+      <c s="10" r="A743"/>
     </row>
     <row r="744">
-      <c s="8" r="A744"/>
+      <c s="10" r="A744"/>
     </row>
     <row r="745">
-      <c s="8" r="A745"/>
+      <c s="10" r="A745"/>
     </row>
     <row r="746">
-      <c s="8" r="A746"/>
+      <c s="10" r="A746"/>
     </row>
     <row r="747">
-      <c s="8" r="A747"/>
+      <c s="10" r="A747"/>
     </row>
     <row r="748">
-      <c s="8" r="A748"/>
+      <c s="10" r="A748"/>
     </row>
     <row r="749">
-      <c s="8" r="A749"/>
+      <c s="10" r="A749"/>
     </row>
     <row r="750">
-      <c s="8" r="A750"/>
+      <c s="10" r="A750"/>
     </row>
     <row r="751">
-      <c s="8" r="A751"/>
+      <c s="10" r="A751"/>
     </row>
     <row r="752">
-      <c s="8" r="A752"/>
+      <c s="10" r="A752"/>
     </row>
     <row r="753">
-      <c s="8" r="A753"/>
+      <c s="10" r="A753"/>
     </row>
     <row r="754">
-      <c s="8" r="A754"/>
+      <c s="10" r="A754"/>
     </row>
     <row r="755">
-      <c s="8" r="A755"/>
+      <c s="10" r="A755"/>
     </row>
     <row r="756">
-      <c s="8" r="A756"/>
+      <c s="10" r="A756"/>
     </row>
     <row r="757">
-      <c s="8" r="A757"/>
+      <c s="10" r="A757"/>
     </row>
     <row r="758">
-      <c s="8" r="A758"/>
+      <c s="10" r="A758"/>
     </row>
     <row r="759">
-      <c s="8" r="A759"/>
+      <c s="10" r="A759"/>
     </row>
     <row r="760">
-      <c s="8" r="A760"/>
+      <c s="10" r="A760"/>
     </row>
     <row r="761">
-      <c s="8" r="A761"/>
+      <c s="10" r="A761"/>
     </row>
     <row r="762">
-      <c s="8" r="A762"/>
+      <c s="10" r="A762"/>
     </row>
     <row r="763">
-      <c s="8" r="A763"/>
+      <c s="10" r="A763"/>
     </row>
     <row r="764">
-      <c s="8" r="A764"/>
+      <c s="10" r="A764"/>
     </row>
     <row r="765">
-      <c s="8" r="A765"/>
+      <c s="10" r="A765"/>
     </row>
     <row r="766">
-      <c s="8" r="A766"/>
+      <c s="10" r="A766"/>
     </row>
     <row r="767">
-      <c s="8" r="A767"/>
+      <c s="10" r="A767"/>
     </row>
     <row r="768">
-      <c s="8" r="A768"/>
+      <c s="10" r="A768"/>
     </row>
     <row r="769">
-      <c s="8" r="A769"/>
+      <c s="10" r="A769"/>
     </row>
     <row r="770">
-      <c s="8" r="A770"/>
+      <c s="10" r="A770"/>
     </row>
     <row r="771">
-      <c s="8" r="A771"/>
+      <c s="10" r="A771"/>
     </row>
     <row r="772">
-      <c s="8" r="A772"/>
+      <c s="10" r="A772"/>
     </row>
     <row r="773">
-      <c s="8" r="A773"/>
+      <c s="10" r="A773"/>
     </row>
     <row r="774">
-      <c s="8" r="A774"/>
+      <c s="10" r="A774"/>
     </row>
     <row r="775">
-      <c s="8" r="A775"/>
+      <c s="10" r="A775"/>
     </row>
     <row r="776">
-      <c s="8" r="A776"/>
+      <c s="10" r="A776"/>
     </row>
     <row r="777">
-      <c s="8" r="A777"/>
+      <c s="10" r="A777"/>
     </row>
     <row r="778">
-      <c s="8" r="A778"/>
+      <c s="10" r="A778"/>
     </row>
     <row r="779">
-      <c s="8" r="A779"/>
+      <c s="10" r="A779"/>
     </row>
     <row r="780">
-      <c s="8" r="A780"/>
+      <c s="10" r="A780"/>
     </row>
     <row r="781">
-      <c s="8" r="A781"/>
+      <c s="10" r="A781"/>
     </row>
     <row r="782">
-      <c s="8" r="A782"/>
+      <c s="10" r="A782"/>
     </row>
     <row r="783">
-      <c s="8" r="A783"/>
+      <c s="10" r="A783"/>
     </row>
     <row r="784">
-      <c s="8" r="A784"/>
+      <c s="10" r="A784"/>
     </row>
     <row r="785">
-      <c s="8" r="A785"/>
+      <c s="10" r="A785"/>
     </row>
     <row r="786">
-      <c s="8" r="A786"/>
+      <c s="10" r="A786"/>
     </row>
     <row r="787">
-      <c s="8" r="A787"/>
+      <c s="10" r="A787"/>
     </row>
     <row r="788">
-      <c s="8" r="A788"/>
+      <c s="10" r="A788"/>
     </row>
     <row r="789">
-      <c s="8" r="A789"/>
+      <c s="10" r="A789"/>
     </row>
     <row r="790">
-      <c s="8" r="A790"/>
+      <c s="10" r="A790"/>
     </row>
     <row r="791">
-      <c s="8" r="A791"/>
+      <c s="10" r="A791"/>
     </row>
     <row r="792">
-      <c s="8" r="A792"/>
+      <c s="10" r="A792"/>
     </row>
     <row r="793">
-      <c s="8" r="A793"/>
+      <c s="10" r="A793"/>
     </row>
     <row r="794">
-      <c s="8" r="A794"/>
+      <c s="10" r="A794"/>
     </row>
     <row r="795">
-      <c s="8" r="A795"/>
+      <c s="10" r="A795"/>
     </row>
     <row r="796">
-      <c s="8" r="A796"/>
+      <c s="10" r="A796"/>
     </row>
     <row r="797">
-      <c s="8" r="A797"/>
+      <c s="10" r="A797"/>
     </row>
     <row r="798">
-      <c s="8" r="A798"/>
+      <c s="10" r="A798"/>
     </row>
     <row r="799">
-      <c s="8" r="A799"/>
+      <c s="10" r="A799"/>
     </row>
     <row r="800">
-      <c s="8" r="A800"/>
+      <c s="10" r="A800"/>
     </row>
     <row r="801">
-      <c s="8" r="A801"/>
+      <c s="10" r="A801"/>
     </row>
     <row r="802">
-      <c s="8" r="A802"/>
+      <c s="10" r="A802"/>
     </row>
     <row r="803">
-      <c s="8" r="A803"/>
+      <c s="10" r="A803"/>
     </row>
     <row r="804">
-      <c s="8" r="A804"/>
+      <c s="10" r="A804"/>
     </row>
     <row r="805">
-      <c s="8" r="A805"/>
+      <c s="10" r="A805"/>
     </row>
     <row r="806">
-      <c s="8" r="A806"/>
+      <c s="10" r="A806"/>
     </row>
     <row r="807">
-      <c s="8" r="A807"/>
+      <c s="10" r="A807"/>
     </row>
     <row r="808">
-      <c s="8" r="A808"/>
+      <c s="10" r="A808"/>
     </row>
     <row r="809">
-      <c s="8" r="A809"/>
+      <c s="10" r="A809"/>
     </row>
     <row r="810">
-      <c s="8" r="A810"/>
+      <c s="10" r="A810"/>
     </row>
     <row r="811">
-      <c s="8" r="A811"/>
+      <c s="10" r="A811"/>
     </row>
     <row r="812">
-      <c s="8" r="A812"/>
+      <c s="10" r="A812"/>
     </row>
     <row r="813">
-      <c s="8" r="A813"/>
+      <c s="10" r="A813"/>
     </row>
     <row r="814">
-      <c s="8" r="A814"/>
+      <c s="10" r="A814"/>
     </row>
     <row r="815">
-      <c s="8" r="A815"/>
+      <c s="10" r="A815"/>
     </row>
     <row r="816">
-      <c s="8" r="A816"/>
+      <c s="10" r="A816"/>
     </row>
     <row r="817">
-      <c s="8" r="A817"/>
+      <c s="10" r="A817"/>
     </row>
     <row r="818">
-      <c s="8" r="A818"/>
+      <c s="10" r="A818"/>
     </row>
     <row r="819">
-      <c s="8" r="A819"/>
+      <c s="10" r="A819"/>
     </row>
     <row r="820">
-      <c s="8" r="A820"/>
+      <c s="10" r="A820"/>
     </row>
     <row r="821">
-      <c s="8" r="A821"/>
+      <c s="10" r="A821"/>
     </row>
     <row r="822">
-      <c s="8" r="A822"/>
+      <c s="10" r="A822"/>
     </row>
     <row r="823">
-      <c s="8" r="A823"/>
+      <c s="10" r="A823"/>
     </row>
     <row r="824">
-      <c s="8" r="A824"/>
+      <c s="10" r="A824"/>
     </row>
     <row r="825">
-      <c s="8" r="A825"/>
+      <c s="10" r="A825"/>
     </row>
     <row r="826">
-      <c s="8" r="A826"/>
+      <c s="10" r="A826"/>
     </row>
     <row r="827">
-      <c s="8" r="A827"/>
+      <c s="10" r="A827"/>
     </row>
     <row r="828">
-      <c s="8" r="A828"/>
+      <c s="10" r="A828"/>
     </row>
     <row r="829">
-      <c s="8" r="A829"/>
+      <c s="10" r="A829"/>
     </row>
     <row r="830">
-      <c s="8" r="A830"/>
+      <c s="10" r="A830"/>
     </row>
     <row r="831">
-      <c s="8" r="A831"/>
+      <c s="10" r="A831"/>
     </row>
     <row r="832">
-      <c s="8" r="A832"/>
+      <c s="10" r="A832"/>
     </row>
     <row r="833">
-      <c s="8" r="A833"/>
+      <c s="10" r="A833"/>
     </row>
     <row r="834">
-      <c s="8" r="A834"/>
+      <c s="10" r="A834"/>
     </row>
     <row r="835">
-      <c s="8" r="A835"/>
+      <c s="10" r="A835"/>
     </row>
     <row r="836">
-      <c s="8" r="A836"/>
+      <c s="10" r="A836"/>
     </row>
     <row r="837">
-      <c s="8" r="A837"/>
+      <c s="10" r="A837"/>
     </row>
     <row r="838">
-      <c s="8" r="A838"/>
+      <c s="10" r="A838"/>
     </row>
     <row r="839">
-      <c s="8" r="A839"/>
+      <c s="10" r="A839"/>
     </row>
     <row r="840">
-      <c s="8" r="A840"/>
+      <c s="10" r="A840"/>
     </row>
     <row r="841">
-      <c s="8" r="A841"/>
+      <c s="10" r="A841"/>
     </row>
     <row r="842">
-      <c s="8" r="A842"/>
+      <c s="10" r="A842"/>
     </row>
     <row r="843">
-      <c s="8" r="A843"/>
+      <c s="10" r="A843"/>
     </row>
     <row r="844">
-      <c s="8" r="A844"/>
+      <c s="10" r="A844"/>
     </row>
     <row r="845">
-      <c s="8" r="A845"/>
+      <c s="10" r="A845"/>
     </row>
     <row r="846">
-      <c s="8" r="A846"/>
+      <c s="10" r="A846"/>
     </row>
     <row r="847">
-      <c s="8" r="A847"/>
+      <c s="10" r="A847"/>
     </row>
     <row r="848">
-      <c s="8" r="A848"/>
+      <c s="10" r="A848"/>
     </row>
     <row r="849">
-      <c s="8" r="A849"/>
+      <c s="10" r="A849"/>
     </row>
     <row r="850">
-      <c s="8" r="A850"/>
+      <c s="10" r="A850"/>
     </row>
     <row r="851">
-      <c s="8" r="A851"/>
+      <c s="10" r="A851"/>
     </row>
     <row r="852">
-      <c s="8" r="A852"/>
+      <c s="10" r="A852"/>
     </row>
     <row r="853">
-      <c s="8" r="A853"/>
+      <c s="10" r="A853"/>
     </row>
     <row r="854">
-      <c s="8" r="A854"/>
+      <c s="10" r="A854"/>
     </row>
     <row r="855">
-      <c s="8" r="A855"/>
+      <c s="10" r="A855"/>
     </row>
     <row r="856">
-      <c s="8" r="A856"/>
+      <c s="10" r="A856"/>
     </row>
     <row r="857">
-      <c s="8" r="A857"/>
+      <c s="10" r="A857"/>
     </row>
     <row r="858">
-      <c s="8" r="A858"/>
+      <c s="10" r="A858"/>
     </row>
     <row r="859">
-      <c s="8" r="A859"/>
+      <c s="10" r="A859"/>
     </row>
     <row r="860">
-      <c s="8" r="A860"/>
+      <c s="10" r="A860"/>
     </row>
     <row r="861">
-      <c s="8" r="A861"/>
+      <c s="10" r="A861"/>
     </row>
     <row r="862">
-      <c s="8" r="A862"/>
+      <c s="10" r="A862"/>
     </row>
     <row r="863">
-      <c s="8" r="A863"/>
+      <c s="10" r="A863"/>
     </row>
     <row r="864">
-      <c s="8" r="A864"/>
+      <c s="10" r="A864"/>
     </row>
     <row r="865">
-      <c s="8" r="A865"/>
+      <c s="10" r="A865"/>
     </row>
     <row r="866">
-      <c s="8" r="A866"/>
+      <c s="10" r="A866"/>
     </row>
     <row r="867">
-      <c s="8" r="A867"/>
+      <c s="10" r="A867"/>
     </row>
     <row r="868">
-      <c s="8" r="A868"/>
+      <c s="10" r="A868"/>
     </row>
     <row r="869">
-      <c s="8" r="A869"/>
+      <c s="10" r="A869"/>
     </row>
     <row r="870">
-      <c s="8" r="A870"/>
+      <c s="10" r="A870"/>
     </row>
     <row r="871">
-      <c s="8" r="A871"/>
+      <c s="10" r="A871"/>
     </row>
     <row r="872">
-      <c s="8" r="A872"/>
+      <c s="10" r="A872"/>
     </row>
     <row r="873">
-      <c s="8" r="A873"/>
+      <c s="10" r="A873"/>
     </row>
     <row r="874">
-      <c s="8" r="A874"/>
+      <c s="10" r="A874"/>
     </row>
     <row r="875">
-      <c s="8" r="A875"/>
+      <c s="10" r="A875"/>
     </row>
     <row r="876">
-      <c s="8" r="A876"/>
+      <c s="10" r="A876"/>
     </row>
     <row r="877">
-      <c s="8" r="A877"/>
+      <c s="10" r="A877"/>
     </row>
     <row r="878">
-      <c s="8" r="A878"/>
+      <c s="10" r="A878"/>
     </row>
     <row r="879">
-      <c s="8" r="A879"/>
+      <c s="10" r="A879"/>
     </row>
     <row r="880">
-      <c s="8" r="A880"/>
+      <c s="10" r="A880"/>
     </row>
     <row r="881">
-      <c s="8" r="A881"/>
+      <c s="10" r="A881"/>
     </row>
     <row r="882">
-      <c s="8" r="A882"/>
+      <c s="10" r="A882"/>
     </row>
     <row r="883">
-      <c s="8" r="A883"/>
+      <c s="10" r="A883"/>
     </row>
     <row r="884">
-      <c s="8" r="A884"/>
+      <c s="10" r="A884"/>
     </row>
     <row r="885">
-      <c s="8" r="A885"/>
+      <c s="10" r="A885"/>
     </row>
     <row r="886">
-      <c s="8" r="A886"/>
+      <c s="10" r="A886"/>
     </row>
     <row r="887">
-      <c s="8" r="A887"/>
+      <c s="10" r="A887"/>
     </row>
     <row r="888">
-      <c s="8" r="A888"/>
+      <c s="10" r="A888"/>
     </row>
     <row r="889">
-      <c s="8" r="A889"/>
+      <c s="10" r="A889"/>
     </row>
     <row r="890">
-      <c s="8" r="A890"/>
+      <c s="10" r="A890"/>
     </row>
     <row r="891">
-      <c s="8" r="A891"/>
+      <c s="10" r="A891"/>
     </row>
     <row r="892">
-      <c s="8" r="A892"/>
+      <c s="10" r="A892"/>
     </row>
     <row r="893">
-      <c s="8" r="A893"/>
+      <c s="10" r="A893"/>
     </row>
     <row r="894">
-      <c s="8" r="A894"/>
+      <c s="10" r="A894"/>
     </row>
     <row r="895">
-      <c s="8" r="A895"/>
+      <c s="10" r="A895"/>
     </row>
     <row r="896">
-      <c s="8" r="A896"/>
+      <c s="10" r="A896"/>
     </row>
     <row r="897">
-      <c s="8" r="A897"/>
+      <c s="10" r="A897"/>
     </row>
     <row r="898">
-      <c s="8" r="A898"/>
+      <c s="10" r="A898"/>
     </row>
     <row r="899">
-      <c s="8" r="A899"/>
+      <c s="10" r="A899"/>
     </row>
     <row r="900">
-      <c s="8" r="A900"/>
+      <c s="10" r="A900"/>
     </row>
     <row r="901">
-      <c s="8" r="A901"/>
+      <c s="10" r="A901"/>
     </row>
     <row r="902">
-      <c s="8" r="A902"/>
+      <c s="10" r="A902"/>
     </row>
     <row r="903">
-      <c s="8" r="A903"/>
+      <c s="10" r="A903"/>
     </row>
     <row r="904">
-      <c s="8" r="A904"/>
+      <c s="10" r="A904"/>
     </row>
     <row r="905">
-      <c s="8" r="A905"/>
+      <c s="10" r="A905"/>
     </row>
     <row r="906">
-      <c s="8" r="A906"/>
+      <c s="10" r="A906"/>
     </row>
     <row r="907">
-      <c s="8" r="A907"/>
+      <c s="10" r="A907"/>
     </row>
     <row r="908">
-      <c s="8" r="A908"/>
+      <c s="10" r="A908"/>
     </row>
     <row r="909">
-      <c s="8" r="A909"/>
+      <c s="10" r="A909"/>
     </row>
     <row r="910">
-      <c s="8" r="A910"/>
+      <c s="10" r="A910"/>
     </row>
     <row r="911">
-      <c s="8" r="A911"/>
+      <c s="10" r="A911"/>
     </row>
     <row r="912">
-      <c s="8" r="A912"/>
+      <c s="10" r="A912"/>
     </row>
     <row r="913">
-      <c s="8" r="A913"/>
+      <c s="10" r="A913"/>
     </row>
     <row r="914">
-      <c s="8" r="A914"/>
+      <c s="10" r="A914"/>
     </row>
     <row r="915">
-      <c s="8" r="A915"/>
+      <c s="10" r="A915"/>
     </row>
     <row r="916">
-      <c s="8" r="A916"/>
+      <c s="10" r="A916"/>
     </row>
     <row r="917">
-      <c s="8" r="A917"/>
+      <c s="10" r="A917"/>
     </row>
     <row r="918">
-      <c s="8" r="A918"/>
+      <c s="10" r="A918"/>
     </row>
     <row r="919">
-      <c s="8" r="A919"/>
+      <c s="10" r="A919"/>
     </row>
     <row r="920">
-      <c s="8" r="A920"/>
+      <c s="10" r="A920"/>
     </row>
     <row r="921">
-      <c s="8" r="A921"/>
+      <c s="10" r="A921"/>
     </row>
     <row r="922">
-      <c s="8" r="A922"/>
+      <c s="10" r="A922"/>
     </row>
     <row r="923">
-      <c s="8" r="A923"/>
+      <c s="10" r="A923"/>
     </row>
     <row r="924">
-      <c s="8" r="A924"/>
+      <c s="10" r="A924"/>
     </row>
     <row r="925">
-      <c s="8" r="A925"/>
+      <c s="10" r="A925"/>
     </row>
     <row r="926">
-      <c s="8" r="A926"/>
+      <c s="10" r="A926"/>
     </row>
     <row r="927">
-      <c s="8" r="A927"/>
+      <c s="10" r="A927"/>
     </row>
     <row r="928">
-      <c s="8" r="A928"/>
+      <c s="10" r="A928"/>
     </row>
     <row r="929">
-      <c s="8" r="A929"/>
+      <c s="10" r="A929"/>
     </row>
     <row r="930">
-      <c s="8" r="A930"/>
+      <c s="10" r="A930"/>
     </row>
     <row r="931">
-      <c s="8" r="A931"/>
+      <c s="10" r="A931"/>
     </row>
     <row r="932">
-      <c s="8" r="A932"/>
+      <c s="10" r="A932"/>
     </row>
     <row r="933">
-      <c s="8" r="A933"/>
+      <c s="10" r="A933"/>
     </row>
     <row r="934">
-      <c s="8" r="A934"/>
+      <c s="10" r="A934"/>
     </row>
     <row r="935">
-      <c s="8" r="A935"/>
+      <c s="10" r="A935"/>
     </row>
     <row r="936">
-      <c s="8" r="A936"/>
+      <c s="10" r="A936"/>
     </row>
     <row r="937">
-      <c s="8" r="A937"/>
+      <c s="10" r="A937"/>
     </row>
     <row r="938">
-      <c s="8" r="A938"/>
+      <c s="10" r="A938"/>
     </row>
     <row r="939">
-      <c s="8" r="A939"/>
+      <c s="10" r="A939"/>
     </row>
     <row r="940">
-      <c s="8" r="A940"/>
+      <c s="10" r="A940"/>
     </row>
     <row r="941">
-      <c s="8" r="A941"/>
+      <c s="10" r="A941"/>
     </row>
     <row r="942">
-      <c s="8" r="A942"/>
+      <c s="10" r="A942"/>
     </row>
     <row r="943">
-      <c s="8" r="A943"/>
+      <c s="10" r="A943"/>
     </row>
     <row r="944">
-      <c s="8" r="A944"/>
+      <c s="10" r="A944"/>
     </row>
     <row r="945">
-      <c s="8" r="A945"/>
+      <c s="10" r="A945"/>
     </row>
     <row r="946">
-      <c s="8" r="A946"/>
+      <c s="10" r="A946"/>
     </row>
     <row r="947">
-      <c s="8" r="A947"/>
+      <c s="10" r="A947"/>
     </row>
     <row r="948">
-      <c s="8" r="A948"/>
+      <c s="10" r="A948"/>
     </row>
     <row r="949">
-      <c s="8" r="A949"/>
+      <c s="10" r="A949"/>
     </row>
     <row r="950">
-      <c s="8" r="A950"/>
+      <c s="10" r="A950"/>
     </row>
     <row r="951">
-      <c s="8" r="A951"/>
+      <c s="10" r="A951"/>
     </row>
     <row r="952">
-      <c s="8" r="A952"/>
+      <c s="10" r="A952"/>
     </row>
     <row r="953">
-      <c s="8" r="A953"/>
+      <c s="10" r="A953"/>
     </row>
     <row r="954">
-      <c s="8" r="A954"/>
+      <c s="10" r="A954"/>
     </row>
     <row r="955">
-      <c s="8" r="A955"/>
+      <c s="10" r="A955"/>
     </row>
     <row r="956">
-      <c s="8" r="A956"/>
+      <c s="10" r="A956"/>
     </row>
     <row r="957">
-      <c s="8" r="A957"/>
+      <c s="10" r="A957"/>
     </row>
     <row r="958">
-      <c s="8" r="A958"/>
+      <c s="10" r="A958"/>
     </row>
     <row r="959">
-      <c s="8" r="A959"/>
+      <c s="10" r="A959"/>
     </row>
     <row r="960">
-      <c s="8" r="A960"/>
+      <c s="10" r="A960"/>
     </row>
     <row r="961">
-      <c s="8" r="A961"/>
+      <c s="10" r="A961"/>
     </row>
     <row r="962">
-      <c s="8" r="A962"/>
+      <c s="10" r="A962"/>
     </row>
     <row r="963">
-      <c s="8" r="A963"/>
+      <c s="10" r="A963"/>
     </row>
     <row r="964">
-      <c s="8" r="A964"/>
+      <c s="10" r="A964"/>
     </row>
     <row r="965">
-      <c s="8" r="A965"/>
+      <c s="10" r="A965"/>
     </row>
     <row r="966">
-      <c s="8" r="A966"/>
+      <c s="10" r="A966"/>
     </row>
     <row r="967">
-      <c s="8" r="A967"/>
+      <c s="10" r="A967"/>
     </row>
     <row r="968">
-      <c s="8" r="A968"/>
+      <c s="10" r="A968"/>
     </row>
     <row r="969">
-      <c s="8" r="A969"/>
+      <c s="10" r="A969"/>
     </row>
     <row r="970">
-      <c s="8" r="A970"/>
+      <c s="10" r="A970"/>
     </row>
     <row r="971">
-      <c s="8" r="A971"/>
+      <c s="10" r="A971"/>
     </row>
     <row r="972">
-      <c s="8" r="A972"/>
+      <c s="10" r="A972"/>
     </row>
     <row r="973">
-      <c s="8" r="A973"/>
+      <c s="10" r="A973"/>
     </row>
     <row r="974">
-      <c s="8" r="A974"/>
+      <c s="10" r="A974"/>
     </row>
     <row r="975">
-      <c s="8" r="A975"/>
+      <c s="10" r="A975"/>
     </row>
     <row r="976">
-      <c s="8" r="A976"/>
+      <c s="10" r="A976"/>
     </row>
     <row r="977">
-      <c s="8" r="A977"/>
+      <c s="10" r="A977"/>
     </row>
     <row r="978">
-      <c s="8" r="A978"/>
+      <c s="10" r="A978"/>
     </row>
     <row r="979">
-      <c s="8" r="A979"/>
+      <c s="10" r="A979"/>
     </row>
     <row r="980">
-      <c s="8" r="A980"/>
+      <c s="10" r="A980"/>
     </row>
     <row r="981">
-      <c s="8" r="A981"/>
+      <c s="10" r="A981"/>
     </row>
     <row r="982">
-      <c s="8" r="A982"/>
+      <c s="10" r="A982"/>
     </row>
     <row r="983">
-      <c s="8" r="A983"/>
+      <c s="10" r="A983"/>
     </row>
     <row r="984">
-      <c s="8" r="A984"/>
+      <c s="10" r="A984"/>
     </row>
     <row r="985">
-      <c s="8" r="A985"/>
+      <c s="10" r="A985"/>
     </row>
     <row r="986">
-      <c s="8" r="A986"/>
+      <c s="10" r="A986"/>
     </row>
     <row r="987">
-      <c s="8" r="A987"/>
+      <c s="10" r="A987"/>
     </row>
     <row r="988">
-      <c s="8" r="A988"/>
+      <c s="10" r="A988"/>
     </row>
     <row r="989">
-      <c s="8" r="A989"/>
+      <c s="10" r="A989"/>
     </row>
     <row r="990">
-      <c s="8" r="A990"/>
+      <c s="10" r="A990"/>
     </row>
     <row r="991">
-      <c s="8" r="A991"/>
+      <c s="10" r="A991"/>
     </row>
     <row r="992">
-      <c s="8" r="A992"/>
+      <c s="10" r="A992"/>
     </row>
     <row r="993">
-      <c s="8" r="A993"/>
+      <c s="10" r="A993"/>
     </row>
     <row r="994">
-      <c s="8" r="A994"/>
+      <c s="10" r="A994"/>
     </row>
     <row r="995">
-      <c s="8" r="A995"/>
+      <c s="10" r="A995"/>
     </row>
     <row r="996">
-      <c s="8" r="A996"/>
+      <c s="10" r="A996"/>
     </row>
     <row r="997">
-      <c s="8" r="A997"/>
+      <c s="10" r="A997"/>
     </row>
     <row r="998">
-      <c s="8" r="A998"/>
+      <c s="10" r="A998"/>
     </row>
     <row r="999">
-      <c s="8" r="A999"/>
+      <c s="10" r="A999"/>
     </row>
     <row r="1000">
-      <c s="8" r="A1000"/>
+      <c s="10" r="A1000"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>